<commit_message>
Valores da HIMB inseridos na tabela de comparação
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,9 @@
       <c r="D3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>746.64</v>
+      </c>
       <c r="F3" s="14">
         <f xml:space="preserve"> AVERAGE(1505.1,1632.26,1696.96)</f>
         <v>1611.4399999999998</v>
@@ -1011,7 +1013,9 @@
       <c r="M3" s="1">
         <v>668</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>558</v>
+      </c>
       <c r="O3" s="1">
         <f>AVERAGE(883,650,909)</f>
         <v>814</v>
@@ -1035,7 +1039,9 @@
       <c r="V3" s="1">
         <v>25126.84</v>
       </c>
-      <c r="W3" s="1"/>
+      <c r="W3" s="1">
+        <v>25126.84</v>
+      </c>
       <c r="X3" s="1">
         <f>AVERAGE(34231.94,35331.27,35580.93)</f>
         <v>35048.046666666662</v>
@@ -1082,7 +1088,9 @@
       <c r="M4" s="1">
         <v>11086.43</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>9934.0499999999993</v>
+      </c>
       <c r="O4" s="14">
         <f>AVERAGE(20093,23146.55,19097.46)</f>
         <v>20779.003333333334</v>
@@ -1106,7 +1114,9 @@
       <c r="V4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1">
+        <v>7486.75</v>
+      </c>
       <c r="X4" s="14">
         <f>AVERAGE(11787.58,13221.13,11889.39)</f>
         <v>12299.366666666667</v>
@@ -1131,7 +1141,9 @@
       <c r="D5" s="3">
         <v>1409</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>1409</v>
+      </c>
       <c r="F5" s="3">
         <f xml:space="preserve"> AVERAGE(1564,1845,2288)</f>
         <v>1899</v>
@@ -1157,7 +1169,9 @@
       <c r="M5" s="1">
         <v>1411</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1">
+        <v>1422</v>
+      </c>
       <c r="O5" s="14">
         <f>AVERAGE(2200,2636,2649)</f>
         <v>2495</v>
@@ -1181,7 +1195,9 @@
       <c r="V5" s="1">
         <v>10765.78</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1">
+        <v>14065.44</v>
+      </c>
       <c r="X5" s="14">
         <f>AVERAGE(28708.52,23641.97,28071.05)</f>
         <v>26807.180000000004</v>
@@ -1206,7 +1222,9 @@
       <c r="D6" s="1">
         <v>5712</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>4475</v>
+      </c>
       <c r="F6" s="14">
         <f xml:space="preserve"> AVERAGE(14321,17859,14830)</f>
         <v>15670</v>
@@ -1252,7 +1270,9 @@
       <c r="V6" s="1">
         <v>22828.74</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="W6" s="1">
+        <v>23907.89</v>
+      </c>
       <c r="X6" s="14">
         <f>AVERAGE(37011.37,39208.49,33323.61)</f>
         <v>36514.49</v>
@@ -1277,7 +1297,9 @@
       <c r="D7" s="3">
         <v>292</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>292</v>
+      </c>
       <c r="F7" s="15">
         <v>292</v>
       </c>
@@ -1324,7 +1346,9 @@
       <c r="V7" s="1">
         <v>10893.75</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1">
+        <v>12001.03</v>
+      </c>
       <c r="X7" s="14">
         <f>AVERAGE(34465.92,32737.24,31541.07)</f>
         <v>32914.743333333339</v>
@@ -1349,7 +1373,9 @@
       <c r="D8" s="3">
         <v>352</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>352</v>
+      </c>
       <c r="F8" s="15">
         <v>352</v>
       </c>
@@ -1396,7 +1422,9 @@
       <c r="V8" s="1">
         <v>17072</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1">
+        <v>17072</v>
+      </c>
       <c r="X8" s="14">
         <f>AVERAGE(37722.49,35121.04,52458.35)</f>
         <v>41767.293333333335</v>
@@ -1421,7 +1449,9 @@
       <c r="D9" s="3">
         <v>604.66</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>604.66</v>
+      </c>
       <c r="F9" s="3">
         <f xml:space="preserve"> AVERAGE(715.59,640.05,1766.47)</f>
         <v>1040.7033333333331</v>
@@ -1469,7 +1499,9 @@
       <c r="V9" s="1">
         <v>22868.63</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1">
+        <v>23494.84</v>
+      </c>
       <c r="X9" s="14">
         <f>AVERAGE(53850.22,59959.36,63479.72)</f>
         <v>59096.433333333327</v>
@@ -1494,7 +1526,9 @@
       <c r="D10" s="1">
         <v>14342.78</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>11706.58</v>
+      </c>
       <c r="F10" s="14">
         <f xml:space="preserve"> AVERAGE(22801.5,24988.75,19031.39)</f>
         <v>22273.88</v>
@@ -1540,7 +1574,9 @@
       <c r="V10" s="1">
         <v>8100</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1">
+        <v>8100</v>
+      </c>
       <c r="X10" s="14">
         <f>AVERAGE(21851.94,25401.1,21951.12)</f>
         <v>23068.05333333333</v>
@@ -1565,7 +1601,9 @@
       <c r="D11" s="1">
         <v>6116</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>4607</v>
+      </c>
       <c r="F11" s="14">
         <f xml:space="preserve"> AVERAGE(4339,4610,6809)</f>
         <v>5252.666666666667</v>
@@ -1589,7 +1627,9 @@
       <c r="M11" s="1">
         <v>3454</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1">
+        <v>3155</v>
+      </c>
       <c r="O11" s="14">
         <f>AVERAGE(2188,2341,3487)</f>
         <v>2672</v>
@@ -1613,7 +1653,9 @@
       <c r="V11" s="6">
         <v>12369.29</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1">
+        <v>12312.57</v>
+      </c>
       <c r="X11" s="14">
         <f>AVERAGE(33103.09,29152.95,27824.8)</f>
         <v>30026.946666666667</v>
@@ -1638,7 +1680,9 @@
       <c r="D12" s="13">
         <v>21120</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13">
+        <v>480</v>
+      </c>
       <c r="F12" s="14">
         <f xml:space="preserve"> AVERAGE(82770,71970,84330)</f>
         <v>79690</v>
@@ -1662,7 +1706,9 @@
       <c r="M12" s="1">
         <v>5157.68</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>4872.0200000000004</v>
+      </c>
       <c r="O12" s="14">
         <f>AVERAGE(7584.43,8374.97,8015.42)</f>
         <v>7991.6066666666666</v>
@@ -1686,7 +1732,9 @@
       <c r="V12" s="1">
         <v>22600.959999999999</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="W12" s="1">
+        <v>23714.23</v>
+      </c>
       <c r="X12" s="14">
         <f>AVERAGE(58160.33,51748.26,59422.06)</f>
         <v>56443.549999999996</v>
@@ -1711,7 +1759,9 @@
       <c r="D13" s="3">
         <v>249.88</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>249.88</v>
+      </c>
       <c r="F13" s="15">
         <v>249.88</v>
       </c>
@@ -1735,7 +1785,9 @@
       <c r="M13" s="1">
         <v>6644.96</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>7646.9</v>
+      </c>
       <c r="O13" s="14">
         <f>AVERAGE(14537.19,11181.93,12864.92)</f>
         <v>12861.346666666666</v>
@@ -1759,7 +1811,9 @@
       <c r="V13" s="1">
         <v>68337.149999999994</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1">
+        <v>66904.56</v>
+      </c>
       <c r="X13" s="14">
         <f>AVERAGE(274864.87,269718.4,278424.19)</f>
         <v>274335.82</v>
@@ -1784,7 +1838,9 @@
       <c r="D14" s="1">
         <v>1211.5899999999999</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>1230.99</v>
+      </c>
       <c r="F14" s="14">
         <f xml:space="preserve"> AVERAGE(2543.27,2264.22,2236.15)</f>
         <v>2347.8799999999997</v>
@@ -1808,7 +1864,9 @@
       <c r="M14" s="1">
         <v>6870.92</v>
       </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1">
+        <v>6899.46</v>
+      </c>
       <c r="O14" s="14">
         <f>AVERAGE(16197.94,15917.45,15432.47)</f>
         <v>15849.286666666667</v>
@@ -1832,7 +1890,9 @@
       <c r="V14" s="1">
         <v>277.23</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="W14" s="1">
+        <v>359.69</v>
+      </c>
       <c r="X14" s="14">
         <f>AVERAGE(434.6,422.28,429.06)</f>
         <v>428.6466666666667</v>
@@ -1857,7 +1917,9 @@
       <c r="D15" s="1">
         <v>1304.57</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>1400.68</v>
+      </c>
       <c r="F15" s="14">
         <f xml:space="preserve"> AVERAGE(2748.74,2857.69,2722.18)</f>
         <v>2776.2033333333334</v>
@@ -1881,7 +1943,9 @@
       <c r="M15" s="1">
         <v>5552.01</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1">
+        <v>4469.8100000000004</v>
+      </c>
       <c r="O15" s="14">
         <f>AVERAGE(8243.9,7828.62,9343.42)</f>
         <v>8471.9800000000014</v>
@@ -1905,7 +1969,9 @@
       <c r="V15" s="1">
         <v>560.07000000000005</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1">
+        <v>606.24</v>
+      </c>
       <c r="X15" s="14">
         <f>AVERAGE(1004.91,1040.98,1126.33)</f>
         <v>1057.4066666666665</v>
@@ -1930,7 +1996,9 @@
       <c r="D16" s="3">
         <v>103</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>103</v>
+      </c>
       <c r="F16" s="3">
         <f xml:space="preserve"> AVERAGE(120,128,115)</f>
         <v>121</v>
@@ -1956,7 +2024,9 @@
       <c r="M16" s="1">
         <v>5199.62</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1">
+        <v>5533.11</v>
+      </c>
       <c r="O16" s="14">
         <f>AVERAGE(12214.44,11244.59,12231.11)</f>
         <v>11896.713333333333</v>
@@ -1980,7 +2050,9 @@
       <c r="V16" s="1">
         <v>1745</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1">
+        <v>1764.02</v>
+      </c>
       <c r="X16" s="17">
         <f>AVERAGE(4825.39,4941.65,5123.81)</f>
         <v>4963.6166666666677</v>
@@ -2005,7 +2077,9 @@
       <c r="D17" s="3">
         <v>77.040000000000006</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>77.040000000000006</v>
+      </c>
       <c r="F17" s="3">
         <f xml:space="preserve"> AVERAGE(97.58,112.27,95.39)</f>
         <v>101.74666666666667</v>
@@ -2031,7 +2105,9 @@
       <c r="M17" s="1">
         <v>6907.12</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>8397.4500000000007</v>
+      </c>
       <c r="O17" s="14">
         <f>AVERAGE(15900.56,15542.01,15610.06)</f>
         <v>15684.21</v>
@@ -2055,7 +2131,9 @@
       <c r="V17" s="1">
         <v>2382.5</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1">
+        <v>2466.0500000000002</v>
+      </c>
       <c r="X17" s="14">
         <f>AVERAGE(7666.21,7493.21,8008.9)</f>
         <v>7722.7733333333335</v>
@@ -2080,7 +2158,9 @@
       <c r="D18" s="1">
         <v>97.38</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>99.45</v>
+      </c>
       <c r="F18" s="14">
         <f xml:space="preserve"> AVERAGE(154.43,150.12,136.69)</f>
         <v>147.08000000000001</v>
@@ -2104,7 +2184,9 @@
       <c r="M18" s="1">
         <v>4346.5200000000004</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>6123.26</v>
+      </c>
       <c r="O18" s="14">
         <f>AVERAGE(7644.11,8352.1,7110.64)</f>
         <v>7702.2833333333328</v>
@@ -2128,7 +2210,9 @@
       <c r="V18" s="1">
         <v>5028</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="W18" s="1">
+        <v>5478</v>
+      </c>
       <c r="X18" s="14">
         <f>AVERAGE(5942,6221,6355)</f>
         <v>6172.666666666667</v>
@@ -2153,7 +2237,9 @@
       <c r="D19" s="1">
         <v>150.96</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>132.75</v>
+      </c>
       <c r="F19" s="14">
         <f xml:space="preserve"> AVERAGE(151.73,211.47,242.02)</f>
         <v>201.74</v>
@@ -2177,7 +2263,9 @@
       <c r="M19" s="1">
         <v>5246.28</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>5246.28</v>
+      </c>
       <c r="O19" s="14">
         <f>AVERAGE(7915.81,9560.27,9212.85)</f>
         <v>8896.31</v>
@@ -2201,7 +2289,9 @@
       <c r="V19" s="1">
         <v>12360</v>
       </c>
-      <c r="W19" s="1"/>
+      <c r="W19" s="1">
+        <v>12196</v>
+      </c>
       <c r="X19" s="14">
         <f>AVERAGE(16179,15753,15546)</f>
         <v>15826</v>
@@ -2226,7 +2316,9 @@
       <c r="D20" s="3">
         <v>147</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>147</v>
+      </c>
       <c r="F20" s="15">
         <v>147</v>
       </c>
@@ -2251,7 +2343,9 @@
       <c r="M20" s="1">
         <v>4123.3500000000004</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>3842.76</v>
+      </c>
       <c r="O20" s="14">
         <f>AVERAGE(8471.76,7370.09,6547.6)</f>
         <v>7463.1500000000005</v>
@@ -2275,7 +2369,9 @@
       <c r="V20" s="1">
         <v>22289</v>
       </c>
-      <c r="W20" s="1"/>
+      <c r="W20" s="1">
+        <v>22414</v>
+      </c>
       <c r="X20" s="14">
         <f>AVERAGE(37635,36780,38408)</f>
         <v>37607.666666666664</v>
@@ -2300,7 +2396,9 @@
       <c r="D21" s="1">
         <v>562.04</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>666.2</v>
+      </c>
       <c r="F21" s="14">
         <f xml:space="preserve"> AVERAGE(1394.04,1547.92,1338.26)</f>
         <v>1426.74</v>
@@ -2324,7 +2422,9 @@
       <c r="M21" s="1">
         <v>2149.8200000000002</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>2067.87</v>
+      </c>
       <c r="O21" s="14">
         <f>AVERAGE(3890.65,4784.86,4636.22)</f>
         <v>4437.2433333333329</v>
@@ -2348,7 +2448,9 @@
       <c r="V21" s="13">
         <v>130.04</v>
       </c>
-      <c r="W21" s="13"/>
+      <c r="W21" s="13">
+        <v>128.07</v>
+      </c>
       <c r="X21" s="14">
         <f>AVERAGE(182.12,212.39,172.41)</f>
         <v>188.97333333333333</v>
@@ -2373,7 +2475,9 @@
       <c r="D22" s="3">
         <v>174</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3">
+        <v>154</v>
+      </c>
       <c r="F22" s="15">
         <v>174</v>
       </c>
@@ -2398,7 +2502,9 @@
       <c r="M22" s="1">
         <v>9156.66</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>9230.75</v>
+      </c>
       <c r="O22" s="14">
         <f>AVERAGE(25401.97,25448.92,26352.32)</f>
         <v>25734.403333333332</v>
@@ -2422,7 +2528,9 @@
       <c r="V22" s="1">
         <v>146</v>
       </c>
-      <c r="W22" s="1"/>
+      <c r="W22" s="1">
+        <v>146</v>
+      </c>
       <c r="X22" s="14">
         <f>AVERAGE(185,182,195)</f>
         <v>187.33333333333334</v>
@@ -2447,7 +2555,9 @@
       <c r="D23" s="3">
         <v>258</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>248</v>
+      </c>
       <c r="F23" s="15">
         <v>258</v>
       </c>
@@ -2472,7 +2582,9 @@
       <c r="M23" s="1">
         <v>13388.78</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>13074.68</v>
+      </c>
       <c r="O23" s="14">
         <f>AVERAGE(59275.29,58450.29,59315.09)</f>
         <v>59013.556666666664</v>
@@ -2496,7 +2608,9 @@
       <c r="V23" s="1">
         <v>27500</v>
       </c>
-      <c r="W23" s="1"/>
+      <c r="W23" s="1">
+        <v>27500</v>
+      </c>
       <c r="X23" s="14">
         <f>AVERAGE(85382.67,73888.73,78761.91)</f>
         <v>79344.436666666661</v>
@@ -2521,7 +2635,9 @@
       <c r="D24" s="3">
         <v>162</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <v>162</v>
+      </c>
       <c r="F24" s="15">
         <v>162</v>
       </c>
@@ -2546,7 +2662,9 @@
       <c r="M24" s="7">
         <v>728</v>
       </c>
-      <c r="N24" s="7"/>
+      <c r="N24" s="7">
+        <v>566</v>
+      </c>
       <c r="O24" s="14">
         <f>AVERAGE(1781,1645,2083)</f>
         <v>1836.3333333333333</v>
@@ -2570,7 +2688,9 @@
       <c r="V24" s="1">
         <v>1036.02</v>
       </c>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1">
+        <v>1056.72</v>
+      </c>
       <c r="X24" s="14">
         <f>AVERAGE(1900.37,1955.94,1523.17)</f>
         <v>1793.1599999999999</v>
@@ -2605,7 +2725,9 @@
       <c r="V25" s="3">
         <v>826.08</v>
       </c>
-      <c r="W25" s="3"/>
+      <c r="W25" s="3">
+        <v>751.06</v>
+      </c>
       <c r="X25" s="15">
         <v>826.08</v>
       </c>
@@ -2647,7 +2769,9 @@
       <c r="V26" s="10">
         <v>456.58</v>
       </c>
-      <c r="W26" s="10"/>
+      <c r="W26" s="10">
+        <v>456.58</v>
+      </c>
       <c r="X26" s="15">
         <v>456.58</v>
       </c>
@@ -2792,8 +2916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2940,7 +3064,9 @@
       <c r="D3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>1551.66</v>
+      </c>
       <c r="F3" s="1">
         <f>AVERAGE(3647.07,3269.08,3255.4)</f>
         <v>3390.5166666666664</v>
@@ -2964,7 +3090,9 @@
       <c r="M3" s="1">
         <v>2139</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>1691</v>
+      </c>
       <c r="O3" s="1">
         <f>AVERAGE(2847,2862,2525)</f>
         <v>2744.6666666666665</v>
@@ -2988,7 +3116,9 @@
       <c r="V3" s="1">
         <v>42676.77</v>
       </c>
-      <c r="W3" s="1"/>
+      <c r="W3" s="1">
+        <v>44191.56</v>
+      </c>
       <c r="X3" s="1">
         <f>AVERAGE(67671.02,71552.62,67721.63)</f>
         <v>68981.756666666668</v>
@@ -3035,7 +3165,9 @@
       <c r="M4" s="1">
         <v>22073.5</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>23897.19</v>
+      </c>
       <c r="O4" s="14">
         <f>AVERAGE(43002.43,42126.39,45047.13)</f>
         <v>43391.983333333337</v>
@@ -3059,7 +3191,9 @@
       <c r="V4" s="1">
         <v>17103.07</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1">
+        <v>15595.35</v>
+      </c>
       <c r="X4" s="14">
         <f>AVERAGE(43965.63,41638.47,55019.8)</f>
         <v>46874.633333333339</v>
@@ -3084,7 +3218,9 @@
       <c r="D5" s="3">
         <v>3574</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>3710</v>
+      </c>
       <c r="F5" s="3">
         <f>AVERAGE(6095,4382,4205)</f>
         <v>4894</v>
@@ -3110,7 +3246,9 @@
       <c r="M5" s="1">
         <v>3174</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1">
+        <v>3062</v>
+      </c>
       <c r="O5" s="14">
         <f>AVERAGE(5034,5155,5513)</f>
         <v>5234</v>
@@ -3134,7 +3272,9 @@
       <c r="V5" s="1">
         <v>26214.19</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1">
+        <v>22543.29</v>
+      </c>
       <c r="X5" s="14">
         <f>AVERAGE(57354.29,64630.46,70897.19)</f>
         <v>64293.98</v>
@@ -3159,7 +3299,9 @@
       <c r="D6" s="1">
         <v>14421</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>10405</v>
+      </c>
       <c r="F6" s="14">
         <f>AVERAGE(36633,36410,36332)</f>
         <v>36458.333333333336</v>
@@ -3205,7 +3347,9 @@
       <c r="V6" s="1">
         <v>53346.76</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="W6" s="1">
+        <v>51047.96</v>
+      </c>
       <c r="X6" s="14">
         <f>AVERAGE(94718.25,98201.9,84465.24)</f>
         <v>92461.796666666676</v>
@@ -3230,7 +3374,9 @@
       <c r="D7" s="3">
         <v>581</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>581</v>
+      </c>
       <c r="F7" s="15">
         <v>581</v>
       </c>
@@ -3277,7 +3423,9 @@
       <c r="V7" s="1">
         <v>26457.22</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1">
+        <v>28471</v>
+      </c>
       <c r="X7" s="14">
         <f>AVERAGE(62535.57,67602.32,64349.75)</f>
         <v>64829.21333333334</v>
@@ -3302,7 +3450,9 @@
       <c r="D8" s="3">
         <v>816</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>818</v>
+      </c>
       <c r="F8" s="15">
         <v>816</v>
       </c>
@@ -3349,7 +3499,9 @@
       <c r="V8" s="1">
         <v>35032.6</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1">
+        <v>35705.47</v>
+      </c>
       <c r="X8" s="14">
         <f>AVERAGE(92260.55,75101.11,80997.32)</f>
         <v>82786.326666666675</v>
@@ -3374,7 +3526,9 @@
       <c r="D9" s="3">
         <v>1809.58</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>1857.02</v>
+      </c>
       <c r="F9" s="3">
         <f>AVERAGE(2651.31,3294.21,2833.02)</f>
         <v>2926.1800000000003</v>
@@ -3422,7 +3576,9 @@
       <c r="V9" s="1">
         <v>51597.94</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1">
+        <v>53661.61</v>
+      </c>
       <c r="X9" s="14">
         <f>AVERAGE(125277.77,124544.19,117939.53)</f>
         <v>122587.16333333333</v>
@@ -3447,7 +3603,9 @@
       <c r="D10" s="1">
         <v>29446.799999999999</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>30074.639999999999</v>
+      </c>
       <c r="F10" s="14">
         <f>AVERAGE(56780.47,53043,50702.91)</f>
         <v>53508.793333333335</v>
@@ -3493,7 +3651,9 @@
       <c r="V10" s="1">
         <v>23011.19</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1">
+        <v>21708.66</v>
+      </c>
       <c r="X10" s="14">
         <f>AVERAGE(97573.93,76410.8,87873.39)</f>
         <v>87286.04</v>
@@ -3518,7 +3678,9 @@
       <c r="D11" s="1">
         <v>10296</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>9828</v>
+      </c>
       <c r="F11" s="16">
         <f>AVERAGE(8182,8938,10118)</f>
         <v>9079.3333333333339</v>
@@ -3542,7 +3704,9 @@
       <c r="M11" s="1">
         <v>6476</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1">
+        <v>5474</v>
+      </c>
       <c r="O11" s="14">
         <f>AVERAGE(8023,4994,8974)</f>
         <v>7330.333333333333</v>
@@ -3566,7 +3730,9 @@
       <c r="V11" s="1">
         <v>27476.07</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1">
+        <v>26159.06</v>
+      </c>
       <c r="X11" s="14">
         <f>AVERAGE(68765.2,64902.05,60570.51)</f>
         <v>64745.920000000006</v>
@@ -3591,7 +3757,9 @@
       <c r="D12" s="1">
         <v>57910</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>980</v>
+      </c>
       <c r="F12" s="14">
         <f>AVERAGE(119890,130840,141420)</f>
         <v>130716.66666666667</v>
@@ -3615,7 +3783,9 @@
       <c r="M12" s="1">
         <v>11572.88</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>10270.1</v>
+      </c>
       <c r="O12" s="14">
         <f>AVERAGE(18246.01,15636.11,15860.69)</f>
         <v>16580.936666666665</v>
@@ -3639,7 +3809,9 @@
       <c r="V12" s="1">
         <v>41333.97</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="W12" s="1">
+        <v>43929.8</v>
+      </c>
       <c r="X12" s="14">
         <f>AVERAGE(130468.43,132240.97,139718.17)</f>
         <v>134142.52333333335</v>
@@ -3664,7 +3836,9 @@
       <c r="D13" s="3">
         <v>1454.84</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>1339.12</v>
+      </c>
       <c r="F13" s="15">
         <v>1454.84</v>
       </c>
@@ -3688,7 +3862,9 @@
       <c r="M13" s="6">
         <v>15643.51</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>50807.89</v>
+      </c>
       <c r="O13" s="14">
         <f>AVERAGE(31530.67,28819.06,27007.27)</f>
         <v>29119</v>
@@ -3712,7 +3888,9 @@
       <c r="V13" s="1">
         <v>133670.14000000001</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1">
+        <v>143817.03</v>
+      </c>
       <c r="X13" s="14">
         <f>AVERAGE(611099.29,611721.92,615676.98)</f>
         <v>612832.73</v>
@@ -3737,7 +3915,9 @@
       <c r="D14" s="1">
         <v>2717.27</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>2792.21</v>
+      </c>
       <c r="F14" s="14">
         <f>AVERAGE(5109.97,5065.25,4645.03)</f>
         <v>4940.083333333333</v>
@@ -3761,7 +3941,9 @@
       <c r="M14" s="1">
         <v>13623.44</v>
       </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1">
+        <v>16093.09</v>
+      </c>
       <c r="O14" s="14">
         <f>AVERAGE(33860.82,35440.32,32829.69)</f>
         <v>34043.61</v>
@@ -3785,7 +3967,9 @@
       <c r="V14" s="1">
         <v>600.15</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="W14" s="1">
+        <v>695.56</v>
+      </c>
       <c r="X14" s="14">
         <f>AVERAGE(915.58,965.96,857.74)</f>
         <v>913.09333333333325</v>
@@ -3810,7 +3994,9 @@
       <c r="D15" s="1">
         <v>3194.43</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>3621.33</v>
+      </c>
       <c r="F15" s="14">
         <f>AVERAGE(5931.11,6725.71,6492.31)</f>
         <v>6383.043333333334</v>
@@ -3834,7 +4020,9 @@
       <c r="M15" s="1">
         <v>11462.54</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1">
+        <v>11768</v>
+      </c>
       <c r="O15" s="14">
         <f>AVERAGE(17548.83,18031.67,17132.19)</f>
         <v>17570.896666666667</v>
@@ -3858,7 +4046,9 @@
       <c r="V15" s="1">
         <v>1135.3800000000001</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1">
+        <v>1293.71</v>
+      </c>
       <c r="X15" s="14">
         <f>AVERAGE(2172,2292.37,2366.69)</f>
         <v>2277.02</v>
@@ -3883,7 +4073,9 @@
       <c r="D16" s="3">
         <v>255</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>251</v>
+      </c>
       <c r="F16" s="3">
         <f>AVERAGE(275,256,347)</f>
         <v>292.66666666666669</v>
@@ -3909,7 +4101,9 @@
       <c r="M16" s="1">
         <v>12323.13</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1">
+        <v>13509.84</v>
+      </c>
       <c r="O16" s="14">
         <f>AVERAGE(25882.97,25132.64,26685.26)</f>
         <v>25900.289999999997</v>
@@ -3933,7 +4127,9 @@
       <c r="V16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1">
+        <v>3690.24</v>
+      </c>
       <c r="X16" s="14">
         <f>AVERAGE(11399.38,10366.03,10813.15)</f>
         <v>10859.519999999999</v>
@@ -3958,7 +4154,9 @@
       <c r="D17" s="3">
         <v>181.41</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>190.34</v>
+      </c>
       <c r="F17" s="3">
         <f>AVERAGE(279.26,215.78,239.33)</f>
         <v>244.79</v>
@@ -3984,7 +4182,9 @@
       <c r="M17" s="1">
         <v>17281.75</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>17169.62</v>
+      </c>
       <c r="O17" s="14">
         <f>AVERAGE(34360.88,33605.76,33152.24)</f>
         <v>33706.293333333335</v>
@@ -4008,7 +4208,9 @@
       <c r="V17" s="1">
         <v>4697.63</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1">
+        <v>4979.6899999999996</v>
+      </c>
       <c r="X17" s="14">
         <f>AVERAGE(17169.52,18058.97,17036.8)</f>
         <v>17421.763333333336</v>
@@ -4033,7 +4235,9 @@
       <c r="D18" s="1">
         <v>232.79</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>240.5</v>
+      </c>
       <c r="F18" s="14">
         <f>AVERAGE(347.21,387.79,356.93)</f>
         <v>363.97666666666669</v>
@@ -4057,7 +4261,9 @@
       <c r="M18" s="1">
         <v>9617.35</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>12165.37</v>
+      </c>
       <c r="O18" s="14">
         <f>AVERAGE(20744.35,18030.82,16756.05)</f>
         <v>18510.406666666666</v>
@@ -4081,7 +4287,9 @@
       <c r="V18" s="1">
         <v>10581</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="W18" s="1">
+        <v>10638</v>
+      </c>
       <c r="X18" s="14">
         <f>AVERAGE(12976,12872,13402)</f>
         <v>13083.333333333334</v>
@@ -4106,7 +4314,9 @@
       <c r="D19" s="1">
         <v>322.75</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>269.56</v>
+      </c>
       <c r="F19" s="14">
         <f>AVERAGE(429.85,402.52,396.58)</f>
         <v>409.65000000000003</v>
@@ -4130,7 +4340,9 @@
       <c r="M19" s="1">
         <v>10720.17</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>11235.04</v>
+      </c>
       <c r="O19" s="14">
         <f>AVERAGE(17595.39,18311.99,19771.19)</f>
         <v>18559.523333333334</v>
@@ -4154,7 +4366,9 @@
       <c r="V19" s="1">
         <v>23690</v>
       </c>
-      <c r="W19" s="1"/>
+      <c r="W19" s="1">
+        <v>23530</v>
+      </c>
       <c r="X19" s="14">
         <f>AVERAGE(36396,36800,33279)</f>
         <v>35491.666666666664</v>
@@ -4179,7 +4393,9 @@
       <c r="D20" s="3">
         <v>334</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>391</v>
+      </c>
       <c r="F20" s="15">
         <v>334</v>
       </c>
@@ -4204,7 +4420,9 @@
       <c r="M20" s="1">
         <v>10228.68</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>10160.41</v>
+      </c>
       <c r="O20" s="14">
         <f>AVERAGE(17133.65,16940.88,17970.63)</f>
         <v>17348.386666666669</v>
@@ -4228,7 +4446,9 @@
       <c r="V20" s="1">
         <v>46820</v>
       </c>
-      <c r="W20" s="1"/>
+      <c r="W20" s="1">
+        <v>46810</v>
+      </c>
       <c r="X20" s="14">
         <f>AVERAGE(72588,76165,72797)</f>
         <v>73850</v>
@@ -4253,7 +4473,9 @@
       <c r="D21" s="1">
         <v>1179.57</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>1397.39</v>
+      </c>
       <c r="F21" s="14">
         <f>AVERAGE(3178.66,2821.46,2883.3)</f>
         <v>2961.14</v>
@@ -4277,7 +4499,9 @@
       <c r="M21" s="1">
         <v>5888.85</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>5350.1</v>
+      </c>
       <c r="O21" s="14">
         <f>AVERAGE(9493.61,12161.74,10876.06)</f>
         <v>10843.803333333331</v>
@@ -4301,7 +4525,9 @@
       <c r="V21" s="13">
         <v>347.28</v>
       </c>
-      <c r="W21" s="13"/>
+      <c r="W21" s="13">
+        <v>250.24</v>
+      </c>
       <c r="X21" s="14">
         <f>AVERAGE(444.2,462.22,453.49)</f>
         <v>453.30333333333334</v>
@@ -4326,7 +4552,9 @@
       <c r="D22" s="3">
         <v>380</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3">
+        <v>426</v>
+      </c>
       <c r="F22" s="18">
         <v>380</v>
       </c>
@@ -4351,7 +4579,9 @@
       <c r="M22" s="1">
         <v>22878.82</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>20965.099999999999</v>
+      </c>
       <c r="O22" s="14">
         <f>AVERAGE(56954.6,54865.21,60437.12)</f>
         <v>57418.976666666662</v>
@@ -4375,7 +4605,9 @@
       <c r="V22" s="1">
         <v>441</v>
       </c>
-      <c r="W22" s="1"/>
+      <c r="W22" s="1">
+        <v>448</v>
+      </c>
       <c r="X22" s="14">
         <f>AVERAGE(616,625,606)</f>
         <v>615.66666666666663</v>
@@ -4400,7 +4632,9 @@
       <c r="D23" s="3">
         <v>1019</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>683</v>
+      </c>
       <c r="F23" s="18">
         <v>1019</v>
       </c>
@@ -4425,7 +4659,9 @@
       <c r="M23" s="1">
         <v>28892.080000000002</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>28532.55</v>
+      </c>
       <c r="O23" s="14">
         <f>AVERAGE(133425.62,129861.81,136169.48)</f>
         <v>133152.30333333334</v>
@@ -4449,7 +4685,9 @@
       <c r="V23" s="1">
         <v>55500</v>
       </c>
-      <c r="W23" s="1"/>
+      <c r="W23" s="1">
+        <v>73643.86</v>
+      </c>
       <c r="X23" s="14">
         <f>AVERAGE(164561.21,166644.63,173340.26)</f>
         <v>168182.03333333333</v>
@@ -4474,7 +4712,9 @@
       <c r="D24" s="3">
         <v>490</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <v>413</v>
+      </c>
       <c r="F24" s="18">
         <v>490</v>
       </c>
@@ -4499,7 +4739,9 @@
       <c r="M24" s="6">
         <v>1370</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="6">
+        <v>1242</v>
+      </c>
       <c r="O24" s="14">
         <f>AVERAGE(3980,4416,3964)</f>
         <v>4120</v>
@@ -4523,7 +4765,9 @@
       <c r="V24" s="1">
         <v>1875.65</v>
       </c>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1">
+        <v>2155.5100000000002</v>
+      </c>
       <c r="X24" s="14">
         <f>AVERAGE(4154.65,3907.26,4018.22)</f>
         <v>4026.7099999999996</v>
@@ -4558,7 +4802,9 @@
       <c r="V25" s="3">
         <v>1981.71</v>
       </c>
-      <c r="W25" s="3"/>
+      <c r="W25" s="3">
+        <v>1981.15</v>
+      </c>
       <c r="X25" s="15">
         <v>1981.71</v>
       </c>
@@ -4600,7 +4846,9 @@
       <c r="V26" s="3">
         <v>2086.59</v>
       </c>
-      <c r="W26" s="3"/>
+      <c r="W26" s="3">
+        <v>2006.03</v>
+      </c>
       <c r="X26" s="15">
         <v>2086.59</v>
       </c>
@@ -4758,8 +5006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4905,7 +5153,9 @@
       <c r="D3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>2333.29</v>
+      </c>
       <c r="F3" s="1">
         <f>AVERAGE(5498.19,5752.9,5622.22)</f>
         <v>5624.4366666666674</v>
@@ -4929,7 +5179,9 @@
       <c r="M3" s="1">
         <v>3478</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>3475</v>
+      </c>
       <c r="O3" s="1">
         <f>AVERAGE(4113,4382,3925)</f>
         <v>4140</v>
@@ -4953,7 +5205,9 @@
       <c r="V3" s="1">
         <v>63830.12</v>
       </c>
-      <c r="W3" s="1"/>
+      <c r="W3" s="1">
+        <v>69764.62</v>
+      </c>
       <c r="X3" s="1">
         <f>AVERAGE(117447.11,116929.81,134420.93)</f>
         <v>122932.61666666665</v>
@@ -5000,7 +5254,9 @@
       <c r="M4" s="1">
         <v>41093.300000000003</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>38395.919999999998</v>
+      </c>
       <c r="O4" s="14">
         <f>AVERAGE(71504.94,77227.03,67640)</f>
         <v>72123.990000000005</v>
@@ -5024,7 +5280,9 @@
       <c r="V4" s="1">
         <v>33252.04</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1">
+        <v>32109.37</v>
+      </c>
       <c r="X4" s="14">
         <f>AVERAGE(72879.96,64236.39,61493.96)</f>
         <v>66203.436666666661</v>
@@ -5049,7 +5307,9 @@
       <c r="D5" s="3">
         <v>7089</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>6671</v>
+      </c>
       <c r="F5" s="3">
         <f>AVERAGE(7838,9402,8578)</f>
         <v>8606</v>
@@ -5075,7 +5335,9 @@
       <c r="M5" s="1">
         <v>4749</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1">
+        <v>4888</v>
+      </c>
       <c r="O5" s="14">
         <f>AVERAGE(8377,8984,9359)</f>
         <v>8906.6666666666661</v>
@@ -5099,7 +5361,9 @@
       <c r="V5" s="1">
         <v>40795.86</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1">
+        <v>41639.79</v>
+      </c>
       <c r="X5" s="14">
         <f>AVERAGE(93776.89,96997.87,89510.79)</f>
         <v>93428.516666666663</v>
@@ -5124,7 +5388,9 @@
       <c r="D6" s="12">
         <v>23269</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>18984</v>
+      </c>
       <c r="F6" s="14">
         <f>AVERAGE(76704,73524,78156)</f>
         <v>76128</v>
@@ -5148,7 +5414,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="14">
-        <f t="shared" ref="O6:Q23" si="2">AVERAGE(1)</f>
+        <f t="shared" ref="O6:O10" si="2">AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="P6" s="14">
@@ -5170,7 +5436,9 @@
       <c r="V6" s="1">
         <v>84256.72</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="W6" s="1">
+        <v>81838.740000000005</v>
+      </c>
       <c r="X6" s="14">
         <f>AVERAGE(132266.71,133094,25,136977.14)</f>
         <v>100590.71249999999</v>
@@ -5195,7 +5463,9 @@
       <c r="D7" s="3">
         <v>1065</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>1068</v>
+      </c>
       <c r="F7" s="15">
         <v>1065</v>
       </c>
@@ -5242,7 +5512,9 @@
       <c r="V7" s="1">
         <v>41326.949999999997</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1">
+        <v>43036.45</v>
+      </c>
       <c r="X7" s="14">
         <f>AVERAGE(113604.96,122890.51,110266.69)</f>
         <v>115587.38666666667</v>
@@ -5267,7 +5539,9 @@
       <c r="D8" s="3">
         <v>1237</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>1174</v>
+      </c>
       <c r="F8" s="15">
         <v>1237</v>
       </c>
@@ -5314,7 +5588,9 @@
       <c r="V8" s="1">
         <v>51636.7</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1">
+        <v>52270.61</v>
+      </c>
       <c r="X8" s="14">
         <f>AVERAGE(150030.4,142468.98,133929.33)</f>
         <v>142142.90333333332</v>
@@ -5339,7 +5615,9 @@
       <c r="D9" s="3">
         <v>4429.84</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>4629.4799999999996</v>
+      </c>
       <c r="F9" s="3">
         <f>AVERAGE(6644.97,6506.27,6688.28)</f>
         <v>6613.1733333333332</v>
@@ -5387,7 +5665,9 @@
       <c r="V9" s="1">
         <v>67272.25</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1">
+        <v>71036.73</v>
+      </c>
       <c r="X9" s="14">
         <f>AVERAGE(178097.34,176328.93,180314.66)</f>
         <v>178246.97666666668</v>
@@ -5412,7 +5692,9 @@
       <c r="D10" s="1">
         <v>56582.89</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>53625.85</v>
+      </c>
       <c r="F10" s="14">
         <f>AVERAGE(137748.6,120237.26,117651.98)</f>
         <v>125212.61333333333</v>
@@ -5458,7 +5740,9 @@
       <c r="V10" s="1">
         <v>36877.03</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="W10" s="1">
+        <v>35720.79</v>
+      </c>
       <c r="X10" s="14">
         <f>AVERAGE(119999.79,117003.94,106132.19)</f>
         <v>114378.64</v>
@@ -5483,7 +5767,9 @@
       <c r="D11" s="1">
         <v>13172</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>13353</v>
+      </c>
       <c r="F11" s="14">
         <f>AVERAGE(19497,15890,17174)</f>
         <v>17520.333333333332</v>
@@ -5507,7 +5793,9 @@
       <c r="M11" s="1">
         <v>8651</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1">
+        <v>7988</v>
+      </c>
       <c r="O11" s="14">
         <f>AVERAGE(8745,12149,9449)</f>
         <v>10114.333333333334</v>
@@ -5531,7 +5819,9 @@
       <c r="V11" s="1">
         <v>38943.230000000003</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="W11" s="1">
+        <v>40552.269999999997</v>
+      </c>
       <c r="X11" s="14">
         <f>AVERAGE(121048.8,115030.75,104405.22)</f>
         <v>113494.92333333334</v>
@@ -5556,7 +5846,9 @@
       <c r="D12" s="1">
         <v>92250</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>1490</v>
+      </c>
       <c r="F12" s="14">
         <f>AVERAGE(192260,178990,179380)</f>
         <v>183543.33333333334</v>
@@ -5580,7 +5872,9 @@
       <c r="M12" s="1">
         <v>19476.54</v>
       </c>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>17516.66</v>
+      </c>
       <c r="O12" s="14">
         <f>AVERAGE(27525.22,27247,27153.45)</f>
         <v>27308.556666666667</v>
@@ -5604,7 +5898,9 @@
       <c r="V12" s="1">
         <v>66131.56</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="W12" s="1">
+        <v>70952.95</v>
+      </c>
       <c r="X12" s="14">
         <f>AVERAGE(274261.1,263443.34,271059.75)</f>
         <v>269588.0633333333</v>
@@ -5629,7 +5925,9 @@
       <c r="D13" s="3">
         <v>1943.98</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>1953.16</v>
+      </c>
       <c r="F13" s="15">
         <v>1943.98</v>
       </c>
@@ -5653,7 +5951,9 @@
       <c r="M13" s="1">
         <v>22938.36</v>
       </c>
-      <c r="N13" s="1"/>
+      <c r="N13" s="1">
+        <v>21753.58</v>
+      </c>
       <c r="O13" s="14">
         <f>AVERAGE(45731.91,39676.2,42516.11)</f>
         <v>42641.406666666669</v>
@@ -5677,7 +5977,9 @@
       <c r="V13" s="1">
         <v>209167.52</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1">
+        <v>218655.55</v>
+      </c>
       <c r="X13" s="14">
         <f>AVERAGE(1044777.76,1050611.75,1058082.78)</f>
         <v>1051157.43</v>
@@ -5702,7 +6004,9 @@
       <c r="D14" s="1">
         <v>4148.87</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>4786.0600000000004</v>
+      </c>
       <c r="F14" s="14">
         <f>AVERAGE(8413.89,9053.43,8139.43)</f>
         <v>8535.5833333333339</v>
@@ -5726,7 +6030,9 @@
       <c r="M14" s="1">
         <v>21433.16</v>
       </c>
-      <c r="N14" s="1"/>
+      <c r="N14" s="1">
+        <v>24404.94</v>
+      </c>
       <c r="O14" s="14">
         <f>AVERAGE(50639.03,52773.37,53019.09)</f>
         <v>52143.829999999994</v>
@@ -5750,7 +6056,9 @@
       <c r="V14" s="1">
         <v>925.25</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="W14" s="1">
+        <v>1047.43</v>
+      </c>
       <c r="X14" s="14">
         <f>AVERAGE(1580.3,1556.26,1531.77)</f>
         <v>1556.11</v>
@@ -5775,7 +6083,9 @@
       <c r="D15" s="1">
         <v>4938.62</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>5392.18</v>
+      </c>
       <c r="F15" s="14">
         <f>AVERAGE(10436.2,10515.28,10764.03)</f>
         <v>10571.836666666668</v>
@@ -5799,7 +6109,9 @@
       <c r="M15" s="1">
         <v>17465.62</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1">
+        <v>18768.060000000001</v>
+      </c>
       <c r="O15" s="14">
         <f>AVERAGE(30281.7,28948.48,27864.93)</f>
         <v>29031.703333333335</v>
@@ -5823,7 +6135,9 @@
       <c r="V15" s="1">
         <v>1695.61</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1">
+        <v>1944.15</v>
+      </c>
       <c r="X15" s="14">
         <f>AVERAGE(4322.14,3865.43,4106.19)</f>
         <v>4097.9199999999992</v>
@@ -5848,7 +6162,9 @@
       <c r="D16" s="3">
         <v>517</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>393</v>
+      </c>
       <c r="F16" s="3">
         <f>AVERAGE(523,694,586)</f>
         <v>601</v>
@@ -5872,7 +6188,9 @@
       <c r="M16" s="1">
         <v>17814.47</v>
       </c>
-      <c r="N16" s="1"/>
+      <c r="N16" s="1">
+        <v>20307.55</v>
+      </c>
       <c r="O16" s="14">
         <f>AVERAGE(39494.51,43021.33,43619.02)</f>
         <v>42044.953333333331</v>
@@ -5896,7 +6214,9 @@
       <c r="V16" s="1">
         <v>5946.93</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1">
+        <v>5694.36</v>
+      </c>
       <c r="X16" s="14">
         <f>AVERAGE(19012.37,18638.86,18931.57)</f>
         <v>18860.933333333331</v>
@@ -5921,7 +6241,9 @@
       <c r="D17" s="3">
         <v>291.58999999999997</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>323.66000000000003</v>
+      </c>
       <c r="F17" s="3">
         <f>AVERAGE(431.16,418.32,422.52)</f>
         <v>424</v>
@@ -5947,7 +6269,9 @@
       <c r="M17" s="1">
         <v>24691.06</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>24802.49</v>
+      </c>
       <c r="O17" s="14">
         <f>AVERAGE(57761.37,55503.47,57973.66)</f>
         <v>57079.5</v>
@@ -5971,7 +6295,9 @@
       <c r="V17" s="1">
         <v>7364.99</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1">
+        <v>7408.05</v>
+      </c>
       <c r="X17" s="14">
         <f>AVERAGE(29654.31,28805.35,29660.73)</f>
         <v>29373.463333333333</v>
@@ -5996,7 +6322,9 @@
       <c r="D18" s="1">
         <v>356.71</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>373.07</v>
+      </c>
       <c r="F18" s="14">
         <f>AVERAGE(573.88,576.15,503.95)</f>
         <v>551.32666666666671</v>
@@ -6020,7 +6348,9 @@
       <c r="M18" s="1">
         <v>14926.51</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>18900.41</v>
+      </c>
       <c r="O18" s="14">
         <f>AVERAGE(29654.14,29587.48,26846.83)</f>
         <v>28696.149999999998</v>
@@ -6044,7 +6374,9 @@
       <c r="V18" s="1">
         <v>16096</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="W18" s="1">
+        <v>16373</v>
+      </c>
       <c r="X18" s="14">
         <f>AVERAGE(20712,20221,20516)</f>
         <v>20483</v>
@@ -6069,7 +6401,9 @@
       <c r="D19" s="1">
         <v>492.25</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>452.67</v>
+      </c>
       <c r="F19" s="14">
         <f>AVERAGE(641.15,690.2,671.97)</f>
         <v>667.77333333333331</v>
@@ -6093,7 +6427,9 @@
       <c r="M19" s="1">
         <v>16252.61</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>17083.72</v>
+      </c>
       <c r="O19" s="14">
         <f>AVERAGE(27837.62,28079.33,27372.98)</f>
         <v>27763.309999999998</v>
@@ -6117,7 +6453,9 @@
       <c r="V19" s="1">
         <v>36872</v>
       </c>
-      <c r="W19" s="1"/>
+      <c r="W19" s="1">
+        <v>35948</v>
+      </c>
       <c r="X19" s="14">
         <f>AVERAGE(55395,53710,55185)</f>
         <v>54763.333333333336</v>
@@ -6142,7 +6480,9 @@
       <c r="D20" s="3">
         <v>744</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>608</v>
+      </c>
       <c r="F20" s="15">
         <v>744</v>
       </c>
@@ -6167,7 +6507,9 @@
       <c r="M20" s="1">
         <v>16441.939999999999</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>17078.29</v>
+      </c>
       <c r="O20" s="14">
         <f>AVERAGE(28486.61,27900.02,35382.74)</f>
         <v>30589.789999999997</v>
@@ -6191,7 +6533,9 @@
       <c r="V20" s="1">
         <v>70582</v>
       </c>
-      <c r="W20" s="1"/>
+      <c r="W20" s="1">
+        <v>70198</v>
+      </c>
       <c r="X20" s="14">
         <f>AVERAGE(113798,114572,110884)</f>
         <v>113084.66666666667</v>
@@ -6216,7 +6560,9 @@
       <c r="D21" s="1">
         <v>1741.09</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>1967.63</v>
+      </c>
       <c r="F21" s="14">
         <f>AVERAGE(4901.96,4962.22,4894.71)</f>
         <v>4919.63</v>
@@ -6240,7 +6586,9 @@
       <c r="M21" s="1">
         <v>9054.34</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>9002.3700000000008</v>
+      </c>
       <c r="O21" s="14">
         <f>AVERAGE(17572.51,17992.8,21124.48)</f>
         <v>18896.596666666665</v>
@@ -6264,7 +6612,9 @@
       <c r="V21" s="13">
         <v>543.95000000000005</v>
       </c>
-      <c r="W21" s="13"/>
+      <c r="W21" s="13">
+        <v>437.11</v>
+      </c>
       <c r="X21" s="14">
         <f>AVERAGE(805.9,739.32,748.97)</f>
         <v>764.73</v>
@@ -6289,7 +6639,9 @@
       <c r="D22" s="3">
         <v>661</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3">
+        <v>813</v>
+      </c>
       <c r="F22" s="15">
         <v>661</v>
       </c>
@@ -6314,7 +6666,9 @@
       <c r="M22" s="1">
         <v>33307.81</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>34803.33</v>
+      </c>
       <c r="O22" s="14">
         <f>AVERAGE(93802.91,100544.44,98586.28)</f>
         <v>97644.543333333335</v>
@@ -6338,7 +6692,9 @@
       <c r="V22" s="1">
         <v>770</v>
       </c>
-      <c r="W22" s="1"/>
+      <c r="W22" s="1">
+        <v>871</v>
+      </c>
       <c r="X22" s="14">
         <f>AVERAGE(1048,1049,1133)</f>
         <v>1076.6666666666667</v>
@@ -6363,7 +6719,9 @@
       <c r="D23" s="3">
         <v>1733</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>1351</v>
+      </c>
       <c r="F23" s="15">
         <v>1733</v>
       </c>
@@ -6388,7 +6746,9 @@
       <c r="M23" s="1">
         <v>47140.73</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>45668.23</v>
+      </c>
       <c r="O23" s="14">
         <f>AVERAGE(238515.69,230603.7,233199.28)</f>
         <v>234106.22333333336</v>
@@ -6412,7 +6772,9 @@
       <c r="V23" s="1">
         <v>89500</v>
       </c>
-      <c r="W23" s="1"/>
+      <c r="W23" s="1">
+        <v>117345.37</v>
+      </c>
       <c r="X23" s="14">
         <f>AVERAGE(284355.59,275262.73,290978.44)</f>
         <v>283532.25333333336</v>
@@ -6437,7 +6799,9 @@
       <c r="D24" s="3">
         <v>794</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <v>802</v>
+      </c>
       <c r="F24" s="15">
         <v>794</v>
       </c>
@@ -6462,7 +6826,9 @@
       <c r="M24" s="6">
         <v>2332</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="6">
+        <v>2150</v>
+      </c>
       <c r="O24" s="14">
         <f>AVERAGE(7378,7503,7350)</f>
         <v>7410.333333333333</v>
@@ -6486,7 +6852,9 @@
       <c r="V24" s="1">
         <v>2917.62</v>
       </c>
-      <c r="W24" s="1"/>
+      <c r="W24" s="1">
+        <v>3247.49</v>
+      </c>
       <c r="X24" s="14">
         <f>AVERAGE(7175.18,7038.94,7174.41)</f>
         <v>7129.5099999999993</v>
@@ -6521,7 +6889,9 @@
       <c r="V25" s="3">
         <v>2785.62</v>
       </c>
-      <c r="W25" s="3"/>
+      <c r="W25" s="3">
+        <v>3035.89</v>
+      </c>
       <c r="X25" s="15">
         <v>2785.62</v>
       </c>
@@ -6563,7 +6933,9 @@
       <c r="V26" s="3">
         <v>3118.04</v>
       </c>
-      <c r="W26" s="3"/>
+      <c r="W26" s="3">
+        <v>2959.96</v>
+      </c>
       <c r="X26" s="15">
         <v>3118.04</v>
       </c>

</xml_diff>

<commit_message>
Adição dos resultados da busca local com vizinhança por inserção
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AS38"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH18" sqref="AH18"/>
+    <sheetView topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO26" sqref="AO26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1125,9 @@
       <c r="J3" s="25">
         <v>625.97</v>
       </c>
-      <c r="K3" s="25"/>
+      <c r="K3" s="25">
+        <v>625.97</v>
+      </c>
       <c r="L3" s="25"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18">
@@ -1164,7 +1166,9 @@
       <c r="Y3" s="25">
         <v>668</v>
       </c>
-      <c r="Z3" s="25"/>
+      <c r="Z3" s="25">
+        <v>668</v>
+      </c>
       <c r="AA3" s="25"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="17">
@@ -1203,7 +1207,9 @@
       <c r="AN3" s="25">
         <v>25126.84</v>
       </c>
-      <c r="AO3" s="25"/>
+      <c r="AO3" s="25">
+        <v>25126.84</v>
+      </c>
       <c r="AP3" s="25"/>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
@@ -1271,7 +1277,9 @@
       <c r="Y4" s="25">
         <v>10630.39</v>
       </c>
-      <c r="Z4" s="25"/>
+      <c r="Z4" s="25">
+        <v>10068.39</v>
+      </c>
       <c r="AA4" s="25"/>
       <c r="AB4" s="18"/>
       <c r="AC4" s="17">
@@ -1310,7 +1318,9 @@
       <c r="AN4" s="25">
         <v>7769.74</v>
       </c>
-      <c r="AO4" s="25"/>
+      <c r="AO4" s="25">
+        <v>7564.94</v>
+      </c>
       <c r="AP4" s="25"/>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
@@ -1351,7 +1361,9 @@
       <c r="J5" s="3">
         <v>1373</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>1373</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3">
         <v>1239</v>
@@ -1388,7 +1400,9 @@
       <c r="Y5" s="25">
         <v>1376</v>
       </c>
-      <c r="Z5" s="25"/>
+      <c r="Z5" s="25">
+        <v>1376</v>
+      </c>
       <c r="AA5" s="25"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="17"/>
@@ -1423,7 +1437,9 @@
       <c r="AN5" s="25">
         <v>10765.78</v>
       </c>
-      <c r="AO5" s="25"/>
+      <c r="AO5" s="25">
+        <v>10765.78</v>
+      </c>
       <c r="AP5" s="25"/>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
@@ -1464,7 +1480,9 @@
       <c r="J6" s="25">
         <v>5619</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="25">
+        <v>5553</v>
+      </c>
       <c r="L6" s="25"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
@@ -1530,7 +1548,9 @@
       <c r="AN6" s="25">
         <v>22828.74</v>
       </c>
-      <c r="AO6" s="25"/>
+      <c r="AO6" s="25">
+        <v>22109.3</v>
+      </c>
       <c r="AP6" s="25"/>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
@@ -1570,7 +1590,9 @@
       <c r="J7" s="3">
         <v>292</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>292</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3">
         <v>246</v>
@@ -1642,7 +1664,9 @@
       <c r="AN7" s="25">
         <v>10778.34</v>
       </c>
-      <c r="AO7" s="25"/>
+      <c r="AO7" s="25">
+        <v>10742.86</v>
+      </c>
       <c r="AP7" s="25"/>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
@@ -1682,7 +1706,9 @@
       <c r="J8" s="3">
         <v>352</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>352</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="4">
         <v>282</v>
@@ -1754,7 +1780,9 @@
       <c r="AN8" s="25">
         <v>15403.26</v>
       </c>
-      <c r="AO8" s="25"/>
+      <c r="AO8" s="25">
+        <v>15403.26</v>
+      </c>
       <c r="AP8" s="25"/>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
@@ -1795,7 +1823,9 @@
       <c r="J9" s="3">
         <v>556.80999999999995</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>556.80999999999995</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="5">
         <v>480.48033445701299</v>
@@ -1863,7 +1893,9 @@
       <c r="AN9" s="25">
         <v>22868.63</v>
       </c>
-      <c r="AO9" s="25"/>
+      <c r="AO9" s="25">
+        <v>22375.1</v>
+      </c>
       <c r="AP9" s="25"/>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
@@ -1904,7 +1936,9 @@
       <c r="J10" s="25">
         <v>14272</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="25">
+        <v>14272.3</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18">
@@ -1970,7 +2004,9 @@
       <c r="AN10" s="25">
         <v>8023.61</v>
       </c>
-      <c r="AO10" s="25"/>
+      <c r="AO10" s="25">
+        <v>8023.61</v>
+      </c>
       <c r="AP10" s="25"/>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
@@ -2007,7 +2043,9 @@
       <c r="J11" s="25">
         <v>6116</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="25">
+        <v>6116</v>
+      </c>
       <c r="L11" s="25"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
@@ -2042,7 +2080,9 @@
       <c r="Y11" s="25">
         <v>3454</v>
       </c>
-      <c r="Z11" s="25"/>
+      <c r="Z11" s="25">
+        <v>3454</v>
+      </c>
       <c r="AA11" s="25"/>
       <c r="AB11" s="18"/>
       <c r="AC11" s="17">
@@ -2081,7 +2121,9 @@
       <c r="AN11" s="25">
         <v>12311.53</v>
       </c>
-      <c r="AO11" s="25"/>
+      <c r="AO11" s="25">
+        <v>12311.53</v>
+      </c>
       <c r="AP11" s="25"/>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
@@ -2118,7 +2160,9 @@
       <c r="J12" s="25">
         <v>16600</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="25">
+        <v>11050</v>
+      </c>
       <c r="L12" s="25"/>
       <c r="M12" s="12"/>
       <c r="N12" s="18"/>
@@ -2153,7 +2197,9 @@
       <c r="Y12" s="25">
         <v>5015.0200000000004</v>
       </c>
-      <c r="Z12" s="25"/>
+      <c r="Z12" s="25">
+        <v>5015.0200000000004</v>
+      </c>
       <c r="AA12" s="25"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="17">
@@ -2192,7 +2238,9 @@
       <c r="AN12" s="25">
         <v>22324.31</v>
       </c>
-      <c r="AO12" s="25"/>
+      <c r="AO12" s="25">
+        <v>22074.32</v>
+      </c>
       <c r="AP12" s="25"/>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
@@ -2227,7 +2275,9 @@
       <c r="J13" s="3">
         <v>249.88</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>249.88</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
         <v>224.88</v>
@@ -2268,7 +2318,9 @@
       <c r="Y13" s="25">
         <v>6632.55</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="25">
+        <v>6632.55</v>
+      </c>
       <c r="AA13" s="25"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="17">
@@ -2307,7 +2359,9 @@
       <c r="AN13" s="25">
         <v>67085.41</v>
       </c>
-      <c r="AO13" s="25"/>
+      <c r="AO13" s="25">
+        <v>66266.210000000006</v>
+      </c>
       <c r="AP13" s="25"/>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
@@ -2344,7 +2398,9 @@
       <c r="J14" s="25">
         <v>1207.1500000000001</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="25">
+        <v>1205.2</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18">
@@ -2383,7 +2439,9 @@
       <c r="Y14" s="25">
         <v>6767.07</v>
       </c>
-      <c r="Z14" s="25"/>
+      <c r="Z14" s="25">
+        <v>6767.07</v>
+      </c>
       <c r="AA14" s="25"/>
       <c r="AB14" s="18"/>
       <c r="AC14" s="17">
@@ -2422,7 +2480,9 @@
       <c r="AN14" s="25">
         <v>266.87</v>
       </c>
-      <c r="AO14" s="25"/>
+      <c r="AO14" s="25">
+        <v>263.3</v>
+      </c>
       <c r="AP14" s="25"/>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
@@ -2463,7 +2523,9 @@
       <c r="J15" s="25">
         <v>1304.57</v>
       </c>
-      <c r="K15" s="25"/>
+      <c r="K15" s="25">
+        <v>1304.57</v>
+      </c>
       <c r="L15" s="25"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18">
@@ -2502,7 +2564,9 @@
       <c r="Y15" s="25">
         <v>5507.89</v>
       </c>
-      <c r="Z15" s="25"/>
+      <c r="Z15" s="25">
+        <v>5507.89</v>
+      </c>
       <c r="AA15" s="25"/>
       <c r="AB15" s="18"/>
       <c r="AC15" s="17">
@@ -2541,7 +2605,9 @@
       <c r="AN15" s="25">
         <v>560.07000000000005</v>
       </c>
-      <c r="AO15" s="25"/>
+      <c r="AO15" s="25">
+        <v>558.64</v>
+      </c>
       <c r="AP15" s="25"/>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
@@ -2582,7 +2648,9 @@
       <c r="J16" s="3">
         <v>100</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>100</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3">
         <v>99</v>
@@ -2623,7 +2691,9 @@
       <c r="Y16" s="25">
         <v>5119.54</v>
       </c>
-      <c r="Z16" s="25"/>
+      <c r="Z16" s="25">
+        <v>5119.54</v>
+      </c>
       <c r="AA16" s="25"/>
       <c r="AB16" s="18"/>
       <c r="AC16" s="17">
@@ -2662,7 +2732,9 @@
       <c r="AN16" s="25">
         <v>1733.54</v>
       </c>
-      <c r="AO16" s="25"/>
+      <c r="AO16" s="25">
+        <v>1724.97</v>
+      </c>
       <c r="AP16" s="25"/>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
@@ -2699,7 +2771,9 @@
       <c r="J17" s="3">
         <v>77.040000000000006</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>77.040000000000006</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3">
         <v>76.72</v>
@@ -2740,7 +2814,9 @@
       <c r="Y17" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="Z17" s="25"/>
+      <c r="Z17" s="25">
+        <v>6789.91</v>
+      </c>
       <c r="AA17" s="25"/>
       <c r="AB17" s="18"/>
       <c r="AC17" s="17">
@@ -2779,7 +2855,9 @@
       <c r="AN17" s="25">
         <v>2260.06</v>
       </c>
-      <c r="AO17" s="25"/>
+      <c r="AO17" s="25">
+        <v>2280.65</v>
+      </c>
       <c r="AP17" s="25"/>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
@@ -2816,7 +2894,9 @@
       <c r="J18" s="25">
         <v>97.38</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="25">
+        <v>97.38</v>
+      </c>
       <c r="L18" s="25"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18">
@@ -2855,7 +2935,9 @@
       <c r="Y18" s="25">
         <v>4293.0200000000004</v>
       </c>
-      <c r="Z18" s="25"/>
+      <c r="Z18" s="25">
+        <v>4293.0200000000004</v>
+      </c>
       <c r="AA18" s="25"/>
       <c r="AB18" s="18"/>
       <c r="AC18" s="17">
@@ -2894,7 +2976,9 @@
       <c r="AN18" s="25">
         <v>5243</v>
       </c>
-      <c r="AO18" s="25"/>
+      <c r="AO18" s="25">
+        <v>5238</v>
+      </c>
       <c r="AP18" s="25"/>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
@@ -2931,7 +3015,9 @@
       <c r="J19" s="25">
         <v>150.4</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="25">
+        <v>150.4</v>
+      </c>
       <c r="L19" s="25"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18">
@@ -2970,7 +3056,9 @@
       <c r="Y19" s="25">
         <v>5246.28</v>
       </c>
-      <c r="Z19" s="25"/>
+      <c r="Z19" s="25">
+        <v>5246.28</v>
+      </c>
       <c r="AA19" s="25"/>
       <c r="AB19" s="18"/>
       <c r="AC19" s="17">
@@ -3009,7 +3097,9 @@
       <c r="AN19" s="25">
         <v>12275</v>
       </c>
-      <c r="AO19" s="25"/>
+      <c r="AO19" s="25">
+        <v>12252</v>
+      </c>
       <c r="AP19" s="25"/>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
@@ -3045,7 +3135,9 @@
       <c r="J20" s="3">
         <v>147</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3">
+        <v>147</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3">
         <v>145</v>
@@ -3086,7 +3178,9 @@
       <c r="Y20" s="25">
         <v>4087.21</v>
       </c>
-      <c r="Z20" s="25"/>
+      <c r="Z20" s="25">
+        <v>4087.21</v>
+      </c>
       <c r="AA20" s="25"/>
       <c r="AB20" s="18"/>
       <c r="AC20" s="17">
@@ -3125,7 +3219,9 @@
       <c r="AN20" s="25">
         <v>22289</v>
       </c>
-      <c r="AO20" s="25"/>
+      <c r="AO20" s="25">
+        <v>22289</v>
+      </c>
       <c r="AP20" s="25"/>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
@@ -3162,7 +3258,9 @@
       <c r="J21" s="25">
         <v>559.01</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="25">
+        <v>559.01</v>
+      </c>
       <c r="L21" s="25"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18">
@@ -3201,7 +3299,9 @@
       <c r="Y21" s="25">
         <v>2109.4299999999998</v>
       </c>
-      <c r="Z21" s="25"/>
+      <c r="Z21" s="25">
+        <v>2109.4299999999998</v>
+      </c>
       <c r="AA21" s="25"/>
       <c r="AB21" s="18"/>
       <c r="AC21" s="17">
@@ -3240,7 +3340,9 @@
       <c r="AN21" s="25">
         <v>129.15</v>
       </c>
-      <c r="AO21" s="25"/>
+      <c r="AO21" s="25">
+        <v>129.15</v>
+      </c>
       <c r="AP21" s="25"/>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
@@ -3280,7 +3382,9 @@
       <c r="J22" s="3">
         <v>154</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3">
+        <v>165</v>
+      </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3">
         <v>143</v>
@@ -3321,7 +3425,9 @@
       <c r="Y22" s="25">
         <v>9035.18</v>
       </c>
-      <c r="Z22" s="25"/>
+      <c r="Z22" s="25">
+        <v>8860.4699999999993</v>
+      </c>
       <c r="AA22" s="25"/>
       <c r="AB22" s="18"/>
       <c r="AC22" s="17">
@@ -3360,7 +3466,9 @@
       <c r="AN22" s="25">
         <v>146</v>
       </c>
-      <c r="AO22" s="25"/>
+      <c r="AO22" s="25">
+        <v>146</v>
+      </c>
       <c r="AP22" s="25"/>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
@@ -3400,7 +3508,9 @@
       <c r="J23" s="3">
         <v>258</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>258</v>
+      </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3">
         <v>181</v>
@@ -3441,7 +3551,9 @@
       <c r="Y23" s="25">
         <v>13172.65</v>
       </c>
-      <c r="Z23" s="25"/>
+      <c r="Z23" s="25">
+        <v>13194.03</v>
+      </c>
       <c r="AA23" s="25"/>
       <c r="AB23" s="18"/>
       <c r="AC23" s="17"/>
@@ -3476,7 +3588,9 @@
       <c r="AN23" s="25">
         <v>27500</v>
       </c>
-      <c r="AO23" s="25"/>
+      <c r="AO23" s="25">
+        <v>27500</v>
+      </c>
       <c r="AP23" s="25"/>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
@@ -3512,7 +3626,9 @@
       <c r="J24" s="3">
         <v>162</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>162</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3">
         <v>162</v>
@@ -3554,7 +3670,9 @@
       <c r="Y24" s="25">
         <v>726</v>
       </c>
-      <c r="Z24" s="25"/>
+      <c r="Z24" s="25">
+        <v>720</v>
+      </c>
       <c r="AA24" s="25"/>
       <c r="AB24" s="18"/>
       <c r="AC24" s="17"/>
@@ -3589,7 +3707,9 @@
       <c r="AN24" s="25">
         <v>964.26</v>
       </c>
-      <c r="AO24" s="25"/>
+      <c r="AO24" s="25">
+        <v>964.26</v>
+      </c>
       <c r="AP24" s="25"/>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
@@ -3628,7 +3748,9 @@
       <c r="AN25" s="3">
         <v>826.08</v>
       </c>
-      <c r="AO25" s="3"/>
+      <c r="AO25" s="3">
+        <v>826.08</v>
+      </c>
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3">
         <v>714.33</v>
@@ -3695,7 +3817,9 @@
       <c r="AN26" s="3">
         <v>456.58</v>
       </c>
-      <c r="AO26" s="3"/>
+      <c r="AO26" s="3">
+        <v>456.58</v>
+      </c>
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3">
         <v>662.17</v>
@@ -3863,7 +3987,7 @@
   <dimension ref="B1:AS38"/>
   <sheetViews>
     <sheetView topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+      <selection activeCell="AG37" sqref="AG37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,7 +4240,9 @@
       <c r="J3" s="25">
         <v>1322.11</v>
       </c>
-      <c r="K3" s="25"/>
+      <c r="K3" s="25">
+        <v>1318.03</v>
+      </c>
       <c r="L3" s="25"/>
       <c r="M3" s="1"/>
       <c r="N3" s="18">
@@ -4155,7 +4281,9 @@
       <c r="Y3" s="25">
         <v>2139</v>
       </c>
-      <c r="Z3" s="25"/>
+      <c r="Z3" s="25">
+        <v>2122</v>
+      </c>
       <c r="AA3" s="25"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="18">
@@ -4194,7 +4322,9 @@
       <c r="AN3" s="25">
         <v>42676.77</v>
       </c>
-      <c r="AO3" s="25"/>
+      <c r="AO3" s="25">
+        <v>42676.77</v>
+      </c>
       <c r="AP3" s="25"/>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
@@ -4262,7 +4392,9 @@
       <c r="Y4" s="25">
         <v>21617.45</v>
       </c>
-      <c r="Z4" s="25"/>
+      <c r="Z4" s="25">
+        <v>21055.45</v>
+      </c>
       <c r="AA4" s="25"/>
       <c r="AB4" s="18"/>
       <c r="AC4" s="18">
@@ -4301,7 +4433,9 @@
       <c r="AN4" s="25">
         <v>16472.98</v>
       </c>
-      <c r="AO4" s="25"/>
+      <c r="AO4" s="25">
+        <v>15960.98</v>
+      </c>
       <c r="AP4" s="25"/>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
@@ -4342,7 +4476,9 @@
       <c r="J5" s="3">
         <v>3447</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>3231</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
         <v>76</v>
@@ -4379,7 +4515,9 @@
       <c r="Y5" s="25">
         <v>3120</v>
       </c>
-      <c r="Z5" s="25"/>
+      <c r="Z5" s="25">
+        <v>3120</v>
+      </c>
       <c r="AA5" s="25"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
@@ -4414,7 +4552,9 @@
       <c r="AN5" s="25">
         <v>24187.51</v>
       </c>
-      <c r="AO5" s="25"/>
+      <c r="AO5" s="25">
+        <v>25633.65</v>
+      </c>
       <c r="AP5" s="25"/>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
@@ -4455,7 +4595,9 @@
       <c r="J6" s="25">
         <v>14250</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="25">
+        <v>14128</v>
+      </c>
       <c r="L6" s="25"/>
       <c r="M6" s="1"/>
       <c r="N6" s="18"/>
@@ -4521,7 +4663,9 @@
       <c r="AN6" s="25">
         <v>53346.76</v>
       </c>
-      <c r="AO6" s="25"/>
+      <c r="AO6" s="25">
+        <v>46726.91</v>
+      </c>
       <c r="AP6" s="25"/>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
@@ -4561,7 +4705,9 @@
       <c r="J7" s="3">
         <v>581</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>581</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
         <v>81</v>
@@ -4633,7 +4779,9 @@
       <c r="AN7" s="25">
         <v>26341.82</v>
       </c>
-      <c r="AO7" s="25"/>
+      <c r="AO7" s="25">
+        <v>26306.34</v>
+      </c>
       <c r="AP7" s="25"/>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
@@ -4673,7 +4821,9 @@
       <c r="J8" s="3">
         <v>816</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>816</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
         <v>83</v>
@@ -4745,7 +4895,9 @@
       <c r="AN8" s="25">
         <v>33363.86</v>
       </c>
-      <c r="AO8" s="25"/>
+      <c r="AO8" s="25">
+        <v>32745.67</v>
+      </c>
       <c r="AP8" s="25"/>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
@@ -4786,7 +4938,9 @@
       <c r="J9" s="3">
         <v>1766.5</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>1766.5</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="5">
         <v>3303.71452420693</v>
@@ -4854,7 +5008,9 @@
       <c r="AN9" s="25">
         <v>49141.62</v>
       </c>
-      <c r="AO9" s="25"/>
+      <c r="AO9" s="25">
+        <v>48156.03</v>
+      </c>
       <c r="AP9" s="25"/>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
@@ -4895,7 +5051,9 @@
       <c r="J10" s="25">
         <v>29120.17</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="25">
+        <v>28429.05</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="1"/>
       <c r="N10" s="18">
@@ -4961,7 +5119,9 @@
       <c r="AN10" s="25">
         <v>22934.79</v>
       </c>
-      <c r="AO10" s="25"/>
+      <c r="AO10" s="25">
+        <v>21889.15</v>
+      </c>
       <c r="AP10" s="25"/>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
@@ -4998,7 +5158,9 @@
       <c r="J11" s="25">
         <v>10262</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="25">
+        <v>10262</v>
+      </c>
       <c r="L11" s="25"/>
       <c r="M11" s="1"/>
       <c r="N11" s="18"/>
@@ -5033,7 +5195,9 @@
       <c r="Y11" s="25">
         <v>6284</v>
       </c>
-      <c r="Z11" s="25"/>
+      <c r="Z11" s="25">
+        <v>6284</v>
+      </c>
       <c r="AA11" s="25"/>
       <c r="AB11" s="18"/>
       <c r="AC11" s="18">
@@ -5072,7 +5236,9 @@
       <c r="AN11" s="25">
         <v>26442.77</v>
       </c>
-      <c r="AO11" s="25"/>
+      <c r="AO11" s="25">
+        <v>25630.01</v>
+      </c>
       <c r="AP11" s="25"/>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
@@ -5109,7 +5275,9 @@
       <c r="J12" s="25">
         <v>22550</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="25">
+        <v>25610</v>
+      </c>
       <c r="L12" s="25"/>
       <c r="M12" s="1"/>
       <c r="N12" s="18"/>
@@ -5144,7 +5312,9 @@
       <c r="Y12" s="25">
         <v>11430.22</v>
       </c>
-      <c r="Z12" s="25"/>
+      <c r="Z12" s="25">
+        <v>10638.41</v>
+      </c>
       <c r="AA12" s="25"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="18">
@@ -5183,7 +5353,9 @@
       <c r="AN12" s="25">
         <v>40759.29</v>
       </c>
-      <c r="AO12" s="25"/>
+      <c r="AO12" s="25">
+        <v>40496.9</v>
+      </c>
       <c r="AP12" s="25"/>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
@@ -5218,7 +5390,9 @@
       <c r="J13" s="3">
         <v>1454.84</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>1454.84</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
         <v>966.37</v>
@@ -5259,7 +5433,9 @@
       <c r="Y13" s="25">
         <v>15430.01</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="25">
+        <v>14772.08</v>
+      </c>
       <c r="AA13" s="25"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18">
@@ -5298,7 +5474,9 @@
       <c r="AN13" s="25">
         <v>131441.76</v>
       </c>
-      <c r="AO13" s="25"/>
+      <c r="AO13" s="25">
+        <v>129086.31</v>
+      </c>
       <c r="AP13" s="25"/>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
@@ -5335,7 +5513,9 @@
       <c r="J14" s="25">
         <v>2710.19</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="25">
+        <v>2708.24</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="M14" s="1"/>
       <c r="N14" s="18">
@@ -5374,7 +5554,9 @@
       <c r="Y14" s="25">
         <v>13485.45</v>
       </c>
-      <c r="Z14" s="25"/>
+      <c r="Z14" s="25">
+        <v>13485.45</v>
+      </c>
       <c r="AA14" s="25"/>
       <c r="AB14" s="18"/>
       <c r="AC14" s="18">
@@ -5413,7 +5595,9 @@
       <c r="AN14" s="25">
         <v>584.59</v>
       </c>
-      <c r="AO14" s="25"/>
+      <c r="AO14" s="25">
+        <v>578.70000000000005</v>
+      </c>
       <c r="AP14" s="25"/>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
@@ -5454,7 +5638,9 @@
       <c r="J15" s="25">
         <v>3169.82</v>
       </c>
-      <c r="K15" s="25"/>
+      <c r="K15" s="25">
+        <v>3082.54</v>
+      </c>
       <c r="L15" s="25"/>
       <c r="M15" s="1"/>
       <c r="N15" s="18">
@@ -5493,7 +5679,9 @@
       <c r="Y15" s="25">
         <v>11418.42</v>
       </c>
-      <c r="Z15" s="25"/>
+      <c r="Z15" s="25">
+        <v>11366.47</v>
+      </c>
       <c r="AA15" s="25"/>
       <c r="AB15" s="18"/>
       <c r="AC15" s="18">
@@ -5532,7 +5720,9 @@
       <c r="AN15" s="25">
         <v>1135.3800000000001</v>
       </c>
-      <c r="AO15" s="25"/>
+      <c r="AO15" s="25">
+        <v>1133.95</v>
+      </c>
       <c r="AP15" s="25"/>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
@@ -5573,7 +5763,9 @@
       <c r="J16" s="3">
         <v>239</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>239</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3">
         <v>230</v>
@@ -5614,7 +5806,9 @@
       <c r="Y16" s="25">
         <v>12099.43</v>
       </c>
-      <c r="Z16" s="25"/>
+      <c r="Z16" s="25">
+        <v>11909.87</v>
+      </c>
       <c r="AA16" s="25"/>
       <c r="AB16" s="18"/>
       <c r="AC16" s="18">
@@ -5653,7 +5847,9 @@
       <c r="AN16" s="25">
         <v>3448.29</v>
       </c>
-      <c r="AO16" s="25"/>
+      <c r="AO16" s="25">
+        <v>3407.23</v>
+      </c>
       <c r="AP16" s="25"/>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
@@ -5690,7 +5886,9 @@
       <c r="J17" s="3">
         <v>181.41</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>181.41</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
         <v>85</v>
@@ -5731,7 +5929,9 @@
       <c r="Y17" s="25">
         <v>17110.47</v>
       </c>
-      <c r="Z17" s="25"/>
+      <c r="Z17" s="25">
+        <v>16276.03</v>
+      </c>
       <c r="AA17" s="25"/>
       <c r="AB17" s="18"/>
       <c r="AC17" s="18">
@@ -5770,7 +5970,9 @@
       <c r="AN17" s="25">
         <v>4617.92</v>
       </c>
-      <c r="AO17" s="25"/>
+      <c r="AO17" s="25">
+        <v>4535.42</v>
+      </c>
       <c r="AP17" s="25"/>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
@@ -5807,7 +6009,9 @@
       <c r="J18" s="25">
         <v>229.64</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="25">
+        <v>229.64</v>
+      </c>
       <c r="L18" s="25"/>
       <c r="M18" s="1"/>
       <c r="N18" s="18">
@@ -5846,7 +6050,9 @@
       <c r="Y18" s="25">
         <v>9555.73</v>
       </c>
-      <c r="Z18" s="25"/>
+      <c r="Z18" s="25">
+        <v>9555.73</v>
+      </c>
       <c r="AA18" s="25"/>
       <c r="AB18" s="18"/>
       <c r="AC18" s="18">
@@ -5885,7 +6091,9 @@
       <c r="AN18" s="25">
         <v>10537</v>
       </c>
-      <c r="AO18" s="25"/>
+      <c r="AO18" s="25">
+        <v>10528</v>
+      </c>
       <c r="AP18" s="25"/>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
@@ -5922,7 +6130,9 @@
       <c r="J19" s="25">
         <v>314.43</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="25">
+        <v>314.43</v>
+      </c>
       <c r="L19" s="25"/>
       <c r="M19" s="1"/>
       <c r="N19" s="18">
@@ -5961,7 +6171,9 @@
       <c r="Y19" s="25">
         <v>10636.85</v>
       </c>
-      <c r="Z19" s="25"/>
+      <c r="Z19" s="25">
+        <v>10587.17</v>
+      </c>
       <c r="AA19" s="25"/>
       <c r="AB19" s="18"/>
       <c r="AC19" s="18">
@@ -6000,7 +6212,9 @@
       <c r="AN19" s="25">
         <v>23558</v>
       </c>
-      <c r="AO19" s="25"/>
+      <c r="AO19" s="25">
+        <v>23495</v>
+      </c>
       <c r="AP19" s="25"/>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
@@ -6036,7 +6250,9 @@
       <c r="J20" s="3">
         <v>334</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3">
+        <v>331</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3">
         <v>308</v>
@@ -6077,7 +6293,9 @@
       <c r="Y20" s="25">
         <v>10167.799999999999</v>
       </c>
-      <c r="Z20" s="25"/>
+      <c r="Z20" s="25">
+        <v>9911.8700000000008</v>
+      </c>
       <c r="AA20" s="25"/>
       <c r="AB20" s="18"/>
       <c r="AC20" s="18">
@@ -6116,7 +6334,9 @@
       <c r="AN20" s="25">
         <v>46817</v>
       </c>
-      <c r="AO20" s="25"/>
+      <c r="AO20" s="25">
+        <v>46817</v>
+      </c>
       <c r="AP20" s="25"/>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
@@ -6153,7 +6373,9 @@
       <c r="J21" s="25">
         <v>1176.3699999999999</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="25">
+        <v>1176.3699999999999</v>
+      </c>
       <c r="L21" s="25"/>
       <c r="M21" s="1"/>
       <c r="N21" s="18">
@@ -6192,7 +6414,9 @@
       <c r="Y21" s="25">
         <v>5848.46</v>
       </c>
-      <c r="Z21" s="25"/>
+      <c r="Z21" s="25">
+        <v>5673.74</v>
+      </c>
       <c r="AA21" s="25"/>
       <c r="AB21" s="18"/>
       <c r="AC21" s="18">
@@ -6231,7 +6455,9 @@
       <c r="AN21" s="25">
         <v>320.01</v>
       </c>
-      <c r="AO21" s="25"/>
+      <c r="AO21" s="25">
+        <v>323.07</v>
+      </c>
       <c r="AP21" s="25"/>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
@@ -6271,7 +6497,9 @@
       <c r="J22" s="3">
         <v>359</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3">
+        <v>359</v>
+      </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3">
         <v>380</v>
@@ -6312,7 +6540,9 @@
       <c r="Y22" s="25">
         <v>22464.99</v>
       </c>
-      <c r="Z22" s="25"/>
+      <c r="Z22" s="25">
+        <v>21495.02</v>
+      </c>
       <c r="AA22" s="25"/>
       <c r="AB22" s="18"/>
       <c r="AC22" s="18">
@@ -6351,7 +6581,9 @@
       <c r="AN22" s="25">
         <v>425</v>
       </c>
-      <c r="AO22" s="25"/>
+      <c r="AO22" s="25">
+        <v>425</v>
+      </c>
       <c r="AP22" s="25"/>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
@@ -6391,7 +6623,9 @@
       <c r="J23" s="3">
         <v>989</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>989</v>
+      </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3">
         <v>683</v>
@@ -6432,7 +6666,9 @@
       <c r="Y23" s="25">
         <v>28386.639999999999</v>
       </c>
-      <c r="Z23" s="25"/>
+      <c r="Z23" s="25">
+        <v>28189.25</v>
+      </c>
       <c r="AA23" s="25"/>
       <c r="AB23" s="18"/>
       <c r="AC23" s="18"/>
@@ -6467,7 +6703,9 @@
       <c r="AN23" s="25">
         <v>55500</v>
       </c>
-      <c r="AO23" s="25"/>
+      <c r="AO23" s="25">
+        <v>55500</v>
+      </c>
       <c r="AP23" s="25"/>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
@@ -6503,7 +6741,9 @@
       <c r="J24" s="3">
         <v>490</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>490</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3">
         <v>409</v>
@@ -6544,7 +6784,9 @@
       <c r="Y24" s="25">
         <v>1356</v>
       </c>
-      <c r="Z24" s="25"/>
+      <c r="Z24" s="25">
+        <v>1341</v>
+      </c>
       <c r="AA24" s="25"/>
       <c r="AB24" s="18"/>
       <c r="AC24" s="18"/>
@@ -6579,7 +6821,9 @@
       <c r="AN24" s="25">
         <v>1803.89</v>
       </c>
-      <c r="AO24" s="25"/>
+      <c r="AO24" s="25">
+        <v>1803.89</v>
+      </c>
       <c r="AP24" s="25"/>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
@@ -6629,7 +6873,9 @@
       <c r="AN25" s="3">
         <v>1981.71</v>
       </c>
-      <c r="AO25" s="3"/>
+      <c r="AO25" s="3">
+        <v>1981.71</v>
+      </c>
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3">
         <v>1505.95</v>
@@ -6692,7 +6938,9 @@
       <c r="AN26" s="3">
         <v>2062.92</v>
       </c>
-      <c r="AO26" s="3"/>
+      <c r="AO26" s="3">
+        <v>2062.92</v>
+      </c>
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3">
         <v>1647.33</v>
@@ -6841,8 +7089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN20" sqref="AN20"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO19" sqref="AO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7091,7 +7339,9 @@
       <c r="J3" s="25">
         <v>2071.5700000000002</v>
       </c>
-      <c r="K3" s="25"/>
+      <c r="K3" s="25">
+        <v>2055.2600000000002</v>
+      </c>
       <c r="L3" s="25"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18">
@@ -7130,7 +7380,9 @@
       <c r="Y3" s="25">
         <v>3456</v>
       </c>
-      <c r="Z3" s="25"/>
+      <c r="Z3" s="25">
+        <v>3340</v>
+      </c>
       <c r="AA3" s="25"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="17">
@@ -7169,7 +7421,9 @@
       <c r="AN3" s="25">
         <v>63830.12</v>
       </c>
-      <c r="AO3" s="25"/>
+      <c r="AO3" s="25">
+        <v>63719.25</v>
+      </c>
       <c r="AP3" s="25"/>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
@@ -7237,7 +7491,9 @@
       <c r="Y4" s="25">
         <v>40637.25</v>
       </c>
-      <c r="Z4" s="25"/>
+      <c r="Z4" s="25">
+        <v>39556.93</v>
+      </c>
       <c r="AA4" s="25"/>
       <c r="AB4" s="18"/>
       <c r="AC4" s="17">
@@ -7276,7 +7532,9 @@
       <c r="AN4" s="25">
         <v>32157.040000000001</v>
       </c>
-      <c r="AO4" s="25"/>
+      <c r="AO4" s="25">
+        <v>31557.54</v>
+      </c>
       <c r="AP4" s="25"/>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
@@ -7317,7 +7575,9 @@
       <c r="J5" s="3">
         <v>6962</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>6649</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
         <v>77</v>
@@ -7354,7 +7614,9 @@
       <c r="Y5" s="25">
         <v>4673</v>
       </c>
-      <c r="Z5" s="25"/>
+      <c r="Z5" s="25">
+        <v>4643</v>
+      </c>
       <c r="AA5" s="25"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="17"/>
@@ -7389,7 +7651,9 @@
       <c r="AN5" s="25">
         <v>38002.1</v>
       </c>
-      <c r="AO5" s="25"/>
+      <c r="AO5" s="25">
+        <v>39424.629999999997</v>
+      </c>
       <c r="AP5" s="25"/>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
@@ -7430,7 +7694,9 @@
       <c r="J6" s="25">
         <v>22861</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="25">
+        <v>22317</v>
+      </c>
       <c r="L6" s="25"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
@@ -7496,7 +7762,9 @@
       <c r="AN6" s="25">
         <v>83744.61</v>
       </c>
-      <c r="AO6" s="25"/>
+      <c r="AO6" s="25">
+        <v>77379.09</v>
+      </c>
       <c r="AP6" s="25"/>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
@@ -7536,7 +7804,9 @@
       <c r="J7" s="3">
         <v>1035</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>1035</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
         <v>82</v>
@@ -7608,7 +7878,9 @@
       <c r="AN7" s="25">
         <v>41096.15</v>
       </c>
-      <c r="AO7" s="25"/>
+      <c r="AO7" s="25">
+        <v>40842.559999999998</v>
+      </c>
       <c r="AP7" s="25"/>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
@@ -7648,7 +7920,9 @@
       <c r="J8" s="3">
         <v>1218</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>1218</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
         <v>84</v>
@@ -7720,7 +7994,9 @@
       <c r="AN8" s="25">
         <v>49580.44</v>
       </c>
-      <c r="AO8" s="25"/>
+      <c r="AO8" s="25">
+        <v>46572.18</v>
+      </c>
       <c r="AP8" s="25"/>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
@@ -7761,7 +8037,9 @@
       <c r="J9" s="3">
         <v>4246.84</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>4246.84</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="5">
         <v>7619.8989577796901</v>
@@ -7829,7 +8107,9 @@
       <c r="AN9" s="25">
         <v>64612.26</v>
       </c>
-      <c r="AO9" s="25"/>
+      <c r="AO9" s="25">
+        <v>63619.98</v>
+      </c>
       <c r="AP9" s="25"/>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
@@ -7870,7 +8150,9 @@
       <c r="J10" s="25">
         <v>55846.91</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="25">
+        <v>54985.65</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18">
@@ -7936,7 +8218,9 @@
       <c r="AN10" s="25">
         <v>36678.97</v>
       </c>
-      <c r="AO10" s="25"/>
+      <c r="AO10" s="25">
+        <v>35636.33</v>
+      </c>
       <c r="AP10" s="25"/>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
@@ -7973,7 +8257,9 @@
       <c r="J11" s="25">
         <v>13127</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="25">
+        <v>13072</v>
+      </c>
       <c r="L11" s="25"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
@@ -8008,7 +8294,9 @@
       <c r="Y11" s="25">
         <v>8459</v>
       </c>
-      <c r="Z11" s="25"/>
+      <c r="Z11" s="25">
+        <v>8459</v>
+      </c>
       <c r="AA11" s="25"/>
       <c r="AB11" s="18"/>
       <c r="AC11" s="17">
@@ -8047,7 +8335,9 @@
       <c r="AN11" s="25">
         <v>37664.620000000003</v>
       </c>
-      <c r="AO11" s="25"/>
+      <c r="AO11" s="25">
+        <v>36725.06</v>
+      </c>
       <c r="AP11" s="25"/>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
@@ -8084,7 +8374,9 @@
       <c r="J12" s="25">
         <v>9360</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="25">
+        <v>26510</v>
+      </c>
       <c r="L12" s="25"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
@@ -8119,7 +8411,9 @@
       <c r="Y12" s="25">
         <v>17585.830000000002</v>
       </c>
-      <c r="Z12" s="25"/>
+      <c r="Z12" s="25">
+        <v>15968.78</v>
+      </c>
       <c r="AA12" s="25"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="17">
@@ -8158,7 +8452,9 @@
       <c r="AN12" s="25">
         <v>65334.95</v>
       </c>
-      <c r="AO12" s="25"/>
+      <c r="AO12" s="25">
+        <v>64446.87</v>
+      </c>
       <c r="AP12" s="25"/>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
@@ -8193,7 +8489,9 @@
       <c r="J13" s="3">
         <v>1943.98</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>1943.98</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
         <v>1690.16</v>
@@ -8234,7 +8532,9 @@
       <c r="Y13" s="25">
         <v>22681.11</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="25">
+        <v>21220.720000000001</v>
+      </c>
       <c r="AA13" s="25"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="17">
@@ -8273,7 +8573,9 @@
       <c r="AN13" s="25">
         <v>205376.77</v>
       </c>
-      <c r="AO13" s="25"/>
+      <c r="AO13" s="25">
+        <v>201207.83</v>
+      </c>
       <c r="AP13" s="25"/>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
@@ -8310,7 +8612,9 @@
       <c r="J14" s="25">
         <v>4152.75</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="25">
+        <v>4150.8</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18">
@@ -8349,7 +8653,9 @@
       <c r="Y14" s="25">
         <v>20952.57</v>
       </c>
-      <c r="Z14" s="25"/>
+      <c r="Z14" s="25">
+        <v>21135.27</v>
+      </c>
       <c r="AA14" s="25"/>
       <c r="AB14" s="18"/>
       <c r="AC14" s="17">
@@ -8388,7 +8694,9 @@
       <c r="AN14" s="27">
         <v>900.63</v>
       </c>
-      <c r="AO14" s="25"/>
+      <c r="AO14" s="25">
+        <v>894.74</v>
+      </c>
       <c r="AP14" s="25"/>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
@@ -8429,7 +8737,9 @@
       <c r="J15" s="25">
         <v>4898.32</v>
       </c>
-      <c r="K15" s="25"/>
+      <c r="K15" s="25">
+        <v>4802.63</v>
+      </c>
       <c r="L15" s="25"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18">
@@ -8468,7 +8778,9 @@
       <c r="Y15" s="25">
         <v>17195.84</v>
       </c>
-      <c r="Z15" s="25"/>
+      <c r="Z15" s="25">
+        <v>17065.96</v>
+      </c>
       <c r="AA15" s="25"/>
       <c r="AB15" s="18"/>
       <c r="AC15" s="17">
@@ -8507,7 +8819,9 @@
       <c r="AN15" s="25">
         <v>1695.61</v>
       </c>
-      <c r="AO15" s="25"/>
+      <c r="AO15" s="25">
+        <v>1694.18</v>
+      </c>
       <c r="AP15" s="25"/>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
@@ -8548,7 +8862,9 @@
       <c r="J16" s="3">
         <v>486</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>438</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3">
@@ -8587,7 +8903,9 @@
       <c r="Y16" s="25">
         <v>17422.93</v>
       </c>
-      <c r="Z16" s="25"/>
+      <c r="Z16" s="25">
+        <v>17327.34</v>
+      </c>
       <c r="AA16" s="25"/>
       <c r="AB16" s="18"/>
       <c r="AC16" s="17">
@@ -8626,7 +8944,9 @@
       <c r="AN16" s="25">
         <v>5770.28</v>
       </c>
-      <c r="AO16" s="25"/>
+      <c r="AO16" s="25">
+        <v>5518.62</v>
+      </c>
       <c r="AP16" s="25"/>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
@@ -8663,7 +8983,9 @@
       <c r="J17" s="3">
         <v>291.58999999999997</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3">
+        <v>291.58999999999997</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3">
         <v>414.92</v>
@@ -8704,7 +9026,9 @@
       <c r="Y17" s="25">
         <v>24207.55</v>
       </c>
-      <c r="Z17" s="25"/>
+      <c r="Z17" s="25">
+        <v>23373.11</v>
+      </c>
       <c r="AA17" s="25"/>
       <c r="AB17" s="18"/>
       <c r="AC17" s="17">
@@ -8743,7 +9067,9 @@
       <c r="AN17" s="25">
         <v>7263.55</v>
       </c>
-      <c r="AO17" s="25"/>
+      <c r="AO17" s="25">
+        <v>6992.53</v>
+      </c>
       <c r="AP17" s="25"/>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
@@ -8780,7 +9106,9 @@
       <c r="J18" s="25">
         <v>353.56</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="25">
+        <v>353.56</v>
+      </c>
       <c r="L18" s="25"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18">
@@ -8819,7 +9147,9 @@
       <c r="Y18" s="25">
         <v>14510</v>
       </c>
-      <c r="Z18" s="25"/>
+      <c r="Z18" s="25">
+        <v>14305.64</v>
+      </c>
       <c r="AA18" s="25"/>
       <c r="AB18" s="18"/>
       <c r="AC18" s="17">
@@ -8858,7 +9188,9 @@
       <c r="AN18" s="25">
         <v>15988</v>
       </c>
-      <c r="AO18" s="25"/>
+      <c r="AO18" s="25">
+        <v>15995</v>
+      </c>
       <c r="AP18" s="25"/>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
@@ -8895,7 +9227,9 @@
       <c r="J19" s="25">
         <v>479.74</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="25">
+        <v>461.5</v>
+      </c>
       <c r="L19" s="25"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18">
@@ -8934,7 +9268,9 @@
       <c r="Y19" s="25">
         <v>16131.15</v>
       </c>
-      <c r="Z19" s="25"/>
+      <c r="Z19" s="25">
+        <v>15374.89</v>
+      </c>
       <c r="AA19" s="25"/>
       <c r="AB19" s="18"/>
       <c r="AC19" s="17">
@@ -8973,7 +9309,9 @@
       <c r="AN19" s="25">
         <v>36577</v>
       </c>
-      <c r="AO19" s="25"/>
+      <c r="AO19" s="25">
+        <v>36505</v>
+      </c>
       <c r="AP19" s="25"/>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
@@ -9009,7 +9347,9 @@
       <c r="J20" s="3">
         <v>684</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3">
+        <v>672</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3">
         <v>492</v>
@@ -9050,7 +9390,9 @@
       <c r="Y20" s="25">
         <v>16256.53</v>
       </c>
-      <c r="Z20" s="25"/>
+      <c r="Z20" s="25">
+        <v>15982.98</v>
+      </c>
       <c r="AA20" s="25"/>
       <c r="AB20" s="18"/>
       <c r="AC20" s="17">
@@ -9089,7 +9431,9 @@
       <c r="AN20" s="25">
         <v>70571</v>
       </c>
-      <c r="AO20" s="25"/>
+      <c r="AO20" s="25">
+        <v>70401</v>
+      </c>
       <c r="AP20" s="25"/>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
@@ -9126,7 +9470,9 @@
       <c r="J21" s="25">
         <v>1733.52</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="25">
+        <v>1721.15</v>
+      </c>
       <c r="L21" s="25"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18">
@@ -9165,7 +9511,9 @@
       <c r="Y21" s="25">
         <v>8932.8700000000008</v>
       </c>
-      <c r="Z21" s="25"/>
+      <c r="Z21" s="25">
+        <v>8758.16</v>
+      </c>
       <c r="AA21" s="25"/>
       <c r="AB21" s="18"/>
       <c r="AC21" s="17">
@@ -9204,7 +9552,9 @@
       <c r="AN21" s="25">
         <v>514.70000000000005</v>
       </c>
-      <c r="AO21" s="25"/>
+      <c r="AO21" s="25">
+        <v>516.14</v>
+      </c>
       <c r="AP21" s="25"/>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
@@ -9244,7 +9594,9 @@
       <c r="J22" s="3">
         <v>640</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3">
+        <v>640</v>
+      </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3">
         <v>810</v>
@@ -9285,7 +9637,9 @@
       <c r="Y22" s="25">
         <v>32712.82</v>
       </c>
-      <c r="Z22" s="25"/>
+      <c r="Z22" s="25">
+        <v>31655.11</v>
+      </c>
       <c r="AA22" s="25"/>
       <c r="AB22" s="18"/>
       <c r="AC22" s="17">
@@ -9324,7 +9678,9 @@
       <c r="AN22" s="25">
         <v>732</v>
       </c>
-      <c r="AO22" s="25"/>
+      <c r="AO22" s="25">
+        <v>720</v>
+      </c>
       <c r="AP22" s="25"/>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
@@ -9364,7 +9720,9 @@
       <c r="J23" s="3">
         <v>1703</v>
       </c>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>1697</v>
+      </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3">
         <v>1377</v>
@@ -9405,7 +9763,9 @@
       <c r="Y23" s="25">
         <v>46167.02</v>
       </c>
-      <c r="Z23" s="25"/>
+      <c r="Z23" s="25">
+        <v>45404.9</v>
+      </c>
       <c r="AA23" s="25"/>
       <c r="AB23" s="18"/>
       <c r="AC23" s="17"/>
@@ -9440,7 +9800,9 @@
       <c r="AN23" s="25">
         <v>89500</v>
       </c>
-      <c r="AO23" s="25"/>
+      <c r="AO23" s="25">
+        <v>88061.21</v>
+      </c>
       <c r="AP23" s="25"/>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
@@ -9476,7 +9838,9 @@
       <c r="J24" s="3">
         <v>794</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>794</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3">
         <v>764</v>
@@ -9517,7 +9881,9 @@
       <c r="Y24" s="25">
         <v>2300</v>
       </c>
-      <c r="Z24" s="25"/>
+      <c r="Z24" s="25">
+        <v>2246</v>
+      </c>
       <c r="AA24" s="25"/>
       <c r="AB24" s="18"/>
       <c r="AC24" s="17"/>
@@ -9552,7 +9918,9 @@
       <c r="AN24" s="25">
         <v>2794.99</v>
       </c>
-      <c r="AO24" s="25"/>
+      <c r="AO24" s="25">
+        <v>2751.96</v>
+      </c>
       <c r="AP24" s="25"/>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
@@ -9602,7 +9970,9 @@
       <c r="AN25" s="3">
         <v>2741.1</v>
       </c>
-      <c r="AO25" s="3"/>
+      <c r="AO25" s="3">
+        <v>2741.1</v>
+      </c>
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3">
         <v>2980.94</v>
@@ -9665,7 +10035,9 @@
       <c r="AN26" s="3">
         <v>3049.85</v>
       </c>
-      <c r="AO26" s="3"/>
+      <c r="AO26" s="3">
+        <v>3049.85</v>
+      </c>
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3">
         <v>2806.25</v>

</xml_diff>

<commit_message>
Tabela atualizada com os valores da busca local 2OPT
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -566,11 +566,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,7 +876,7 @@
   <dimension ref="B1:AS38"/>
   <sheetViews>
     <sheetView topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO26" sqref="AO26"/>
+      <selection activeCell="AP26" sqref="AP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +893,9 @@
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" customWidth="1"/>
     <col min="25" max="27" width="12.28515625" customWidth="1"/>
     <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -904,7 +906,9 @@
     <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.5703125" customWidth="1"/>
+    <col min="38" max="38" width="8.42578125" customWidth="1"/>
+    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="42" width="12.28515625" customWidth="1"/>
     <col min="44" max="44" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1128,7 +1132,9 @@
       <c r="K3" s="25">
         <v>625.97</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="25">
+        <v>625.97</v>
+      </c>
       <c r="M3" s="18"/>
       <c r="N3" s="18">
         <v>670</v>
@@ -1169,7 +1175,9 @@
       <c r="Z3" s="25">
         <v>668</v>
       </c>
-      <c r="AA3" s="25"/>
+      <c r="AA3" s="25">
+        <v>668</v>
+      </c>
       <c r="AB3" s="18"/>
       <c r="AC3" s="17">
         <v>874</v>
@@ -1210,7 +1218,9 @@
       <c r="AO3" s="25">
         <v>25126.84</v>
       </c>
-      <c r="AP3" s="25"/>
+      <c r="AP3" s="25">
+        <v>25126.84</v>
+      </c>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
         <v>23450</v>
@@ -1234,11 +1244,11 @@
         <v>1</v>
       </c>
       <c r="H4" s="18">
-        <f t="shared" ref="H4:I4" si="0" xml:space="preserve"> AVERAGE(1)</f>
+        <f xml:space="preserve"> AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="I4" s="18">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="J4" s="25"/>
@@ -1280,7 +1290,9 @@
       <c r="Z4" s="25">
         <v>10068.39</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="25">
+        <v>10660.31</v>
+      </c>
       <c r="AB4" s="18"/>
       <c r="AC4" s="17">
         <v>10460</v>
@@ -1321,7 +1333,9 @@
       <c r="AO4" s="25">
         <v>7564.94</v>
       </c>
-      <c r="AP4" s="25"/>
+      <c r="AP4" s="25">
+        <v>7359.17</v>
+      </c>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
         <v>8443</v>
@@ -1364,7 +1378,9 @@
       <c r="K5" s="3">
         <v>1373</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3">
+        <v>1373</v>
+      </c>
       <c r="M5" s="3">
         <v>1239</v>
       </c>
@@ -1403,7 +1419,9 @@
       <c r="Z5" s="25">
         <v>1376</v>
       </c>
-      <c r="AA5" s="25"/>
+      <c r="AA5" s="25">
+        <v>1376</v>
+      </c>
       <c r="AB5" s="18"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="17"/>
@@ -1440,7 +1458,9 @@
       <c r="AO5" s="25">
         <v>10765.78</v>
       </c>
-      <c r="AP5" s="25"/>
+      <c r="AP5" s="25">
+        <v>10765.78</v>
+      </c>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
         <v>14640</v>
@@ -1483,7 +1503,9 @@
       <c r="K6" s="25">
         <v>5553</v>
       </c>
-      <c r="L6" s="25"/>
+      <c r="L6" s="25">
+        <v>5550</v>
+      </c>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="17"/>
@@ -1497,15 +1519,15 @@
       <c r="T6" s="18"/>
       <c r="U6" s="20"/>
       <c r="V6" s="18">
-        <f t="shared" ref="V6:V10" si="1">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W6" s="18">
-        <f t="shared" ref="W6:X10" si="2">AVERAGE(1)</f>
+        <f t="shared" ref="W6:X10" si="0">AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="X6" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y6" s="25"/>
@@ -1551,7 +1573,9 @@
       <c r="AO6" s="25">
         <v>22109.3</v>
       </c>
-      <c r="AP6" s="25"/>
+      <c r="AP6" s="25">
+        <v>21887.32</v>
+      </c>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
         <v>21116</v>
@@ -1593,7 +1617,9 @@
       <c r="K7" s="3">
         <v>292</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3">
+        <v>292</v>
+      </c>
       <c r="M7" s="3">
         <v>246</v>
       </c>
@@ -1613,15 +1639,15 @@
       <c r="T7" s="18"/>
       <c r="U7" s="20"/>
       <c r="V7" s="18">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W7" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X7" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y7" s="25"/>
@@ -1667,7 +1693,9 @@
       <c r="AO7" s="25">
         <v>10742.86</v>
       </c>
-      <c r="AP7" s="25"/>
+      <c r="AP7" s="25">
+        <v>10778.43</v>
+      </c>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
         <v>14327</v>
@@ -1709,7 +1737,9 @@
       <c r="K8" s="3">
         <v>352</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3">
+        <v>352</v>
+      </c>
       <c r="M8" s="4">
         <v>282</v>
       </c>
@@ -1729,15 +1759,15 @@
       <c r="T8" s="18"/>
       <c r="U8" s="20"/>
       <c r="V8" s="18">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W8" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X8" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y8" s="25"/>
@@ -1783,7 +1813,9 @@
       <c r="AO8" s="25">
         <v>15403.26</v>
       </c>
-      <c r="AP8" s="25"/>
+      <c r="AP8" s="25">
+        <v>15403.26</v>
+      </c>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
         <v>23195</v>
@@ -1826,7 +1858,9 @@
       <c r="K9" s="3">
         <v>556.80999999999995</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <v>556.80999999999995</v>
+      </c>
       <c r="M9" s="5">
         <v>480.48033445701299</v>
       </c>
@@ -1846,15 +1880,15 @@
       <c r="T9" s="18"/>
       <c r="U9" s="20"/>
       <c r="V9" s="18">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W9" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X9" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y9" s="25"/>
@@ -1896,7 +1930,9 @@
       <c r="AO9" s="25">
         <v>22375.1</v>
       </c>
-      <c r="AP9" s="25"/>
+      <c r="AP9" s="25">
+        <v>21631.43</v>
+      </c>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
         <v>20033</v>
@@ -1939,7 +1975,9 @@
       <c r="K10" s="25">
         <v>14272.3</v>
       </c>
-      <c r="L10" s="25"/>
+      <c r="L10" s="25">
+        <v>14272.3</v>
+      </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18">
         <v>10619</v>
@@ -1957,15 +1995,15 @@
       <c r="T10" s="18"/>
       <c r="U10" s="20"/>
       <c r="V10" s="18">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W10" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X10" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y10" s="25"/>
@@ -2007,7 +2045,9 @@
       <c r="AO10" s="25">
         <v>8023.61</v>
       </c>
-      <c r="AP10" s="25"/>
+      <c r="AP10" s="25">
+        <v>8023.61</v>
+      </c>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
       <c r="AS10" s="17"/>
@@ -2046,7 +2086,9 @@
       <c r="K11" s="25">
         <v>6116</v>
       </c>
-      <c r="L11" s="25"/>
+      <c r="L11" s="25">
+        <v>6116</v>
+      </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="17"/>
@@ -2083,7 +2125,9 @@
       <c r="Z11" s="25">
         <v>3454</v>
       </c>
-      <c r="AA11" s="25"/>
+      <c r="AA11" s="25">
+        <v>3454</v>
+      </c>
       <c r="AB11" s="18"/>
       <c r="AC11" s="17">
         <v>2827</v>
@@ -2124,7 +2168,9 @@
       <c r="AO11" s="25">
         <v>12311.53</v>
       </c>
-      <c r="AP11" s="25"/>
+      <c r="AP11" s="25">
+        <v>11960.02</v>
+      </c>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
       <c r="AS11" s="17"/>
@@ -2163,7 +2209,9 @@
       <c r="K12" s="25">
         <v>11050</v>
       </c>
-      <c r="L12" s="25"/>
+      <c r="L12" s="25">
+        <v>11010</v>
+      </c>
       <c r="M12" s="12"/>
       <c r="N12" s="18"/>
       <c r="O12" s="17"/>
@@ -2200,7 +2248,9 @@
       <c r="Z12" s="25">
         <v>5015.0200000000004</v>
       </c>
-      <c r="AA12" s="25"/>
+      <c r="AA12" s="25">
+        <v>5015.0200000000004</v>
+      </c>
       <c r="AB12" s="18"/>
       <c r="AC12" s="17">
         <v>4970</v>
@@ -2241,7 +2291,9 @@
       <c r="AO12" s="25">
         <v>22074.32</v>
       </c>
-      <c r="AP12" s="25"/>
+      <c r="AP12" s="25">
+        <v>21798.44</v>
+      </c>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
       <c r="AS12" s="17"/>
@@ -2278,7 +2330,9 @@
       <c r="K13" s="3">
         <v>249.88</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3">
+        <v>249.88</v>
+      </c>
       <c r="M13" s="3">
         <v>224.88</v>
       </c>
@@ -2321,7 +2375,9 @@
       <c r="Z13" s="25">
         <v>6632.55</v>
       </c>
-      <c r="AA13" s="25"/>
+      <c r="AA13" s="25">
+        <v>6632.55</v>
+      </c>
       <c r="AB13" s="18"/>
       <c r="AC13" s="17">
         <v>5690</v>
@@ -2362,7 +2418,9 @@
       <c r="AO13" s="25">
         <v>66266.210000000006</v>
       </c>
-      <c r="AP13" s="25"/>
+      <c r="AP13" s="25">
+        <v>66267.63</v>
+      </c>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
@@ -2401,7 +2459,9 @@
       <c r="K14" s="25">
         <v>1205.2</v>
       </c>
-      <c r="L14" s="25"/>
+      <c r="L14" s="25">
+        <v>1207.1500000000001</v>
+      </c>
       <c r="M14" s="18"/>
       <c r="N14" s="18">
         <v>1130</v>
@@ -2442,7 +2502,9 @@
       <c r="Z14" s="25">
         <v>6767.07</v>
       </c>
-      <c r="AA14" s="25"/>
+      <c r="AA14" s="25">
+        <v>6767.07</v>
+      </c>
       <c r="AB14" s="18"/>
       <c r="AC14" s="17">
         <v>6202</v>
@@ -2483,7 +2545,9 @@
       <c r="AO14" s="25">
         <v>263.3</v>
       </c>
-      <c r="AP14" s="25"/>
+      <c r="AP14" s="25">
+        <v>266.87</v>
+      </c>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
         <v>284</v>
@@ -2526,7 +2590,9 @@
       <c r="K15" s="25">
         <v>1304.57</v>
       </c>
-      <c r="L15" s="25"/>
+      <c r="L15" s="25">
+        <v>1304.57</v>
+      </c>
       <c r="M15" s="18"/>
       <c r="N15" s="18">
         <v>1276</v>
@@ -2567,7 +2633,9 @@
       <c r="Z15" s="25">
         <v>5507.89</v>
       </c>
-      <c r="AA15" s="25"/>
+      <c r="AA15" s="25">
+        <v>5507.89</v>
+      </c>
       <c r="AB15" s="18"/>
       <c r="AC15" s="17">
         <v>4305</v>
@@ -2608,7 +2676,9 @@
       <c r="AO15" s="25">
         <v>558.64</v>
       </c>
-      <c r="AP15" s="25"/>
+      <c r="AP15" s="25">
+        <v>553.95000000000005</v>
+      </c>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
         <v>557</v>
@@ -2651,7 +2721,9 @@
       <c r="K16" s="3">
         <v>100</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <v>100</v>
+      </c>
       <c r="M16" s="3">
         <v>99</v>
       </c>
@@ -2694,7 +2766,9 @@
       <c r="Z16" s="25">
         <v>5119.54</v>
       </c>
-      <c r="AA16" s="25"/>
+      <c r="AA16" s="25">
+        <v>5119.54</v>
+      </c>
       <c r="AB16" s="18"/>
       <c r="AC16" s="17">
         <v>5812</v>
@@ -2735,7 +2809,9 @@
       <c r="AO16" s="25">
         <v>1724.97</v>
       </c>
-      <c r="AP16" s="25"/>
+      <c r="AP16" s="25">
+        <v>1670.87</v>
+      </c>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
       <c r="AS16" s="17"/>
@@ -2774,7 +2850,9 @@
       <c r="K17" s="3">
         <v>77.040000000000006</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3">
+        <v>77.040000000000006</v>
+      </c>
       <c r="M17" s="3">
         <v>76.72</v>
       </c>
@@ -2817,7 +2895,9 @@
       <c r="Z17" s="25">
         <v>6789.91</v>
       </c>
-      <c r="AA17" s="25"/>
+      <c r="AA17" s="25">
+        <v>6789.91</v>
+      </c>
       <c r="AB17" s="18"/>
       <c r="AC17" s="17">
         <v>6368</v>
@@ -2858,7 +2938,9 @@
       <c r="AO17" s="25">
         <v>2280.65</v>
       </c>
-      <c r="AP17" s="25"/>
+      <c r="AP17" s="25">
+        <v>2236.9899999999998</v>
+      </c>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
       <c r="AS17" s="17"/>
@@ -2897,7 +2979,9 @@
       <c r="K18" s="25">
         <v>97.38</v>
       </c>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25">
+        <v>97.38</v>
+      </c>
       <c r="M18" s="18"/>
       <c r="N18" s="18">
         <v>102</v>
@@ -2938,7 +3022,9 @@
       <c r="Z18" s="25">
         <v>4293.0200000000004</v>
       </c>
-      <c r="AA18" s="25"/>
+      <c r="AA18" s="25">
+        <v>4293.0200000000004</v>
+      </c>
       <c r="AB18" s="18"/>
       <c r="AC18" s="17">
         <v>4964</v>
@@ -2979,7 +3065,9 @@
       <c r="AO18" s="25">
         <v>5238</v>
       </c>
-      <c r="AP18" s="25"/>
+      <c r="AP18" s="25">
+        <v>5225</v>
+      </c>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
       <c r="AS18" s="17"/>
@@ -3018,7 +3106,9 @@
       <c r="K19" s="25">
         <v>150.4</v>
       </c>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25">
+        <v>150.4</v>
+      </c>
       <c r="M19" s="18"/>
       <c r="N19" s="18">
         <v>107</v>
@@ -3059,7 +3149,9 @@
       <c r="Z19" s="25">
         <v>5246.28</v>
       </c>
-      <c r="AA19" s="25"/>
+      <c r="AA19" s="25">
+        <v>5246.28</v>
+      </c>
       <c r="AB19" s="18"/>
       <c r="AC19" s="17">
         <v>4762</v>
@@ -3100,7 +3192,9 @@
       <c r="AO19" s="25">
         <v>12252</v>
       </c>
-      <c r="AP19" s="25"/>
+      <c r="AP19" s="25">
+        <v>12083</v>
+      </c>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
       <c r="AS19" s="17"/>
@@ -3138,7 +3232,9 @@
       <c r="K20" s="3">
         <v>147</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>147</v>
+      </c>
       <c r="M20" s="3">
         <v>145</v>
       </c>
@@ -3181,7 +3277,9 @@
       <c r="Z20" s="25">
         <v>4087.21</v>
       </c>
-      <c r="AA20" s="25"/>
+      <c r="AA20" s="25">
+        <v>4087.21</v>
+      </c>
       <c r="AB20" s="18"/>
       <c r="AC20" s="17">
         <v>3905</v>
@@ -3222,7 +3320,9 @@
       <c r="AO20" s="25">
         <v>22289</v>
       </c>
-      <c r="AP20" s="25"/>
+      <c r="AP20" s="25">
+        <v>22289</v>
+      </c>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
       <c r="AS20" s="17"/>
@@ -3261,7 +3361,9 @@
       <c r="K21" s="25">
         <v>559.01</v>
       </c>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25">
+        <v>559.01</v>
+      </c>
       <c r="M21" s="18"/>
       <c r="N21" s="18">
         <v>540</v>
@@ -3302,7 +3404,9 @@
       <c r="Z21" s="25">
         <v>2109.4299999999998</v>
       </c>
-      <c r="AA21" s="25"/>
+      <c r="AA21" s="25">
+        <v>2109.4299999999998</v>
+      </c>
       <c r="AB21" s="18"/>
       <c r="AC21" s="17">
         <v>2606</v>
@@ -3343,7 +3447,9 @@
       <c r="AO21" s="25">
         <v>129.15</v>
       </c>
-      <c r="AP21" s="25"/>
+      <c r="AP21" s="25">
+        <v>129.15</v>
+      </c>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
         <v>120</v>
@@ -3385,7 +3491,9 @@
       <c r="K22" s="3">
         <v>165</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>154</v>
+      </c>
       <c r="M22" s="3">
         <v>143</v>
       </c>
@@ -3428,7 +3536,9 @@
       <c r="Z22" s="25">
         <v>8860.4699999999993</v>
       </c>
-      <c r="AA22" s="25"/>
+      <c r="AA22" s="25">
+        <v>8865.39</v>
+      </c>
       <c r="AB22" s="18"/>
       <c r="AC22" s="17">
         <v>8901</v>
@@ -3469,7 +3579,9 @@
       <c r="AO22" s="25">
         <v>146</v>
       </c>
-      <c r="AP22" s="25"/>
+      <c r="AP22" s="25">
+        <v>146</v>
+      </c>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
         <v>192</v>
@@ -3511,7 +3623,9 @@
       <c r="K23" s="3">
         <v>258</v>
       </c>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3">
+        <v>258</v>
+      </c>
       <c r="M23" s="3">
         <v>181</v>
       </c>
@@ -3554,7 +3668,9 @@
       <c r="Z23" s="25">
         <v>13194.03</v>
       </c>
-      <c r="AA23" s="25"/>
+      <c r="AA23" s="25">
+        <v>13100.47</v>
+      </c>
       <c r="AB23" s="18"/>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -3591,7 +3707,9 @@
       <c r="AO23" s="25">
         <v>27500</v>
       </c>
-      <c r="AP23" s="25"/>
+      <c r="AP23" s="25">
+        <v>27500</v>
+      </c>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
       <c r="AS23" s="17"/>
@@ -3629,7 +3747,9 @@
       <c r="K24" s="3">
         <v>162</v>
       </c>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3">
+        <v>162</v>
+      </c>
       <c r="M24" s="3">
         <v>162</v>
       </c>
@@ -3673,7 +3793,9 @@
       <c r="Z24" s="25">
         <v>720</v>
       </c>
-      <c r="AA24" s="25"/>
+      <c r="AA24" s="25">
+        <v>718</v>
+      </c>
       <c r="AB24" s="18"/>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -3710,7 +3832,9 @@
       <c r="AO24" s="25">
         <v>964.26</v>
       </c>
-      <c r="AP24" s="25"/>
+      <c r="AP24" s="25">
+        <v>996.51</v>
+      </c>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
       <c r="AS24" s="17"/>
@@ -3751,7 +3875,9 @@
       <c r="AO25" s="3">
         <v>826.08</v>
       </c>
-      <c r="AP25" s="3"/>
+      <c r="AP25" s="3">
+        <v>826.08</v>
+      </c>
       <c r="AQ25" s="3">
         <v>714.33</v>
       </c>
@@ -3820,7 +3946,9 @@
       <c r="AO26" s="3">
         <v>456.58</v>
       </c>
-      <c r="AP26" s="3"/>
+      <c r="AP26" s="3">
+        <v>456.58</v>
+      </c>
       <c r="AQ26" s="3">
         <v>662.17</v>
       </c>
@@ -3986,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AS38"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG37" sqref="AG37"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP26" sqref="AP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,7 +4136,7 @@
     <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.42578125" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" customWidth="1"/>
     <col min="25" max="27" width="12.28515625" customWidth="1"/>
     <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -4017,8 +4145,9 @@
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="35" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.28515625" customWidth="1"/>
-    <col min="37" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" customWidth="1"/>
+    <col min="37" max="38" width="7.7109375" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" customWidth="1"/>
     <col min="40" max="42" width="12.28515625" customWidth="1"/>
     <col min="43" max="43" width="8" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -4243,7 +4372,9 @@
       <c r="K3" s="25">
         <v>1318.03</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="25">
+        <v>1309.68</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="18">
         <v>1314</v>
@@ -4284,7 +4415,9 @@
       <c r="Z3" s="25">
         <v>2122</v>
       </c>
-      <c r="AA3" s="25"/>
+      <c r="AA3" s="25">
+        <v>2011</v>
+      </c>
       <c r="AB3" s="18"/>
       <c r="AC3" s="18">
         <v>1819</v>
@@ -4325,7 +4458,9 @@
       <c r="AO3" s="25">
         <v>42676.77</v>
       </c>
-      <c r="AP3" s="25"/>
+      <c r="AP3" s="25">
+        <v>42676.77</v>
+      </c>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
         <v>41248</v>
@@ -4345,15 +4480,15 @@
       <c r="E4" s="1"/>
       <c r="F4" s="20"/>
       <c r="G4" s="13">
-        <f t="shared" ref="G4" si="0">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="H4" s="13">
-        <f t="shared" ref="H4:I4" si="1">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="I4" s="13">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="J4" s="25"/>
@@ -4395,7 +4530,9 @@
       <c r="Z4" s="25">
         <v>21055.45</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="25">
+        <v>21657.37</v>
+      </c>
       <c r="AB4" s="18"/>
       <c r="AC4" s="18">
         <v>20688</v>
@@ -4436,7 +4573,9 @@
       <c r="AO4" s="25">
         <v>15960.98</v>
       </c>
-      <c r="AP4" s="25"/>
+      <c r="AP4" s="25">
+        <v>15262.35</v>
+      </c>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
         <v>18028</v>
@@ -4479,7 +4618,9 @@
       <c r="K5" s="3">
         <v>3231</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3">
+        <v>3231</v>
+      </c>
       <c r="M5" s="3" t="s">
         <v>76</v>
       </c>
@@ -4518,7 +4659,9 @@
       <c r="Z5" s="25">
         <v>3120</v>
       </c>
-      <c r="AA5" s="25"/>
+      <c r="AA5" s="25">
+        <v>3120</v>
+      </c>
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
       <c r="AD5" s="17"/>
@@ -4555,7 +4698,9 @@
       <c r="AO5" s="25">
         <v>25633.65</v>
       </c>
-      <c r="AP5" s="25"/>
+      <c r="AP5" s="25">
+        <v>23691.5</v>
+      </c>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
         <v>22998</v>
@@ -4598,7 +4743,9 @@
       <c r="K6" s="25">
         <v>14128</v>
       </c>
-      <c r="L6" s="25"/>
+      <c r="L6" s="25">
+        <v>14036</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="18"/>
       <c r="O6" s="17"/>
@@ -4612,15 +4759,15 @@
       <c r="T6" s="18"/>
       <c r="U6" s="20"/>
       <c r="V6" s="18">
-        <f t="shared" ref="V6:V10" si="2">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W6" s="18">
-        <f t="shared" ref="W6:X10" si="3">AVERAGE(1)</f>
+        <f t="shared" ref="W6:X10" si="0">AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="X6" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y6" s="25"/>
@@ -4666,7 +4813,9 @@
       <c r="AO6" s="25">
         <v>46726.91</v>
       </c>
-      <c r="AP6" s="25"/>
+      <c r="AP6" s="25">
+        <v>50028.99</v>
+      </c>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
         <v>46890</v>
@@ -4708,7 +4857,9 @@
       <c r="K7" s="3">
         <v>581</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3">
+        <v>581</v>
+      </c>
       <c r="M7" s="3" t="s">
         <v>81</v>
       </c>
@@ -4728,15 +4879,15 @@
       <c r="T7" s="18"/>
       <c r="U7" s="20"/>
       <c r="V7" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y7" s="25"/>
@@ -4782,7 +4933,9 @@
       <c r="AO7" s="25">
         <v>26306.34</v>
       </c>
-      <c r="AP7" s="25"/>
+      <c r="AP7" s="25">
+        <v>26331.47</v>
+      </c>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
         <v>28402</v>
@@ -4824,7 +4977,9 @@
       <c r="K8" s="3">
         <v>816</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3">
+        <v>816</v>
+      </c>
       <c r="M8" s="3" t="s">
         <v>83</v>
       </c>
@@ -4844,15 +4999,15 @@
       <c r="T8" s="18"/>
       <c r="U8" s="20"/>
       <c r="V8" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y8" s="25"/>
@@ -4898,7 +5053,9 @@
       <c r="AO8" s="25">
         <v>32745.67</v>
       </c>
-      <c r="AP8" s="25"/>
+      <c r="AP8" s="25">
+        <v>32794.53</v>
+      </c>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
         <v>36637</v>
@@ -4941,7 +5098,9 @@
       <c r="K9" s="3">
         <v>1766.5</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <v>1766.5</v>
+      </c>
       <c r="M9" s="5">
         <v>3303.71452420693</v>
       </c>
@@ -4961,15 +5120,15 @@
       <c r="T9" s="18"/>
       <c r="U9" s="20"/>
       <c r="V9" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y9" s="25"/>
@@ -5011,7 +5170,9 @@
       <c r="AO9" s="25">
         <v>48156.03</v>
       </c>
-      <c r="AP9" s="25"/>
+      <c r="AP9" s="25">
+        <v>47039.29</v>
+      </c>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
         <v>38718</v>
@@ -5054,7 +5215,9 @@
       <c r="K10" s="25">
         <v>28429.05</v>
       </c>
-      <c r="L10" s="25"/>
+      <c r="L10" s="25">
+        <v>27862.639999999999</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="18">
         <v>26062</v>
@@ -5072,15 +5235,15 @@
       <c r="T10" s="18"/>
       <c r="U10" s="20"/>
       <c r="V10" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y10" s="25"/>
@@ -5122,7 +5285,9 @@
       <c r="AO10" s="25">
         <v>21889.15</v>
       </c>
-      <c r="AP10" s="25"/>
+      <c r="AP10" s="25">
+        <v>22363.5</v>
+      </c>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
       <c r="AS10" s="17"/>
@@ -5161,7 +5326,9 @@
       <c r="K11" s="25">
         <v>10262</v>
       </c>
-      <c r="L11" s="25"/>
+      <c r="L11" s="25">
+        <v>10262</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="18"/>
       <c r="O11" s="17"/>
@@ -5198,7 +5365,9 @@
       <c r="Z11" s="25">
         <v>6284</v>
       </c>
-      <c r="AA11" s="25"/>
+      <c r="AA11" s="25">
+        <v>6284</v>
+      </c>
       <c r="AB11" s="18"/>
       <c r="AC11" s="18">
         <v>4701</v>
@@ -5239,7 +5408,9 @@
       <c r="AO11" s="25">
         <v>25630.01</v>
       </c>
-      <c r="AP11" s="25"/>
+      <c r="AP11" s="25">
+        <v>24829.1</v>
+      </c>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
       <c r="AS11" s="17"/>
@@ -5278,7 +5449,9 @@
       <c r="K12" s="25">
         <v>25610</v>
       </c>
-      <c r="L12" s="25"/>
+      <c r="L12" s="25">
+        <v>4770</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="18"/>
       <c r="O12" s="17"/>
@@ -5315,7 +5488,9 @@
       <c r="Z12" s="25">
         <v>10638.41</v>
       </c>
-      <c r="AA12" s="25"/>
+      <c r="AA12" s="25">
+        <v>10809.47</v>
+      </c>
       <c r="AB12" s="18"/>
       <c r="AC12" s="18">
         <v>9184</v>
@@ -5356,7 +5531,9 @@
       <c r="AO12" s="25">
         <v>40496.9</v>
       </c>
-      <c r="AP12" s="25"/>
+      <c r="AP12" s="25">
+        <v>39951.51</v>
+      </c>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
       <c r="AS12" s="17"/>
@@ -5393,7 +5570,9 @@
       <c r="K13" s="3">
         <v>1454.84</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3">
+        <v>1454.84</v>
+      </c>
       <c r="M13" s="3">
         <v>966.37</v>
       </c>
@@ -5436,7 +5615,9 @@
       <c r="Z13" s="25">
         <v>14772.08</v>
       </c>
-      <c r="AA13" s="25"/>
+      <c r="AA13" s="25">
+        <v>14026.18</v>
+      </c>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18">
         <v>11625</v>
@@ -5477,7 +5658,9 @@
       <c r="AO13" s="25">
         <v>129086.31</v>
       </c>
-      <c r="AP13" s="25"/>
+      <c r="AP13" s="25">
+        <v>128728.12</v>
+      </c>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
@@ -5516,7 +5699,9 @@
       <c r="K14" s="25">
         <v>2708.24</v>
       </c>
-      <c r="L14" s="25"/>
+      <c r="L14" s="25">
+        <v>2710.19</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="18">
         <v>2408</v>
@@ -5557,7 +5742,9 @@
       <c r="Z14" s="25">
         <v>13485.45</v>
       </c>
-      <c r="AA14" s="25"/>
+      <c r="AA14" s="25">
+        <v>13485.45</v>
+      </c>
       <c r="AB14" s="18"/>
       <c r="AC14" s="18">
         <v>12753</v>
@@ -5598,7 +5785,9 @@
       <c r="AO14" s="25">
         <v>578.70000000000005</v>
       </c>
-      <c r="AP14" s="25"/>
+      <c r="AP14" s="25">
+        <v>571.6</v>
+      </c>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
         <v>574</v>
@@ -5641,7 +5830,9 @@
       <c r="K15" s="25">
         <v>3082.54</v>
       </c>
-      <c r="L15" s="25"/>
+      <c r="L15" s="25">
+        <v>3087.18</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="18">
         <v>2761</v>
@@ -5682,7 +5873,9 @@
       <c r="Z15" s="25">
         <v>11366.47</v>
       </c>
-      <c r="AA15" s="25"/>
+      <c r="AA15" s="25">
+        <v>11184.6</v>
+      </c>
       <c r="AB15" s="18"/>
       <c r="AC15" s="18">
         <v>9096</v>
@@ -5723,7 +5916,9 @@
       <c r="AO15" s="25">
         <v>1133.95</v>
       </c>
-      <c r="AP15" s="25"/>
+      <c r="AP15" s="25">
+        <v>1125.23</v>
+      </c>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
         <v>1140</v>
@@ -5766,7 +5961,9 @@
       <c r="K16" s="3">
         <v>239</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <v>239</v>
+      </c>
       <c r="M16" s="3">
         <v>230</v>
       </c>
@@ -5809,7 +6006,9 @@
       <c r="Z16" s="25">
         <v>11909.87</v>
       </c>
-      <c r="AA16" s="25"/>
+      <c r="AA16" s="25">
+        <v>12016.93</v>
+      </c>
       <c r="AB16" s="18"/>
       <c r="AC16" s="18">
         <v>11535</v>
@@ -5850,7 +6049,9 @@
       <c r="AO16" s="25">
         <v>3407.23</v>
       </c>
-      <c r="AP16" s="25"/>
+      <c r="AP16" s="25">
+        <v>3354.21</v>
+      </c>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
       <c r="AS16" s="17"/>
@@ -5889,7 +6090,9 @@
       <c r="K17" s="3">
         <v>181.41</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3">
+        <v>181.41</v>
+      </c>
       <c r="M17" s="3" t="s">
         <v>85</v>
       </c>
@@ -5932,7 +6135,9 @@
       <c r="Z17" s="25">
         <v>16276.03</v>
       </c>
-      <c r="AA17" s="25"/>
+      <c r="AA17" s="25">
+        <v>15963.66</v>
+      </c>
       <c r="AB17" s="18"/>
       <c r="AC17" s="18">
         <v>13080</v>
@@ -5973,7 +6178,9 @@
       <c r="AO17" s="25">
         <v>4535.42</v>
       </c>
-      <c r="AP17" s="25"/>
+      <c r="AP17" s="25">
+        <v>4472.01</v>
+      </c>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
       <c r="AS17" s="17"/>
@@ -6012,7 +6219,9 @@
       <c r="K18" s="25">
         <v>229.64</v>
       </c>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25">
+        <v>229.64</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="18">
         <v>216</v>
@@ -6053,7 +6262,9 @@
       <c r="Z18" s="25">
         <v>9555.73</v>
       </c>
-      <c r="AA18" s="25"/>
+      <c r="AA18" s="25">
+        <v>9555.73</v>
+      </c>
       <c r="AB18" s="18"/>
       <c r="AC18" s="18">
         <v>9457</v>
@@ -6094,7 +6305,9 @@
       <c r="AO18" s="25">
         <v>10528</v>
       </c>
-      <c r="AP18" s="25"/>
+      <c r="AP18" s="25">
+        <v>10498</v>
+      </c>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
       <c r="AS18" s="17"/>
@@ -6133,7 +6346,9 @@
       <c r="K19" s="25">
         <v>314.43</v>
       </c>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25">
+        <v>314.43</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="18">
         <v>227</v>
@@ -6174,7 +6389,9 @@
       <c r="Z19" s="25">
         <v>10587.17</v>
       </c>
-      <c r="AA19" s="25"/>
+      <c r="AA19" s="25">
+        <v>10205.07</v>
+      </c>
       <c r="AB19" s="18"/>
       <c r="AC19" s="18">
         <v>8719</v>
@@ -6215,7 +6432,9 @@
       <c r="AO19" s="25">
         <v>23495</v>
       </c>
-      <c r="AP19" s="25"/>
+      <c r="AP19" s="25">
+        <v>23164</v>
+      </c>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
       <c r="AS19" s="17"/>
@@ -6253,7 +6472,9 @@
       <c r="K20" s="3">
         <v>331</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>334</v>
+      </c>
       <c r="M20" s="3">
         <v>308</v>
       </c>
@@ -6296,7 +6517,9 @@
       <c r="Z20" s="25">
         <v>9911.8700000000008</v>
       </c>
-      <c r="AA20" s="25"/>
+      <c r="AA20" s="25">
+        <v>9424.1</v>
+      </c>
       <c r="AB20" s="18"/>
       <c r="AC20" s="18">
         <v>9102</v>
@@ -6337,7 +6560,9 @@
       <c r="AO20" s="25">
         <v>46817</v>
       </c>
-      <c r="AP20" s="25"/>
+      <c r="AP20" s="25">
+        <v>46591</v>
+      </c>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
       <c r="AS20" s="17"/>
@@ -6376,7 +6601,9 @@
       <c r="K21" s="25">
         <v>1176.3699999999999</v>
       </c>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25">
+        <v>1169.1600000000001</v>
+      </c>
       <c r="M21" s="1"/>
       <c r="N21" s="18">
         <v>1042</v>
@@ -6417,7 +6644,9 @@
       <c r="Z21" s="25">
         <v>5673.74</v>
       </c>
-      <c r="AA21" s="25"/>
+      <c r="AA21" s="25">
+        <v>5691.96</v>
+      </c>
       <c r="AB21" s="18"/>
       <c r="AC21" s="18">
         <v>5848</v>
@@ -6458,7 +6687,9 @@
       <c r="AO21" s="25">
         <v>323.07</v>
       </c>
-      <c r="AP21" s="25"/>
+      <c r="AP21" s="25">
+        <v>308.25</v>
+      </c>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
         <v>260</v>
@@ -6500,7 +6731,9 @@
       <c r="K22" s="3">
         <v>359</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>359</v>
+      </c>
       <c r="M22" s="3">
         <v>380</v>
       </c>
@@ -6543,7 +6776,9 @@
       <c r="Z22" s="25">
         <v>21495.02</v>
       </c>
-      <c r="AA22" s="25"/>
+      <c r="AA22" s="25">
+        <v>20813.25</v>
+      </c>
       <c r="AB22" s="18"/>
       <c r="AC22" s="18">
         <v>18600</v>
@@ -6584,7 +6819,9 @@
       <c r="AO22" s="25">
         <v>425</v>
       </c>
-      <c r="AP22" s="25"/>
+      <c r="AP22" s="25">
+        <v>425</v>
+      </c>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
         <v>458</v>
@@ -6626,7 +6863,9 @@
       <c r="K23" s="3">
         <v>989</v>
       </c>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3">
+        <v>989</v>
+      </c>
       <c r="M23" s="3">
         <v>683</v>
       </c>
@@ -6669,7 +6908,9 @@
       <c r="Z23" s="25">
         <v>28189.25</v>
       </c>
-      <c r="AA23" s="25"/>
+      <c r="AA23" s="25">
+        <v>28110.73</v>
+      </c>
       <c r="AB23" s="18"/>
       <c r="AC23" s="18"/>
       <c r="AD23" s="17"/>
@@ -6706,7 +6947,9 @@
       <c r="AO23" s="25">
         <v>55500</v>
       </c>
-      <c r="AP23" s="25"/>
+      <c r="AP23" s="25">
+        <v>55500</v>
+      </c>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
       <c r="AS23" s="17"/>
@@ -6744,7 +6987,9 @@
       <c r="K24" s="3">
         <v>490</v>
       </c>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3">
+        <v>490</v>
+      </c>
       <c r="M24" s="3">
         <v>409</v>
       </c>
@@ -6787,7 +7032,9 @@
       <c r="Z24" s="25">
         <v>1341</v>
       </c>
-      <c r="AA24" s="25"/>
+      <c r="AA24" s="25">
+        <v>1336</v>
+      </c>
       <c r="AB24" s="18"/>
       <c r="AC24" s="18"/>
       <c r="AD24" s="17"/>
@@ -6824,7 +7071,9 @@
       <c r="AO24" s="25">
         <v>1803.89</v>
       </c>
-      <c r="AP24" s="25"/>
+      <c r="AP24" s="25">
+        <v>1836.14</v>
+      </c>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
       <c r="AS24" s="17"/>
@@ -6876,7 +7125,9 @@
       <c r="AO25" s="3">
         <v>1981.71</v>
       </c>
-      <c r="AP25" s="3"/>
+      <c r="AP25" s="3">
+        <v>1981.71</v>
+      </c>
       <c r="AQ25" s="3">
         <v>1505.95</v>
       </c>
@@ -6941,7 +7192,9 @@
       <c r="AO26" s="3">
         <v>2062.92</v>
       </c>
-      <c r="AP26" s="3"/>
+      <c r="AP26" s="3">
+        <v>2062.92</v>
+      </c>
       <c r="AQ26" s="3">
         <v>1647.33</v>
       </c>
@@ -7063,22 +7316,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AH1:AS1"/>
-    <mergeCell ref="S1:AD1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E28"/>
-    <mergeCell ref="B29:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B29:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="AH1:AS1"/>
+    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7089,8 +7342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO19" sqref="AO19"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP17" sqref="AP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7108,7 +7361,9 @@
     <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" customWidth="1"/>
     <col min="25" max="27" width="12.28515625" customWidth="1"/>
     <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -7118,7 +7373,7 @@
     <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="10.7109375" customWidth="1"/>
     <col min="40" max="42" width="12.28515625" customWidth="1"/>
     <col min="44" max="44" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -7342,7 +7597,9 @@
       <c r="K3" s="25">
         <v>2055.2600000000002</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="25">
+        <v>2024.94</v>
+      </c>
       <c r="M3" s="18"/>
       <c r="N3" s="18">
         <v>2066</v>
@@ -7383,7 +7640,9 @@
       <c r="Z3" s="25">
         <v>3340</v>
       </c>
-      <c r="AA3" s="25"/>
+      <c r="AA3" s="25">
+        <v>3164</v>
+      </c>
       <c r="AB3" s="18"/>
       <c r="AC3" s="17">
         <v>3104</v>
@@ -7424,7 +7683,9 @@
       <c r="AO3" s="25">
         <v>63719.25</v>
       </c>
-      <c r="AP3" s="25"/>
+      <c r="AP3" s="25">
+        <v>62471.59</v>
+      </c>
       <c r="AQ3" s="18"/>
       <c r="AR3" s="17">
         <v>64142</v>
@@ -7444,15 +7705,15 @@
       <c r="E4" s="18"/>
       <c r="F4" s="20"/>
       <c r="G4" s="18">
-        <f t="shared" ref="G4" si="0">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="H4" s="18">
-        <f t="shared" ref="H4:I4" si="1">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="I4" s="18">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="J4" s="25"/>
@@ -7494,7 +7755,9 @@
       <c r="Z4" s="25">
         <v>39556.93</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="25">
+        <v>40066.080000000002</v>
+      </c>
       <c r="AB4" s="18"/>
       <c r="AC4" s="17">
         <v>31437</v>
@@ -7535,7 +7798,9 @@
       <c r="AO4" s="25">
         <v>31557.54</v>
       </c>
-      <c r="AP4" s="25"/>
+      <c r="AP4" s="25">
+        <v>30370.62</v>
+      </c>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="17">
         <v>36468</v>
@@ -7578,7 +7843,9 @@
       <c r="K5" s="3">
         <v>6649</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3">
+        <v>6505</v>
+      </c>
       <c r="M5" s="3" t="s">
         <v>77</v>
       </c>
@@ -7617,7 +7884,9 @@
       <c r="Z5" s="25">
         <v>4643</v>
       </c>
-      <c r="AA5" s="25"/>
+      <c r="AA5" s="25">
+        <v>4635</v>
+      </c>
       <c r="AB5" s="18"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="17"/>
@@ -7654,7 +7923,9 @@
       <c r="AO5" s="25">
         <v>39424.629999999997</v>
       </c>
-      <c r="AP5" s="25"/>
+      <c r="AP5" s="25">
+        <v>37725.64</v>
+      </c>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="17">
         <v>39174</v>
@@ -7697,7 +7968,9 @@
       <c r="K6" s="25">
         <v>22317</v>
       </c>
-      <c r="L6" s="25"/>
+      <c r="L6" s="25">
+        <v>21862</v>
+      </c>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="17"/>
@@ -7711,15 +7984,15 @@
       <c r="T6" s="18"/>
       <c r="U6" s="20"/>
       <c r="V6" s="18">
-        <f t="shared" ref="V6:V10" si="2">AVERAGE(1)</f>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W6" s="18">
-        <f t="shared" ref="W6:X10" si="3">AVERAGE(1)</f>
+        <f t="shared" ref="W6:X10" si="0">AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="X6" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y6" s="25"/>
@@ -7765,7 +8038,9 @@
       <c r="AO6" s="25">
         <v>77379.09</v>
       </c>
-      <c r="AP6" s="25"/>
+      <c r="AP6" s="25">
+        <v>76340.25</v>
+      </c>
       <c r="AQ6" s="18"/>
       <c r="AR6" s="17">
         <v>69690</v>
@@ -7807,7 +8082,9 @@
       <c r="K7" s="3">
         <v>1035</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3">
+        <v>1035</v>
+      </c>
       <c r="M7" s="3" t="s">
         <v>82</v>
       </c>
@@ -7827,15 +8104,15 @@
       <c r="T7" s="18"/>
       <c r="U7" s="20"/>
       <c r="V7" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y7" s="25"/>
@@ -7881,7 +8158,9 @@
       <c r="AO7" s="25">
         <v>40842.559999999998</v>
       </c>
-      <c r="AP7" s="25"/>
+      <c r="AP7" s="25">
+        <v>41085.79</v>
+      </c>
       <c r="AQ7" s="18"/>
       <c r="AR7" s="17">
         <v>41452</v>
@@ -7923,7 +8202,9 @@
       <c r="K8" s="3">
         <v>1218</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3">
+        <v>1218</v>
+      </c>
       <c r="M8" s="3" t="s">
         <v>84</v>
       </c>
@@ -7943,15 +8224,15 @@
       <c r="T8" s="18"/>
       <c r="U8" s="20"/>
       <c r="V8" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y8" s="25"/>
@@ -7997,7 +8278,9 @@
       <c r="AO8" s="25">
         <v>46572.18</v>
       </c>
-      <c r="AP8" s="25"/>
+      <c r="AP8" s="25">
+        <v>46589.23</v>
+      </c>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="17">
         <v>57431</v>
@@ -8040,7 +8323,9 @@
       <c r="K9" s="3">
         <v>4246.84</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3">
+        <v>4246.84</v>
+      </c>
       <c r="M9" s="5">
         <v>7619.8989577796901</v>
       </c>
@@ -8060,15 +8345,15 @@
       <c r="T9" s="18"/>
       <c r="U9" s="20"/>
       <c r="V9" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y9" s="25"/>
@@ -8110,7 +8395,9 @@
       <c r="AO9" s="25">
         <v>63619.98</v>
       </c>
-      <c r="AP9" s="25"/>
+      <c r="AP9" s="25">
+        <v>62428.38</v>
+      </c>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="17">
         <v>47516</v>
@@ -8153,7 +8440,9 @@
       <c r="K10" s="25">
         <v>54985.65</v>
       </c>
-      <c r="L10" s="25"/>
+      <c r="L10" s="25">
+        <v>54589.39</v>
+      </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18">
         <v>50324</v>
@@ -8171,15 +8460,15 @@
       <c r="T10" s="18"/>
       <c r="U10" s="20"/>
       <c r="V10" s="18">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
       <c r="W10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y10" s="25"/>
@@ -8221,7 +8510,9 @@
       <c r="AO10" s="25">
         <v>35636.33</v>
       </c>
-      <c r="AP10" s="25"/>
+      <c r="AP10" s="25">
+        <v>36106.68</v>
+      </c>
       <c r="AQ10" s="18"/>
       <c r="AR10" s="17"/>
       <c r="AS10" s="17"/>
@@ -8260,7 +8551,9 @@
       <c r="K11" s="25">
         <v>13072</v>
       </c>
-      <c r="L11" s="25"/>
+      <c r="L11" s="25">
+        <v>13109</v>
+      </c>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="17"/>
@@ -8297,7 +8590,9 @@
       <c r="Z11" s="25">
         <v>8459</v>
       </c>
-      <c r="AA11" s="25"/>
+      <c r="AA11" s="25">
+        <v>8308</v>
+      </c>
       <c r="AB11" s="18"/>
       <c r="AC11" s="17">
         <v>7278</v>
@@ -8338,7 +8633,9 @@
       <c r="AO11" s="25">
         <v>36725.06</v>
       </c>
-      <c r="AP11" s="25"/>
+      <c r="AP11" s="25">
+        <v>36050.949999999997</v>
+      </c>
       <c r="AQ11" s="18"/>
       <c r="AR11" s="17"/>
       <c r="AS11" s="17"/>
@@ -8377,7 +8674,9 @@
       <c r="K12" s="25">
         <v>26510</v>
       </c>
-      <c r="L12" s="25"/>
+      <c r="L12" s="25">
+        <v>1830</v>
+      </c>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="17"/>
@@ -8414,7 +8713,9 @@
       <c r="Z12" s="25">
         <v>15968.78</v>
       </c>
-      <c r="AA12" s="25"/>
+      <c r="AA12" s="25">
+        <v>15544.88</v>
+      </c>
       <c r="AB12" s="18"/>
       <c r="AC12" s="17">
         <v>14492</v>
@@ -8455,7 +8756,9 @@
       <c r="AO12" s="25">
         <v>64446.87</v>
       </c>
-      <c r="AP12" s="25"/>
+      <c r="AP12" s="25">
+        <v>64127.51</v>
+      </c>
       <c r="AQ12" s="18"/>
       <c r="AR12" s="17"/>
       <c r="AS12" s="17"/>
@@ -8492,7 +8795,9 @@
       <c r="K13" s="3">
         <v>1943.98</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3">
+        <v>1943.98</v>
+      </c>
       <c r="M13" s="3">
         <v>1690.16</v>
       </c>
@@ -8535,7 +8840,9 @@
       <c r="Z13" s="25">
         <v>21220.720000000001</v>
       </c>
-      <c r="AA13" s="25"/>
+      <c r="AA13" s="25">
+        <v>20322.55</v>
+      </c>
       <c r="AB13" s="18"/>
       <c r="AC13" s="17">
         <v>18210</v>
@@ -8576,7 +8883,9 @@
       <c r="AO13" s="25">
         <v>201207.83</v>
       </c>
-      <c r="AP13" s="25"/>
+      <c r="AP13" s="25">
+        <v>197692.25</v>
+      </c>
       <c r="AQ13" s="18"/>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
@@ -8615,7 +8924,9 @@
       <c r="K14" s="25">
         <v>4150.8</v>
       </c>
-      <c r="L14" s="25"/>
+      <c r="L14" s="25">
+        <v>4141.5</v>
+      </c>
       <c r="M14" s="18"/>
       <c r="N14" s="18">
         <v>3907</v>
@@ -8656,7 +8967,9 @@
       <c r="Z14" s="25">
         <v>21135.27</v>
       </c>
-      <c r="AA14" s="25"/>
+      <c r="AA14" s="25">
+        <v>20907.740000000002</v>
+      </c>
       <c r="AB14" s="18"/>
       <c r="AC14" s="17">
         <v>20723</v>
@@ -8697,7 +9010,9 @@
       <c r="AO14" s="25">
         <v>894.74</v>
       </c>
-      <c r="AP14" s="25"/>
+      <c r="AP14" s="25">
+        <v>887.64</v>
+      </c>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17">
         <v>861</v>
@@ -8740,7 +9055,9 @@
       <c r="K15" s="25">
         <v>4802.63</v>
       </c>
-      <c r="L15" s="25"/>
+      <c r="L15" s="25">
+        <v>4751.72</v>
+      </c>
       <c r="M15" s="18"/>
       <c r="N15" s="18">
         <v>4499</v>
@@ -8781,7 +9098,9 @@
       <c r="Z15" s="25">
         <v>17065.96</v>
       </c>
-      <c r="AA15" s="25"/>
+      <c r="AA15" s="25">
+        <v>16962.009999999998</v>
+      </c>
       <c r="AB15" s="18"/>
       <c r="AC15" s="17">
         <v>14744</v>
@@ -8822,7 +9141,9 @@
       <c r="AO15" s="25">
         <v>1694.18</v>
       </c>
-      <c r="AP15" s="25"/>
+      <c r="AP15" s="25">
+        <v>1685.46</v>
+      </c>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="17">
         <v>1753</v>
@@ -8865,7 +9186,9 @@
       <c r="K16" s="3">
         <v>438</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <v>441</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3">
         <v>427</v>
@@ -8906,7 +9229,9 @@
       <c r="Z16" s="25">
         <v>17327.34</v>
       </c>
-      <c r="AA16" s="25"/>
+      <c r="AA16" s="25">
+        <v>17311.439999999999</v>
+      </c>
       <c r="AB16" s="18"/>
       <c r="AC16" s="17">
         <v>17501</v>
@@ -8947,7 +9272,9 @@
       <c r="AO16" s="25">
         <v>5518.62</v>
       </c>
-      <c r="AP16" s="25"/>
+      <c r="AP16" s="25">
+        <v>5282.69</v>
+      </c>
       <c r="AQ16" s="18"/>
       <c r="AR16" s="17"/>
       <c r="AS16" s="17"/>
@@ -8986,7 +9313,9 @@
       <c r="K17" s="3">
         <v>291.58999999999997</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3">
+        <v>291.58999999999997</v>
+      </c>
       <c r="M17" s="3">
         <v>414.92</v>
       </c>
@@ -9029,7 +9358,9 @@
       <c r="Z17" s="25">
         <v>23373.11</v>
       </c>
-      <c r="AA17" s="25"/>
+      <c r="AA17" s="25">
+        <v>23060.74</v>
+      </c>
       <c r="AB17" s="18"/>
       <c r="AC17" s="17">
         <v>20508</v>
@@ -9070,7 +9401,9 @@
       <c r="AO17" s="25">
         <v>6992.53</v>
       </c>
-      <c r="AP17" s="25"/>
+      <c r="AP17" s="25">
+        <v>6847.53</v>
+      </c>
       <c r="AQ17" s="18"/>
       <c r="AR17" s="17"/>
       <c r="AS17" s="17"/>
@@ -9109,7 +9442,9 @@
       <c r="K18" s="25">
         <v>353.56</v>
       </c>
-      <c r="L18" s="25"/>
+      <c r="L18" s="25">
+        <v>350.84</v>
+      </c>
       <c r="M18" s="18"/>
       <c r="N18" s="18">
         <v>336</v>
@@ -9150,7 +9485,9 @@
       <c r="Z18" s="25">
         <v>14305.64</v>
       </c>
-      <c r="AA18" s="25"/>
+      <c r="AA18" s="25">
+        <v>14510</v>
+      </c>
       <c r="AB18" s="18"/>
       <c r="AC18" s="17">
         <v>14067</v>
@@ -9191,7 +9528,9 @@
       <c r="AO18" s="25">
         <v>15995</v>
       </c>
-      <c r="AP18" s="25"/>
+      <c r="AP18" s="25">
+        <v>15870</v>
+      </c>
       <c r="AQ18" s="18"/>
       <c r="AR18" s="17"/>
       <c r="AS18" s="17"/>
@@ -9230,7 +9569,9 @@
       <c r="K19" s="25">
         <v>461.5</v>
       </c>
-      <c r="L19" s="25"/>
+      <c r="L19" s="25">
+        <v>454.54</v>
+      </c>
       <c r="M19" s="18"/>
       <c r="N19" s="18">
         <v>396</v>
@@ -9271,7 +9612,9 @@
       <c r="Z19" s="25">
         <v>15374.89</v>
       </c>
-      <c r="AA19" s="25"/>
+      <c r="AA19" s="25">
+        <v>15399.66</v>
+      </c>
       <c r="AB19" s="18"/>
       <c r="AC19" s="17">
         <v>14171</v>
@@ -9312,7 +9655,9 @@
       <c r="AO19" s="25">
         <v>36505</v>
       </c>
-      <c r="AP19" s="25"/>
+      <c r="AP19" s="25">
+        <v>35922</v>
+      </c>
       <c r="AQ19" s="18"/>
       <c r="AR19" s="17"/>
       <c r="AS19" s="17"/>
@@ -9350,7 +9695,9 @@
       <c r="K20" s="3">
         <v>672</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>602</v>
+      </c>
       <c r="M20" s="3">
         <v>492</v>
       </c>
@@ -9393,7 +9740,9 @@
       <c r="Z20" s="25">
         <v>15982.98</v>
       </c>
-      <c r="AA20" s="25"/>
+      <c r="AA20" s="25">
+        <v>15400.35</v>
+      </c>
       <c r="AB20" s="18"/>
       <c r="AC20" s="17">
         <v>14640</v>
@@ -9434,7 +9783,9 @@
       <c r="AO20" s="25">
         <v>70401</v>
       </c>
-      <c r="AP20" s="25"/>
+      <c r="AP20" s="25">
+        <v>70120</v>
+      </c>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="17"/>
       <c r="AS20" s="17"/>
@@ -9473,7 +9824,9 @@
       <c r="K21" s="25">
         <v>1721.15</v>
       </c>
-      <c r="L21" s="25"/>
+      <c r="L21" s="25">
+        <v>1707.45</v>
+      </c>
       <c r="M21" s="18"/>
       <c r="N21" s="18">
         <v>1672</v>
@@ -9514,7 +9867,9 @@
       <c r="Z21" s="25">
         <v>8758.16</v>
       </c>
-      <c r="AA21" s="25"/>
+      <c r="AA21" s="25">
+        <v>8763.08</v>
+      </c>
       <c r="AB21" s="18"/>
       <c r="AC21" s="17">
         <v>9034</v>
@@ -9555,7 +9910,9 @@
       <c r="AO21" s="25">
         <v>516.14</v>
       </c>
-      <c r="AP21" s="25"/>
+      <c r="AP21" s="25">
+        <v>476.47</v>
+      </c>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="17">
         <v>428</v>
@@ -9597,7 +9954,9 @@
       <c r="K22" s="3">
         <v>640</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>640</v>
+      </c>
       <c r="M22" s="3">
         <v>810</v>
       </c>
@@ -9640,7 +9999,9 @@
       <c r="Z22" s="25">
         <v>31655.11</v>
       </c>
-      <c r="AA22" s="25"/>
+      <c r="AA22" s="25">
+        <v>30461.5</v>
+      </c>
       <c r="AB22" s="18"/>
       <c r="AC22" s="17">
         <v>29829</v>
@@ -9681,7 +10042,9 @@
       <c r="AO22" s="25">
         <v>720</v>
       </c>
-      <c r="AP22" s="25"/>
+      <c r="AP22" s="25">
+        <v>732</v>
+      </c>
       <c r="AQ22" s="18"/>
       <c r="AR22" s="17">
         <v>760</v>
@@ -9723,7 +10086,9 @@
       <c r="K23" s="3">
         <v>1697</v>
       </c>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3">
+        <v>1573</v>
+      </c>
       <c r="M23" s="3">
         <v>1377</v>
       </c>
@@ -9766,7 +10131,9 @@
       <c r="Z23" s="25">
         <v>45404.9</v>
       </c>
-      <c r="AA23" s="25"/>
+      <c r="AA23" s="25">
+        <v>44910.01</v>
+      </c>
       <c r="AB23" s="18"/>
       <c r="AC23" s="17"/>
       <c r="AD23" s="17"/>
@@ -9803,7 +10170,9 @@
       <c r="AO23" s="25">
         <v>88061.21</v>
       </c>
-      <c r="AP23" s="25"/>
+      <c r="AP23" s="25">
+        <v>87156.85</v>
+      </c>
       <c r="AQ23" s="18"/>
       <c r="AR23" s="17"/>
       <c r="AS23" s="17"/>
@@ -9841,7 +10210,9 @@
       <c r="K24" s="3">
         <v>794</v>
       </c>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3">
+        <v>794</v>
+      </c>
       <c r="M24" s="3">
         <v>764</v>
       </c>
@@ -9884,7 +10255,9 @@
       <c r="Z24" s="25">
         <v>2246</v>
       </c>
-      <c r="AA24" s="25"/>
+      <c r="AA24" s="25">
+        <v>2207</v>
+      </c>
       <c r="AB24" s="18"/>
       <c r="AC24" s="17"/>
       <c r="AD24" s="17"/>
@@ -9921,7 +10294,9 @@
       <c r="AO24" s="25">
         <v>2751.96</v>
       </c>
-      <c r="AP24" s="25"/>
+      <c r="AP24" s="25">
+        <v>2767.74</v>
+      </c>
       <c r="AQ24" s="18"/>
       <c r="AR24" s="17"/>
       <c r="AS24" s="17"/>
@@ -9973,7 +10348,9 @@
       <c r="AO25" s="3">
         <v>2741.1</v>
       </c>
-      <c r="AP25" s="3"/>
+      <c r="AP25" s="3">
+        <v>2741.1</v>
+      </c>
       <c r="AQ25" s="3">
         <v>2980.94</v>
       </c>
@@ -10038,7 +10415,9 @@
       <c r="AO26" s="3">
         <v>3049.85</v>
       </c>
-      <c r="AP26" s="3"/>
+      <c r="AP26" s="3">
+        <v>3049.85</v>
+      </c>
       <c r="AQ26" s="3">
         <v>2806.25</v>
       </c>
@@ -10082,17 +10461,17 @@
       <c r="AJ27" s="7"/>
     </row>
     <row r="28" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
       <c r="F28" s="26"/>
     </row>
     <row r="29" spans="2:45" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:45" x14ac:dyDescent="0.25">
@@ -10160,22 +10539,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AH1:AS1"/>
-    <mergeCell ref="S1:AD1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E28"/>
-    <mergeCell ref="B29:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B29:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="AH1:AS1"/>
+    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da tabela de heuristicas
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12345" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="14400" windowHeight="12345" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -308,10 +308,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -327,13 +327,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -341,51 +334,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -401,6 +349,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -409,9 +372,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,16 +410,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -455,9 +433,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -499,31 +499,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,43 +511,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,6 +529,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -601,13 +559,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +595,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,55 +679,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,21 +829,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -855,6 +840,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,20 +877,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -920,31 +920,49 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -953,115 +971,97 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4752,7 +4752,7 @@
   <sheetPr/>
   <dimension ref="B1:AJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
@@ -8041,8 +8041,8 @@
   <sheetPr/>
   <dimension ref="B1:AJ1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -8235,7 +8235,9 @@
       <c r="E3" s="4">
         <v>2333.29</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4">
+        <v>2016.55</v>
+      </c>
       <c r="G3" s="4">
         <v>2071.57</v>
       </c>
@@ -8264,7 +8266,9 @@
       <c r="Q3" s="4">
         <v>3475</v>
       </c>
-      <c r="R3" s="4"/>
+      <c r="R3" s="4">
+        <v>3439</v>
+      </c>
       <c r="S3" s="4">
         <v>3456</v>
       </c>
@@ -8293,7 +8297,9 @@
       <c r="AC3" s="4">
         <v>69764.62</v>
       </c>
-      <c r="AD3" s="4"/>
+      <c r="AD3" s="4">
+        <v>62006.81</v>
+      </c>
       <c r="AE3" s="4">
         <v>63830.12</v>
       </c>
@@ -8339,7 +8345,9 @@
       <c r="Q4" s="4">
         <v>38395.92</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" s="4">
+        <v>40746.39</v>
+      </c>
       <c r="S4" s="4">
         <v>40637.25</v>
       </c>
@@ -8368,7 +8376,9 @@
       <c r="AC4" s="4">
         <v>32109.37</v>
       </c>
-      <c r="AD4" s="4"/>
+      <c r="AD4" s="4">
+        <v>33582.78</v>
+      </c>
       <c r="AE4" s="4">
         <v>32157.04</v>
       </c>
@@ -8399,7 +8409,9 @@
       <c r="E5" s="6">
         <v>6671</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6">
+        <v>6671</v>
+      </c>
       <c r="G5" s="6">
         <v>6962</v>
       </c>
@@ -8426,7 +8438,9 @@
       <c r="Q5" s="4">
         <v>4888</v>
       </c>
-      <c r="R5" s="4"/>
+      <c r="R5" s="4">
+        <v>4861</v>
+      </c>
       <c r="S5" s="4">
         <v>4673</v>
       </c>
@@ -8451,7 +8465,9 @@
       <c r="AC5" s="4">
         <v>41639.79</v>
       </c>
-      <c r="AD5" s="4"/>
+      <c r="AD5" s="4">
+        <v>41609.31</v>
+      </c>
       <c r="AE5" s="4">
         <v>38002.1</v>
       </c>
@@ -8482,7 +8498,9 @@
       <c r="E6" s="4">
         <v>18984</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <v>20179</v>
+      </c>
       <c r="G6" s="4">
         <v>22861</v>
       </c>
@@ -8526,7 +8544,9 @@
       <c r="AC6" s="4">
         <v>81838.74</v>
       </c>
-      <c r="AD6" s="4"/>
+      <c r="AD6" s="4">
+        <v>82975.07</v>
+      </c>
       <c r="AE6" s="4">
         <v>83744.61</v>
       </c>
@@ -8557,7 +8577,9 @@
       <c r="E7" s="6">
         <v>1068</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6">
+        <v>1068</v>
+      </c>
       <c r="G7" s="6">
         <v>1035</v>
       </c>
@@ -8607,7 +8629,9 @@
       <c r="AC7" s="4">
         <v>43036.45</v>
       </c>
-      <c r="AD7" s="4"/>
+      <c r="AD7" s="4">
+        <v>42623.35</v>
+      </c>
       <c r="AE7" s="4">
         <v>41096.15</v>
       </c>
@@ -8638,7 +8662,9 @@
       <c r="E8" s="6">
         <v>1174</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6">
+        <v>1174</v>
+      </c>
       <c r="G8" s="6">
         <v>1218</v>
       </c>
@@ -8688,7 +8714,9 @@
       <c r="AC8" s="4">
         <v>52270.61</v>
       </c>
-      <c r="AD8" s="4"/>
+      <c r="AD8" s="4">
+        <v>52270.61</v>
+      </c>
       <c r="AE8" s="4">
         <v>49580.44</v>
       </c>
@@ -8719,7 +8747,9 @@
       <c r="E9" s="6">
         <v>4629.48</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6">
+        <v>4507.49</v>
+      </c>
       <c r="G9" s="6">
         <v>4246.84</v>
       </c>
@@ -8765,7 +8795,9 @@
       <c r="AC9" s="4">
         <v>71036.73</v>
       </c>
-      <c r="AD9" s="4"/>
+      <c r="AD9" s="4">
+        <v>73236.43</v>
+      </c>
       <c r="AE9" s="4">
         <v>64612.26</v>
       </c>
@@ -8796,7 +8828,9 @@
       <c r="E10" s="4">
         <v>53625.85</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <v>54276.81</v>
+      </c>
       <c r="G10" s="4">
         <v>55846.91</v>
       </c>
@@ -8840,7 +8874,9 @@
       <c r="AC10" s="4">
         <v>35720.79</v>
       </c>
-      <c r="AD10" s="4"/>
+      <c r="AD10" s="4">
+        <v>40013.93</v>
+      </c>
       <c r="AE10" s="4">
         <v>36678.97</v>
       </c>
@@ -8867,7 +8903,9 @@
       <c r="E11" s="4">
         <v>13353</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4">
+        <v>13353</v>
+      </c>
       <c r="G11" s="4">
         <v>13127</v>
       </c>
@@ -8892,7 +8930,9 @@
       <c r="Q11" s="4">
         <v>7988</v>
       </c>
-      <c r="R11" s="4"/>
+      <c r="R11" s="4">
+        <v>8543</v>
+      </c>
       <c r="S11" s="4">
         <v>8459</v>
       </c>
@@ -8921,7 +8961,9 @@
       <c r="AC11" s="4">
         <v>40552.27</v>
       </c>
-      <c r="AD11" s="4"/>
+      <c r="AD11" s="4">
+        <v>39527.08</v>
+      </c>
       <c r="AE11" s="4">
         <v>37664.62</v>
       </c>
@@ -8948,7 +8990,9 @@
       <c r="E12" s="4">
         <v>1490</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <v>3180</v>
+      </c>
       <c r="G12" s="4">
         <v>9360</v>
       </c>
@@ -8973,7 +9017,9 @@
       <c r="Q12" s="4">
         <v>17516.66</v>
       </c>
-      <c r="R12" s="4"/>
+      <c r="R12" s="4">
+        <v>16393.25</v>
+      </c>
       <c r="S12" s="4">
         <v>17585.83</v>
       </c>
@@ -9002,7 +9048,9 @@
       <c r="AC12" s="4">
         <v>70952.95</v>
       </c>
-      <c r="AD12" s="4"/>
+      <c r="AD12" s="4">
+        <v>62693.37</v>
+      </c>
       <c r="AE12" s="4">
         <v>65334.95</v>
       </c>
@@ -9029,7 +9077,9 @@
       <c r="E13" s="6">
         <v>1953.16</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6">
+        <v>1953.16</v>
+      </c>
       <c r="G13" s="6">
         <v>1943.98</v>
       </c>
@@ -9060,7 +9110,9 @@
       <c r="Q13" s="4">
         <v>21753.58</v>
       </c>
-      <c r="R13" s="4"/>
+      <c r="R13" s="4">
+        <v>20552.91</v>
+      </c>
       <c r="S13" s="4">
         <v>22681.11</v>
       </c>
@@ -9089,7 +9141,9 @@
       <c r="AC13" s="4">
         <v>218655.55</v>
       </c>
-      <c r="AD13" s="4"/>
+      <c r="AD13" s="4">
+        <v>197177.83</v>
+      </c>
       <c r="AE13" s="4">
         <v>205376.77</v>
       </c>
@@ -9116,7 +9170,9 @@
       <c r="E14" s="4">
         <v>4786.06</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4">
+        <v>4557.5</v>
+      </c>
       <c r="G14" s="4">
         <v>4152.75</v>
       </c>
@@ -9145,7 +9201,9 @@
       <c r="Q14" s="4">
         <v>24404.94</v>
       </c>
-      <c r="R14" s="4"/>
+      <c r="R14" s="4">
+        <v>21986.72</v>
+      </c>
       <c r="S14" s="4">
         <v>20952.57</v>
       </c>
@@ -9174,7 +9232,9 @@
       <c r="AC14" s="4">
         <v>1047.43</v>
       </c>
-      <c r="AD14" s="4"/>
+      <c r="AD14" s="4">
+        <v>980.84</v>
+      </c>
       <c r="AE14" s="4">
         <v>900.63</v>
       </c>
@@ -9205,7 +9265,9 @@
       <c r="E15" s="4">
         <v>5392.18</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4">
+        <v>5011.93</v>
+      </c>
       <c r="G15" s="4">
         <v>4898.32</v>
       </c>
@@ -9234,7 +9296,9 @@
       <c r="Q15" s="4">
         <v>18768.06</v>
       </c>
-      <c r="R15" s="4"/>
+      <c r="R15" s="4">
+        <v>17378.96</v>
+      </c>
       <c r="S15" s="4">
         <v>17195.84</v>
       </c>
@@ -9263,7 +9327,9 @@
       <c r="AC15" s="4">
         <v>1944.15</v>
       </c>
-      <c r="AD15" s="4"/>
+      <c r="AD15" s="4">
+        <v>1848.69</v>
+      </c>
       <c r="AE15" s="4">
         <v>1695.61</v>
       </c>
@@ -9294,7 +9360,9 @@
       <c r="E16" s="6">
         <v>393</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6">
+        <v>397</v>
+      </c>
       <c r="G16" s="6">
         <v>486</v>
       </c>
@@ -9323,7 +9391,9 @@
       <c r="Q16" s="4">
         <v>20307.55</v>
       </c>
-      <c r="R16" s="4"/>
+      <c r="R16" s="4">
+        <v>19697.26</v>
+      </c>
       <c r="S16" s="4">
         <v>17422.93</v>
       </c>
@@ -9352,7 +9422,9 @@
       <c r="AC16" s="4">
         <v>5694.36</v>
       </c>
-      <c r="AD16" s="4"/>
+      <c r="AD16" s="4">
+        <v>5532.36</v>
+      </c>
       <c r="AE16" s="4">
         <v>5770.28</v>
       </c>
@@ -9379,7 +9451,9 @@
       <c r="E17" s="6">
         <v>323.66</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6">
+        <v>286.55</v>
+      </c>
       <c r="G17" s="6">
         <v>291.59</v>
       </c>
@@ -9410,7 +9484,9 @@
       <c r="Q17" s="4">
         <v>24802.49</v>
       </c>
-      <c r="R17" s="4"/>
+      <c r="R17" s="4">
+        <v>25013.39</v>
+      </c>
       <c r="S17" s="4">
         <v>24207.55</v>
       </c>
@@ -9439,7 +9515,9 @@
       <c r="AC17" s="4">
         <v>7408.05</v>
       </c>
-      <c r="AD17" s="4"/>
+      <c r="AD17" s="4">
+        <v>7252.31</v>
+      </c>
       <c r="AE17" s="4">
         <v>7263.55</v>
       </c>
@@ -9466,7 +9544,9 @@
       <c r="E18" s="4">
         <v>373.07</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4">
+        <v>366.84</v>
+      </c>
       <c r="G18" s="4">
         <v>353.56</v>
       </c>
@@ -9495,7 +9575,9 @@
       <c r="Q18" s="4">
         <v>18900.41</v>
       </c>
-      <c r="R18" s="4"/>
+      <c r="R18" s="4">
+        <v>17330.6</v>
+      </c>
       <c r="S18" s="4">
         <v>14510</v>
       </c>
@@ -9524,7 +9606,9 @@
       <c r="AC18" s="4">
         <v>16373</v>
       </c>
-      <c r="AD18" s="4"/>
+      <c r="AD18" s="4">
+        <v>16157</v>
+      </c>
       <c r="AE18" s="4">
         <v>15988</v>
       </c>
@@ -9551,7 +9635,9 @@
       <c r="E19" s="4">
         <v>452.67</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <v>457.56</v>
+      </c>
       <c r="G19" s="4">
         <v>479.74</v>
       </c>
@@ -9580,7 +9666,9 @@
       <c r="Q19" s="4">
         <v>17083.72</v>
       </c>
-      <c r="R19" s="4"/>
+      <c r="R19" s="4">
+        <v>17083.72</v>
+      </c>
       <c r="S19" s="4">
         <v>16131.15</v>
       </c>
@@ -9609,7 +9697,9 @@
       <c r="AC19" s="4">
         <v>35948</v>
       </c>
-      <c r="AD19" s="4"/>
+      <c r="AD19" s="4">
+        <v>36087</v>
+      </c>
       <c r="AE19" s="4">
         <v>36577</v>
       </c>
@@ -9636,7 +9726,9 @@
       <c r="E20" s="6">
         <v>608</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6">
+        <v>581</v>
+      </c>
       <c r="G20" s="6">
         <v>684</v>
       </c>
@@ -9667,7 +9759,9 @@
       <c r="Q20" s="4">
         <v>17078.29</v>
       </c>
-      <c r="R20" s="4"/>
+      <c r="R20" s="4">
+        <v>17083.72</v>
+      </c>
       <c r="S20" s="4">
         <v>16256.53</v>
       </c>
@@ -9696,7 +9790,9 @@
       <c r="AC20" s="4">
         <v>70198</v>
       </c>
-      <c r="AD20" s="4"/>
+      <c r="AD20" s="4">
+        <v>70536</v>
+      </c>
       <c r="AE20" s="4">
         <v>70571</v>
       </c>
@@ -9723,7 +9819,9 @@
       <c r="E21" s="4">
         <v>1967.63</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4">
+        <v>1882.37</v>
+      </c>
       <c r="G21" s="4">
         <v>1733.52</v>
       </c>
@@ -9752,7 +9850,9 @@
       <c r="Q21" s="4">
         <v>9002.37</v>
       </c>
-      <c r="R21" s="4"/>
+      <c r="R21" s="4">
+        <v>9397.47</v>
+      </c>
       <c r="S21" s="4">
         <v>8932.87</v>
       </c>
@@ -9781,7 +9881,9 @@
       <c r="AC21" s="7">
         <v>437.11</v>
       </c>
-      <c r="AD21" s="7"/>
+      <c r="AD21" s="7">
+        <v>524.62</v>
+      </c>
       <c r="AE21" s="4">
         <v>514.7</v>
       </c>
@@ -9812,7 +9914,9 @@
       <c r="E22" s="6">
         <v>813</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6">
+        <v>661</v>
+      </c>
       <c r="G22" s="6">
         <v>640</v>
       </c>
@@ -9843,7 +9947,9 @@
       <c r="Q22" s="4">
         <v>34803.33</v>
       </c>
-      <c r="R22" s="4"/>
+      <c r="R22" s="4">
+        <v>35374.47</v>
+      </c>
       <c r="S22" s="4">
         <v>32712.82</v>
       </c>
@@ -9872,7 +9978,9 @@
       <c r="AC22" s="4">
         <v>871</v>
       </c>
-      <c r="AD22" s="4"/>
+      <c r="AD22" s="4">
+        <v>757</v>
+      </c>
       <c r="AE22" s="4">
         <v>732</v>
       </c>
@@ -9903,7 +10011,9 @@
       <c r="E23" s="6">
         <v>1351</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="6">
+        <v>1351</v>
+      </c>
       <c r="G23" s="6">
         <v>1703</v>
       </c>
@@ -9959,7 +10069,9 @@
       <c r="AC23" s="4">
         <v>117345.37</v>
       </c>
-      <c r="AD23" s="4"/>
+      <c r="AD23" s="4">
+        <v>87227.92</v>
+      </c>
       <c r="AE23" s="4">
         <v>89500</v>
       </c>
@@ -9986,7 +10098,9 @@
       <c r="E24" s="6">
         <v>802</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="6">
+        <v>802</v>
+      </c>
       <c r="G24" s="6">
         <v>794</v>
       </c>
@@ -10017,7 +10131,9 @@
       <c r="Q24" s="4">
         <v>2150</v>
       </c>
-      <c r="R24" s="4"/>
+      <c r="R24" s="4">
+        <v>2155</v>
+      </c>
       <c r="S24" s="4">
         <v>2300</v>
       </c>
@@ -10042,7 +10158,9 @@
       <c r="AC24" s="4">
         <v>3247.49</v>
       </c>
-      <c r="AD24" s="4"/>
+      <c r="AD24" s="4">
+        <v>2915.74</v>
+      </c>
       <c r="AE24" s="4">
         <v>2794.99</v>
       </c>
@@ -10080,7 +10198,9 @@
       <c r="AC25" s="6">
         <v>3035.89</v>
       </c>
-      <c r="AD25" s="6"/>
+      <c r="AD25" s="6">
+        <v>3035.89</v>
+      </c>
       <c r="AE25" s="6">
         <v>2741.1</v>
       </c>
@@ -10131,7 +10251,9 @@
       <c r="AC26" s="6">
         <v>2959.96</v>
       </c>
-      <c r="AD26" s="6"/>
+      <c r="AD26" s="6">
+        <v>2959.96</v>
+      </c>
       <c r="AE26" s="6">
         <v>3049.85</v>
       </c>

</xml_diff>

<commit_message>
Adição da tabela de Análise(Ainda incompleta)
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -305,8 +305,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -331,29 +331,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -375,6 +360,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -388,14 +388,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -423,6 +415,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -432,9 +432,31 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -447,35 +469,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,12 +508,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -526,19 +520,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,25 +574,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +610,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,67 +658,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,7 +682,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,25 +700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,13 +856,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -884,15 +891,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -923,6 +921,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -944,46 +953,31 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -995,13 +989,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1010,104 +1007,101 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1165,22 +1159,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1217,12 +1208,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1541,8 +1526,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC25" sqref="AC25:AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -1706,23 +1691,23 @@
       <c r="C3" s="1">
         <v>70</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>632.3</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>746.64</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="30">
         <v>746.64</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="31">
         <v>862.87</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30">
         <v>606</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="38">
         <v>606</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1731,23 +1716,23 @@
       <c r="M3" s="1">
         <v>12</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="30">
         <v>668</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="30">
         <v>558</v>
       </c>
-      <c r="P3" s="31">
+      <c r="P3" s="30">
         <v>582</v>
       </c>
-      <c r="Q3" s="32">
+      <c r="Q3" s="31">
         <v>590</v>
       </c>
-      <c r="R3" s="31"/>
-      <c r="S3" s="39">
+      <c r="R3" s="30"/>
+      <c r="S3" s="38">
         <v>558</v>
       </c>
-      <c r="T3" s="39">
+      <c r="T3" s="38">
         <v>558</v>
       </c>
       <c r="V3" s="1" t="s">
@@ -1765,7 +1750,7 @@
       <c r="Z3" s="4">
         <v>25126.84</v>
       </c>
-      <c r="AA3" s="43">
+      <c r="AA3" s="5">
         <v>28078.94</v>
       </c>
       <c r="AB3" s="4"/>
@@ -1783,36 +1768,36 @@
       <c r="C4" s="1">
         <v>133</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="39"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="38"/>
       <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="1">
         <v>24</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="30">
         <v>11086.43</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="30">
         <v>9934.05</v>
       </c>
-      <c r="P4" s="31">
+      <c r="P4" s="30">
         <v>10253.47</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="31">
         <v>9467.2</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="39">
+      <c r="R4" s="30"/>
+      <c r="S4" s="38">
         <v>7704</v>
       </c>
-      <c r="T4" s="39">
+      <c r="T4" s="38">
         <v>7704</v>
       </c>
       <c r="V4" s="1" t="s">
@@ -1830,7 +1815,7 @@
       <c r="Z4" s="4">
         <v>7936.1</v>
       </c>
-      <c r="AA4" s="43">
+      <c r="AA4" s="5">
         <v>7504.68</v>
       </c>
       <c r="AB4" s="4"/>
@@ -1848,44 +1833,44 @@
       <c r="C5" s="6">
         <v>12</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>1409</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>1409</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>1409</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="33">
         <v>1193</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="32">
         <v>1239</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="40"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="39"/>
       <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M5" s="1">
         <v>30</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="30">
         <v>1411</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="30">
         <v>1422</v>
       </c>
-      <c r="P5" s="31">
+      <c r="P5" s="30">
         <v>1356</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="31">
         <v>1790</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
       <c r="V5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1901,7 +1886,7 @@
       <c r="Z5" s="4">
         <v>14065.44</v>
       </c>
-      <c r="AA5" s="43">
+      <c r="AA5" s="5">
         <v>10773.88</v>
       </c>
       <c r="AB5" s="4"/>
@@ -1919,36 +1904,36 @@
       <c r="C6" s="1">
         <v>133</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="30">
         <v>5712</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="30">
         <v>4475</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>4698</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <v>6959</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="39"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="38"/>
       <c r="L6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M6" s="1">
         <v>34</v>
       </c>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="39">
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="38">
         <v>14784</v>
       </c>
-      <c r="T6" s="39">
+      <c r="T6" s="38">
         <v>14784</v>
       </c>
       <c r="V6" s="1" t="s">
@@ -1966,7 +1951,7 @@
       <c r="Z6" s="4">
         <v>23232.62</v>
       </c>
-      <c r="AA6" s="43">
+      <c r="AA6" s="5">
         <v>24290.25</v>
       </c>
       <c r="AB6" s="4"/>
@@ -1984,25 +1969,25 @@
       <c r="C7" s="6">
         <v>7</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>292</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>292</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>292</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="33">
         <v>285</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="32">
         <v>246</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="32">
         <v>246</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="39">
         <v>246</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -2011,15 +1996,15 @@
       <c r="M7" s="1">
         <v>50</v>
       </c>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="39">
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="38">
         <v>6977</v>
       </c>
-      <c r="T7" s="39">
+      <c r="T7" s="38">
         <v>6977</v>
       </c>
       <c r="V7" s="1" t="s">
@@ -2037,7 +2022,7 @@
       <c r="Z7" s="4">
         <v>11559.29</v>
       </c>
-      <c r="AA7" s="43">
+      <c r="AA7" s="5">
         <v>12002.27</v>
       </c>
       <c r="AB7" s="4"/>
@@ -2055,25 +2040,25 @@
       <c r="C8" s="6">
         <v>7</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>352</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>352</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>352</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <v>378</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="34">
         <v>282</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="32">
         <v>282</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="39">
         <v>282</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -2082,15 +2067,15 @@
       <c r="M8" s="1">
         <v>57</v>
       </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="39">
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="38">
         <v>18471</v>
       </c>
-      <c r="T8" s="39">
+      <c r="T8" s="38">
         <v>18471</v>
       </c>
       <c r="V8" s="1" t="s">
@@ -2108,7 +2093,7 @@
       <c r="Z8" s="4">
         <v>17072</v>
       </c>
-      <c r="AA8" s="43">
+      <c r="AA8" s="5">
         <v>14653.02</v>
       </c>
       <c r="AB8" s="4"/>
@@ -2126,25 +2111,25 @@
       <c r="C9" s="6">
         <v>13</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>604.66</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>604.66</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>604.66</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="33">
         <v>575.87</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="32">
         <v>480.480334457013</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="32">
         <v>489</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="39">
         <v>489</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -2153,13 +2138,13 @@
       <c r="M9" s="1">
         <v>107</v>
       </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
       <c r="V9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2175,7 +2160,7 @@
       <c r="Z9" s="4">
         <v>23494.84</v>
       </c>
-      <c r="AA9" s="43">
+      <c r="AA9" s="5">
         <v>24798.56</v>
       </c>
       <c r="AB9" s="4"/>
@@ -2193,23 +2178,23 @@
       <c r="C10" s="1">
         <v>31</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>14342.78</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="30">
         <v>11706.58</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>13031.31</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>14467.58</v>
       </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31">
+      <c r="H10" s="30"/>
+      <c r="I10" s="30">
         <v>9840</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <v>10132</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -2218,13 +2203,13 @@
       <c r="M10" s="1">
         <v>166</v>
       </c>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
       <c r="V10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2240,7 +2225,7 @@
       <c r="Z10" s="4">
         <v>8100</v>
       </c>
-      <c r="AA10" s="43">
+      <c r="AA10" s="5">
         <v>8198.42</v>
       </c>
       <c r="AB10" s="4"/>
@@ -2254,44 +2239,44 @@
       <c r="C11" s="1">
         <v>14</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>6116</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="30">
         <v>4607</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="30">
         <v>4607</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>4530</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="39"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="38"/>
       <c r="L11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M11" s="1">
         <v>12</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="30">
         <v>3454</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="30">
         <v>3155</v>
       </c>
-      <c r="P11" s="31">
+      <c r="P11" s="30">
         <v>3155</v>
       </c>
-      <c r="Q11" s="32">
+      <c r="Q11" s="31">
         <v>3467</v>
       </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="39">
+      <c r="R11" s="30"/>
+      <c r="S11" s="38">
         <v>2094</v>
       </c>
-      <c r="T11" s="39">
+      <c r="T11" s="38">
         <v>2094</v>
       </c>
       <c r="V11" s="1" t="s">
@@ -2309,7 +2294,7 @@
       <c r="Z11" s="4">
         <v>10604.72</v>
       </c>
-      <c r="AA11" s="43">
+      <c r="AA11" s="5">
         <v>12899.09</v>
       </c>
       <c r="AB11" s="4"/>
@@ -2323,42 +2308,42 @@
       <c r="C12" s="24">
         <v>45</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="35">
         <v>21120</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="35">
         <v>480</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="35">
         <v>820</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="39"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="38"/>
       <c r="L12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M12" s="1">
         <v>25</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="30">
         <v>5157.68</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="30">
         <v>4872.02</v>
       </c>
-      <c r="P12" s="31">
+      <c r="P12" s="30">
         <v>4788.84</v>
       </c>
-      <c r="Q12" s="32">
+      <c r="Q12" s="31">
         <v>5274.63</v>
       </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="39">
+      <c r="R12" s="30"/>
+      <c r="S12" s="38">
         <v>4369</v>
       </c>
-      <c r="T12" s="39">
+      <c r="T12" s="38">
         <v>4369</v>
       </c>
       <c r="V12" s="1" t="s">
@@ -2376,7 +2361,7 @@
       <c r="Z12" s="4">
         <v>22455.5</v>
       </c>
-      <c r="AA12" s="43">
+      <c r="AA12" s="5">
         <v>27145.63</v>
       </c>
       <c r="AB12" s="4"/>
@@ -2390,25 +2375,25 @@
       <c r="C13" s="6">
         <v>3</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>249.88</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>249.88</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>249.88</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="33">
         <v>308.18</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="32">
         <v>224.88</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="32">
         <v>151</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="39">
         <v>151</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -2417,23 +2402,23 @@
       <c r="M13" s="1">
         <v>37</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="30">
         <v>6644.96</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="30">
         <v>7646.9</v>
       </c>
-      <c r="P13" s="31">
+      <c r="P13" s="30">
         <v>7646.9</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="31">
         <v>6724.8</v>
       </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="39">
+      <c r="R13" s="30"/>
+      <c r="S13" s="38">
         <v>5286</v>
       </c>
-      <c r="T13" s="39">
+      <c r="T13" s="38">
         <v>5286</v>
       </c>
       <c r="V13" s="1" t="s">
@@ -2451,7 +2436,7 @@
       <c r="Z13" s="4">
         <v>66904.56</v>
       </c>
-      <c r="AA13" s="43">
+      <c r="AA13" s="5">
         <v>83408.29</v>
       </c>
       <c r="AB13" s="4"/>
@@ -2465,23 +2450,23 @@
       <c r="C14" s="1">
         <v>32</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>1211.59</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <v>1230.99</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="30">
         <v>1230.99</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>1380.72</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31">
+      <c r="H14" s="30"/>
+      <c r="I14" s="30">
         <v>1116</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="38">
         <v>1119</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -2490,23 +2475,23 @@
       <c r="M14" s="1">
         <v>50</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="30">
         <v>6870.92</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="30">
         <v>6899.46</v>
       </c>
-      <c r="P14" s="31">
+      <c r="P14" s="30">
         <v>6927.27</v>
       </c>
-      <c r="Q14" s="32">
+      <c r="Q14" s="31">
         <v>9243.01</v>
       </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="39">
+      <c r="R14" s="30"/>
+      <c r="S14" s="38">
         <v>6138</v>
       </c>
-      <c r="T14" s="39">
+      <c r="T14" s="38">
         <v>6138</v>
       </c>
       <c r="V14" s="1" t="s">
@@ -2524,7 +2509,7 @@
       <c r="Z14" s="4">
         <v>292.55</v>
       </c>
-      <c r="AA14" s="43">
+      <c r="AA14" s="5">
         <v>366.6</v>
       </c>
       <c r="AB14" s="4"/>
@@ -2542,23 +2527,23 @@
       <c r="C15" s="1">
         <v>37</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>1304.57</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>1400.68</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="30">
         <v>1245.96</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>1748.47</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31">
+      <c r="H15" s="30"/>
+      <c r="I15" s="30">
         <v>1204</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="38">
         <v>1204</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -2567,23 +2552,23 @@
       <c r="M15" s="1">
         <v>25</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="30">
         <v>5552.01</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="30">
         <v>4469.81</v>
       </c>
-      <c r="P15" s="31">
+      <c r="P15" s="30">
         <v>5429.03</v>
       </c>
-      <c r="Q15" s="32">
+      <c r="Q15" s="31">
         <v>6142.49</v>
       </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="39">
+      <c r="R15" s="30"/>
+      <c r="S15" s="38">
         <v>4014</v>
       </c>
-      <c r="T15" s="39">
+      <c r="T15" s="38">
         <v>4014</v>
       </c>
       <c r="V15" s="1" t="s">
@@ -2601,7 +2586,7 @@
       <c r="Z15" s="4">
         <v>546.13</v>
       </c>
-      <c r="AA15" s="43">
+      <c r="AA15" s="5">
         <v>626.49</v>
       </c>
       <c r="AB15" s="4"/>
@@ -2619,25 +2604,25 @@
       <c r="C16" s="6">
         <v>10</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <v>103</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <v>103</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="36">
         <v>103</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <v>130</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="37">
         <v>99</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="32">
         <v>99</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="39">
         <v>99</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -2646,23 +2631,23 @@
       <c r="M16" s="1">
         <v>37</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="30">
         <v>5199.62</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="30">
         <v>5533.11</v>
       </c>
-      <c r="P16" s="31">
+      <c r="P16" s="30">
         <v>5533.11</v>
       </c>
-      <c r="Q16" s="32">
+      <c r="Q16" s="31">
         <v>5488.4</v>
       </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="39">
+      <c r="R16" s="30"/>
+      <c r="S16" s="38">
         <v>5119</v>
       </c>
-      <c r="T16" s="39">
+      <c r="T16" s="38">
         <v>5119</v>
       </c>
       <c r="V16" s="1" t="s">
@@ -2680,7 +2665,7 @@
       <c r="Z16" s="4">
         <v>1726.09</v>
       </c>
-      <c r="AA16" s="43">
+      <c r="AA16" s="5">
         <v>1838.06</v>
       </c>
       <c r="AB16" s="4"/>
@@ -2694,25 +2679,25 @@
       <c r="C17" s="6">
         <v>12</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <v>77.04</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <v>77.04</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="36">
         <v>77.04</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="33">
         <v>81.96</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="37">
         <v>76.72</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="32">
         <v>71</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="39">
         <v>71</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -2721,23 +2706,23 @@
       <c r="M17" s="1">
         <v>50</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="30">
         <v>6907.12</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="30">
         <v>8397.45</v>
       </c>
-      <c r="P17" s="31">
+      <c r="P17" s="30">
         <v>7306.16</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="31">
         <v>6956.31</v>
       </c>
-      <c r="R17" s="31"/>
-      <c r="S17" s="39">
+      <c r="R17" s="30"/>
+      <c r="S17" s="38">
         <v>5890</v>
       </c>
-      <c r="T17" s="39">
+      <c r="T17" s="38">
         <v>5890</v>
       </c>
       <c r="V17" s="1" t="s">
@@ -2755,7 +2740,7 @@
       <c r="Z17" s="4">
         <v>2280.15</v>
       </c>
-      <c r="AA17" s="43">
+      <c r="AA17" s="5">
         <v>2464.03</v>
       </c>
       <c r="AB17" s="4"/>
@@ -2769,23 +2754,23 @@
       <c r="C18" s="1">
         <v>19</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="30">
         <v>97.38</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="30">
         <v>99.45</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="30">
         <v>99.45</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <v>114.81</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31">
+      <c r="H18" s="30"/>
+      <c r="I18" s="30">
         <v>99</v>
       </c>
-      <c r="J18" s="39">
+      <c r="J18" s="38">
         <v>99</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -2794,23 +2779,23 @@
       <c r="M18" s="1">
         <v>25</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="30">
         <v>4346.52</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O18" s="30">
         <v>6123.26</v>
       </c>
-      <c r="P18" s="31">
+      <c r="P18" s="30">
         <v>4346.52</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="31">
         <v>5038.15</v>
       </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="39">
+      <c r="R18" s="30"/>
+      <c r="S18" s="38">
         <v>4293</v>
       </c>
-      <c r="T18" s="39">
+      <c r="T18" s="38">
         <v>4293</v>
       </c>
       <c r="V18" s="1" t="s">
@@ -2828,7 +2813,7 @@
       <c r="Z18" s="4">
         <v>5420</v>
       </c>
-      <c r="AA18" s="43">
+      <c r="AA18" s="5">
         <v>5214</v>
       </c>
       <c r="AB18" s="4"/>
@@ -2842,23 +2827,23 @@
       <c r="C19" s="1">
         <v>25</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <v>150.96</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="30">
         <v>132.75</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="30">
         <v>139.62</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>142.41</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31">
+      <c r="H19" s="30"/>
+      <c r="I19" s="30">
         <v>101</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="38">
         <v>101</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -2867,23 +2852,23 @@
       <c r="M19" s="1">
         <v>25</v>
       </c>
-      <c r="N19" s="31">
+      <c r="N19" s="30">
         <v>5246.28</v>
       </c>
-      <c r="O19" s="31">
+      <c r="O19" s="30">
         <v>5246.28</v>
       </c>
-      <c r="P19" s="31">
+      <c r="P19" s="30">
         <v>5246.28</v>
       </c>
-      <c r="Q19" s="32">
+      <c r="Q19" s="31">
         <v>5514.75</v>
       </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="39">
+      <c r="R19" s="30"/>
+      <c r="S19" s="38">
         <v>3991</v>
       </c>
-      <c r="T19" s="39">
+      <c r="T19" s="38">
         <v>3991</v>
       </c>
       <c r="V19" s="1" t="s">
@@ -2901,7 +2886,7 @@
       <c r="Z19" s="4">
         <v>12196</v>
       </c>
-      <c r="AA19" s="43">
+      <c r="AA19" s="5">
         <v>12061</v>
       </c>
       <c r="AB19" s="4"/>
@@ -2915,25 +2900,25 @@
       <c r="C20" s="6">
         <v>6</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <v>147</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <v>147</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="32">
         <v>147</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <v>148</v>
       </c>
-      <c r="H20" s="33">
+      <c r="H20" s="32">
         <v>145</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="32">
         <v>145</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J20" s="39">
         <v>145</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -2942,23 +2927,23 @@
       <c r="M20" s="1">
         <v>25</v>
       </c>
-      <c r="N20" s="31">
+      <c r="N20" s="30">
         <v>4123.35</v>
       </c>
-      <c r="O20" s="31">
+      <c r="O20" s="30">
         <v>3842.76</v>
       </c>
-      <c r="P20" s="31">
+      <c r="P20" s="30">
         <v>3955.74</v>
       </c>
-      <c r="Q20" s="32">
+      <c r="Q20" s="31">
         <v>4039.52</v>
       </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="39">
+      <c r="R20" s="30"/>
+      <c r="S20" s="38">
         <v>3663</v>
       </c>
-      <c r="T20" s="39">
+      <c r="T20" s="38">
         <v>3663</v>
       </c>
       <c r="V20" s="1" t="s">
@@ -2976,7 +2961,7 @@
       <c r="Z20" s="4">
         <v>22414</v>
       </c>
-      <c r="AA20" s="43">
+      <c r="AA20" s="5">
         <v>22462</v>
       </c>
       <c r="AB20" s="4"/>
@@ -2990,23 +2975,23 @@
       <c r="C21" s="1">
         <v>65</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <v>562.04</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="30">
         <v>666.2</v>
       </c>
-      <c r="F21" s="31">
+      <c r="F21" s="30">
         <v>666.2</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <v>616.4</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31">
+      <c r="H21" s="30"/>
+      <c r="I21" s="30">
         <v>509</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="38">
         <v>509</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -3015,23 +3000,23 @@
       <c r="M21" s="1">
         <v>26</v>
       </c>
-      <c r="N21" s="31">
+      <c r="N21" s="30">
         <v>2149.82</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="30">
         <v>2067.87</v>
       </c>
-      <c r="P21" s="31">
+      <c r="P21" s="30">
         <v>2002.98</v>
       </c>
-      <c r="Q21" s="32">
+      <c r="Q21" s="31">
         <v>1978.97</v>
       </c>
-      <c r="R21" s="31"/>
-      <c r="S21" s="39">
+      <c r="R21" s="30"/>
+      <c r="S21" s="38">
         <v>2108</v>
       </c>
-      <c r="T21" s="39">
+      <c r="T21" s="38">
         <v>2108</v>
       </c>
       <c r="V21" s="24" t="s">
@@ -3049,7 +3034,7 @@
       <c r="Z21" s="9">
         <v>128.07</v>
       </c>
-      <c r="AA21" s="43">
+      <c r="AA21" s="5">
         <v>103.31</v>
       </c>
       <c r="AB21" s="9"/>
@@ -3067,25 +3052,25 @@
       <c r="C22" s="6">
         <v>4</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <v>174</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>154</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="32">
         <v>154</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <v>154</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="32">
         <v>143</v>
       </c>
-      <c r="I22" s="33">
+      <c r="I22" s="32">
         <v>143</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="39">
         <v>143</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -3094,23 +3079,23 @@
       <c r="M22" s="1">
         <v>79</v>
       </c>
-      <c r="N22" s="31">
+      <c r="N22" s="30">
         <v>9156.66</v>
       </c>
-      <c r="O22" s="31">
+      <c r="O22" s="30">
         <v>9230.75</v>
       </c>
-      <c r="P22" s="31">
+      <c r="P22" s="30">
         <v>9553.4</v>
       </c>
-      <c r="Q22" s="32">
+      <c r="Q22" s="31">
         <v>9113.74</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="39">
+      <c r="R22" s="30"/>
+      <c r="S22" s="38">
         <v>8705</v>
       </c>
-      <c r="T22" s="39">
+      <c r="T22" s="38">
         <v>8705</v>
       </c>
       <c r="V22" s="1" t="s">
@@ -3128,7 +3113,7 @@
       <c r="Z22" s="4">
         <v>146</v>
       </c>
-      <c r="AA22" s="43">
+      <c r="AA22" s="5">
         <v>152</v>
       </c>
       <c r="AB22" s="4"/>
@@ -3146,25 +3131,25 @@
       <c r="C23" s="6">
         <v>5</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="32">
         <v>258</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="32">
         <v>248</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="32">
         <v>248</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <v>202</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="32">
         <v>181</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="32">
         <v>178</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J23" s="39">
         <v>178</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -3173,21 +3158,21 @@
       <c r="M23" s="1">
         <v>344</v>
       </c>
-      <c r="N23" s="31">
+      <c r="N23" s="30">
         <v>13388.78</v>
       </c>
-      <c r="O23" s="31">
+      <c r="O23" s="30">
         <v>13074.68</v>
       </c>
-      <c r="P23" s="31">
+      <c r="P23" s="30">
         <v>12948.7</v>
       </c>
-      <c r="Q23" s="32">
+      <c r="Q23" s="31">
         <v>16673.39</v>
       </c>
-      <c r="R23" s="31"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
       <c r="V23" s="1" t="s">
         <v>75</v>
       </c>
@@ -3203,7 +3188,7 @@
       <c r="Z23" s="4">
         <v>27500</v>
       </c>
-      <c r="AA23" s="43">
+      <c r="AA23" s="5">
         <v>37118.03</v>
       </c>
       <c r="AB23" s="4"/>
@@ -3217,25 +3202,25 @@
       <c r="C24" s="6">
         <v>6</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <v>162</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <v>162</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="32">
         <v>162</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="33">
         <v>162</v>
       </c>
-      <c r="H24" s="33">
+      <c r="H24" s="32">
         <v>162</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="32">
         <v>231</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="39">
         <v>231</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -3244,21 +3229,21 @@
       <c r="M24" s="1">
         <v>140</v>
       </c>
-      <c r="N24" s="31">
+      <c r="N24" s="30">
         <v>728</v>
       </c>
-      <c r="O24" s="31">
+      <c r="O24" s="30">
         <v>566</v>
       </c>
-      <c r="P24" s="31">
+      <c r="P24" s="30">
         <v>642</v>
       </c>
-      <c r="Q24" s="32">
+      <c r="Q24" s="31">
         <v>943</v>
       </c>
-      <c r="R24" s="31"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
       <c r="V24" s="1" t="s">
         <v>78</v>
       </c>
@@ -3274,7 +3259,7 @@
       <c r="Z24" s="4">
         <v>1109.08</v>
       </c>
-      <c r="AA24" s="43">
+      <c r="AA24" s="5">
         <v>1070.78</v>
       </c>
       <c r="AB24" s="4"/>
@@ -3300,7 +3285,7 @@
       <c r="Z25" s="7">
         <v>751.06</v>
       </c>
-      <c r="AA25" s="44">
+      <c r="AA25" s="8">
         <v>751.06</v>
       </c>
       <c r="AB25" s="7">
@@ -3334,7 +3319,7 @@
       <c r="V26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="W26" s="41">
+      <c r="W26" s="40">
         <v>5</v>
       </c>
       <c r="X26" s="7">
@@ -3346,7 +3331,7 @@
       <c r="Z26" s="7">
         <v>456.58</v>
       </c>
-      <c r="AA26" s="44">
+      <c r="AA26" s="8">
         <v>784.47</v>
       </c>
       <c r="AB26" s="7">
@@ -3381,8 +3366,8 @@
       <c r="S27" s="22"/>
       <c r="T27" s="22"/>
       <c r="U27" s="22"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
       <c r="X27" s="22"/>
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
@@ -3397,7 +3382,7 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" customHeight="1" spans="2:2">
-      <c r="B29" s="29"/>
+      <c r="B29" s="28"/>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.75" customHeight="1"/>
@@ -4416,7 +4401,7 @@
   <dimension ref="B1:AD1000"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+      <selection activeCell="AC25" sqref="AC25:AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -4588,7 +4573,7 @@
       <c r="F3" s="4">
         <v>1380.52</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="5">
         <v>1651.14</v>
       </c>
       <c r="H3" s="4"/>
@@ -4613,7 +4598,7 @@
       <c r="P3" s="4">
         <v>1691</v>
       </c>
-      <c r="Q3" s="27">
+      <c r="Q3" s="5">
         <v>1693</v>
       </c>
       <c r="R3" s="4"/>
@@ -4638,7 +4623,7 @@
       <c r="Z3" s="4">
         <v>44191.56</v>
       </c>
-      <c r="AA3" s="27">
+      <c r="AA3" s="5">
         <v>60924.68</v>
       </c>
       <c r="AB3" s="4"/>
@@ -4659,7 +4644,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="27"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="20"/>
@@ -4678,7 +4663,7 @@
       <c r="P4" s="4">
         <v>27135.01</v>
       </c>
-      <c r="Q4" s="27">
+      <c r="Q4" s="5">
         <v>23694.69</v>
       </c>
       <c r="R4" s="4"/>
@@ -4703,7 +4688,7 @@
       <c r="Z4" s="4">
         <v>17103.07</v>
       </c>
-      <c r="AA4" s="27">
+      <c r="AA4" s="5">
         <v>14993.75</v>
       </c>
       <c r="AB4" s="4"/>
@@ -4730,7 +4715,7 @@
       <c r="F5" s="7">
         <v>3710</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="27">
         <v>4246</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -4753,7 +4738,7 @@
       <c r="P5" s="4">
         <v>3010</v>
       </c>
-      <c r="Q5" s="27">
+      <c r="Q5" s="5">
         <v>3259</v>
       </c>
       <c r="R5" s="4"/>
@@ -4774,7 +4759,7 @@
       <c r="Z5" s="4">
         <v>22143.51</v>
       </c>
-      <c r="AA5" s="27">
+      <c r="AA5" s="5">
         <v>24769.39</v>
       </c>
       <c r="AB5" s="4"/>
@@ -4801,7 +4786,7 @@
       <c r="F6" s="4">
         <v>11972</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="5">
         <v>18235</v>
       </c>
       <c r="H6" s="4"/>
@@ -4816,7 +4801,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="5"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4">
         <v>29108</v>
@@ -4839,7 +4824,7 @@
       <c r="Z6" s="4">
         <v>48383.81</v>
       </c>
-      <c r="AA6" s="27">
+      <c r="AA6" s="5">
         <v>58380.19</v>
       </c>
       <c r="AB6" s="4"/>
@@ -4866,7 +4851,7 @@
       <c r="F7" s="7">
         <v>581</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="27">
         <v>765</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -4887,7 +4872,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="27"/>
+      <c r="Q7" s="5"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4">
         <v>13996</v>
@@ -4910,7 +4895,7 @@
       <c r="Z7" s="4">
         <v>26457.22</v>
       </c>
-      <c r="AA7" s="27">
+      <c r="AA7" s="5">
         <v>27761.39</v>
       </c>
       <c r="AB7" s="4"/>
@@ -4937,7 +4922,7 @@
       <c r="F8" s="7">
         <v>818</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>898</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -4958,7 +4943,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="27"/>
+      <c r="Q8" s="5"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4">
         <v>41661</v>
@@ -4981,7 +4966,7 @@
       <c r="Z8" s="4">
         <v>35705.47</v>
       </c>
-      <c r="AA8" s="27">
+      <c r="AA8" s="5">
         <v>34617.99</v>
       </c>
       <c r="AB8" s="4"/>
@@ -5008,7 +4993,7 @@
       <c r="F9" s="7">
         <v>1857.02</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>2376.74</v>
       </c>
       <c r="H9" s="7">
@@ -5029,7 +5014,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="27"/>
+      <c r="Q9" s="5"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="20"/>
@@ -5048,7 +5033,7 @@
       <c r="Z9" s="4">
         <v>53582.58</v>
       </c>
-      <c r="AA9" s="27">
+      <c r="AA9" s="5">
         <v>49797.93</v>
       </c>
       <c r="AB9" s="4"/>
@@ -5075,7 +5060,7 @@
       <c r="F10" s="4">
         <v>29172.34</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="5">
         <v>31348.82</v>
       </c>
       <c r="H10" s="4"/>
@@ -5094,7 +5079,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="27"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="20"/>
@@ -5113,7 +5098,7 @@
       <c r="Z10" s="4">
         <v>21567.68</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AA10" s="5">
         <v>26716</v>
       </c>
       <c r="AB10" s="4"/>
@@ -5136,7 +5121,7 @@
       <c r="F11" s="4">
         <v>9828</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="5">
         <v>9543</v>
       </c>
       <c r="H11" s="4"/>
@@ -5157,7 +5142,7 @@
       <c r="P11" s="4">
         <v>6402</v>
       </c>
-      <c r="Q11" s="27">
+      <c r="Q11" s="5">
         <v>7157</v>
       </c>
       <c r="R11" s="4"/>
@@ -5182,7 +5167,7 @@
       <c r="Z11" s="4">
         <v>25646.32</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AA11" s="5">
         <v>27785.23</v>
       </c>
       <c r="AB11" s="4"/>
@@ -5205,7 +5190,7 @@
       <c r="F12" s="4">
         <v>2020</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="20"/>
@@ -5224,7 +5209,7 @@
       <c r="P12" s="4">
         <v>10587.56</v>
       </c>
-      <c r="Q12" s="27">
+      <c r="Q12" s="5">
         <v>11146.71</v>
       </c>
       <c r="R12" s="4"/>
@@ -5249,7 +5234,7 @@
       <c r="Z12" s="4">
         <v>43231</v>
       </c>
-      <c r="AA12" s="27">
+      <c r="AA12" s="5">
         <v>46147.14</v>
       </c>
       <c r="AB12" s="4"/>
@@ -5272,7 +5257,7 @@
       <c r="F13" s="7">
         <v>1339.12</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="27">
         <v>967.86</v>
       </c>
       <c r="H13" s="7">
@@ -5299,7 +5284,7 @@
       <c r="P13" s="4">
         <v>14034.92</v>
       </c>
-      <c r="Q13" s="27">
+      <c r="Q13" s="5">
         <v>16136.34</v>
       </c>
       <c r="R13" s="4"/>
@@ -5324,7 +5309,7 @@
       <c r="Z13" s="4">
         <v>130460.89</v>
       </c>
-      <c r="AA13" s="27">
+      <c r="AA13" s="5">
         <v>158015.99</v>
       </c>
       <c r="AB13" s="4"/>
@@ -5347,7 +5332,7 @@
       <c r="F14" s="4">
         <v>2588.71</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="5">
         <v>3160.02</v>
       </c>
       <c r="H14" s="4"/>
@@ -5372,7 +5357,7 @@
       <c r="P14" s="4">
         <v>15690.41</v>
       </c>
-      <c r="Q14" s="27">
+      <c r="Q14" s="5">
         <v>18307.67</v>
       </c>
       <c r="R14" s="4"/>
@@ -5397,7 +5382,7 @@
       <c r="Z14" s="4">
         <v>620.12</v>
       </c>
-      <c r="AA14" s="27">
+      <c r="AA14" s="5">
         <v>750.23</v>
       </c>
       <c r="AB14" s="4"/>
@@ -5424,7 +5409,7 @@
       <c r="F15" s="4">
         <v>3114.15</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="5">
         <v>3752.02</v>
       </c>
       <c r="H15" s="4"/>
@@ -5449,7 +5434,7 @@
       <c r="P15" s="4">
         <v>10957.73</v>
       </c>
-      <c r="Q15" s="27">
+      <c r="Q15" s="5">
         <v>13330.73</v>
       </c>
       <c r="R15" s="4"/>
@@ -5474,7 +5459,7 @@
       <c r="Z15" s="4">
         <v>1158.97</v>
       </c>
-      <c r="AA15" s="27">
+      <c r="AA15" s="5">
         <v>1325.34</v>
       </c>
       <c r="AB15" s="4"/>
@@ -5501,7 +5486,7 @@
       <c r="F16" s="7">
         <v>251</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="27">
         <v>299</v>
       </c>
       <c r="H16" s="7">
@@ -5528,7 +5513,7 @@
       <c r="P16" s="4">
         <v>12003.25</v>
       </c>
-      <c r="Q16" s="27">
+      <c r="Q16" s="5">
         <v>14206.26</v>
       </c>
       <c r="R16" s="4"/>
@@ -5553,7 +5538,7 @@
       <c r="Z16" s="4">
         <v>3636.54</v>
       </c>
-      <c r="AA16" s="27">
+      <c r="AA16" s="5">
         <v>3901.7</v>
       </c>
       <c r="AB16" s="4"/>
@@ -5576,7 +5561,7 @@
       <c r="F17" s="7">
         <v>190.34</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="27">
         <v>187.81</v>
       </c>
       <c r="H17" s="7" t="s">
@@ -5603,7 +5588,7 @@
       <c r="P17" s="4">
         <v>16124.85</v>
       </c>
-      <c r="Q17" s="27">
+      <c r="Q17" s="5">
         <v>17081.81</v>
       </c>
       <c r="R17" s="4"/>
@@ -5628,7 +5613,7 @@
       <c r="Z17" s="4">
         <v>4850.7</v>
       </c>
-      <c r="AA17" s="27">
+      <c r="AA17" s="5">
         <v>5235.28</v>
       </c>
       <c r="AB17" s="4"/>
@@ -5651,7 +5636,7 @@
       <c r="F18" s="4">
         <v>227.88</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="5">
         <v>251.65</v>
       </c>
       <c r="H18" s="4"/>
@@ -5676,7 +5661,7 @@
       <c r="P18" s="4">
         <v>10882.65</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="Q18" s="5">
         <v>13417.16</v>
       </c>
       <c r="R18" s="4"/>
@@ -5701,7 +5686,7 @@
       <c r="Z18" s="4">
         <v>10390</v>
       </c>
-      <c r="AA18" s="27">
+      <c r="AA18" s="5">
         <v>10446</v>
       </c>
       <c r="AB18" s="4"/>
@@ -5724,7 +5709,7 @@
       <c r="F19" s="4">
         <v>314.33</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="5">
         <v>325.97</v>
       </c>
       <c r="H19" s="4"/>
@@ -5749,7 +5734,7 @@
       <c r="P19" s="4">
         <v>11235.04</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="Q19" s="5">
         <v>11267.48</v>
       </c>
       <c r="R19" s="4"/>
@@ -5774,7 +5759,7 @@
       <c r="Z19" s="4">
         <v>23598</v>
       </c>
-      <c r="AA19" s="27">
+      <c r="AA19" s="5">
         <v>23239</v>
       </c>
       <c r="AB19" s="4"/>
@@ -5797,7 +5782,7 @@
       <c r="F20" s="7">
         <v>391</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="27">
         <v>361</v>
       </c>
       <c r="H20" s="7">
@@ -5824,7 +5809,7 @@
       <c r="P20" s="4">
         <v>9510.46</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="5">
         <v>10378.57</v>
       </c>
       <c r="R20" s="4"/>
@@ -5849,7 +5834,7 @@
       <c r="Z20" s="4">
         <v>46911</v>
       </c>
-      <c r="AA20" s="27">
+      <c r="AA20" s="5">
         <v>46974</v>
       </c>
       <c r="AB20" s="4"/>
@@ -5872,7 +5857,7 @@
       <c r="F21" s="4">
         <v>1218.6</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="5">
         <v>1316.01</v>
       </c>
       <c r="H21" s="4"/>
@@ -5897,7 +5882,7 @@
       <c r="P21" s="4">
         <v>5879.98</v>
       </c>
-      <c r="Q21" s="27">
+      <c r="Q21" s="5">
         <v>5903.04</v>
       </c>
       <c r="R21" s="4"/>
@@ -5922,7 +5907,7 @@
       <c r="Z21" s="9">
         <v>292.76</v>
       </c>
-      <c r="AA21" s="30">
+      <c r="AA21" s="29">
         <v>282.85</v>
       </c>
       <c r="AB21" s="9"/>
@@ -5949,7 +5934,7 @@
       <c r="F22" s="7">
         <v>380</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="27">
         <v>426</v>
       </c>
       <c r="H22" s="7">
@@ -5976,7 +5961,7 @@
       <c r="P22" s="4">
         <v>21536.24</v>
       </c>
-      <c r="Q22" s="27">
+      <c r="Q22" s="5">
         <v>22300.3</v>
       </c>
       <c r="R22" s="4"/>
@@ -6001,7 +5986,7 @@
       <c r="Z22" s="4">
         <v>502</v>
       </c>
-      <c r="AA22" s="27">
+      <c r="AA22" s="5">
         <v>609</v>
       </c>
       <c r="AB22" s="4"/>
@@ -6028,7 +6013,7 @@
       <c r="F23" s="7">
         <v>732</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23" s="27">
         <v>736</v>
       </c>
       <c r="H23" s="7">
@@ -6055,7 +6040,7 @@
       <c r="P23" s="4">
         <v>27884.83</v>
       </c>
-      <c r="Q23" s="27">
+      <c r="Q23" s="5">
         <v>34630.13</v>
       </c>
       <c r="R23" s="4"/>
@@ -6076,7 +6061,7 @@
       <c r="Z23" s="4">
         <v>73643.86</v>
       </c>
-      <c r="AA23" s="27">
+      <c r="AA23" s="5">
         <v>70289.87</v>
       </c>
       <c r="AB23" s="4"/>
@@ -6099,7 +6084,7 @@
       <c r="F24" s="7">
         <v>413</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <v>469</v>
       </c>
       <c r="H24" s="7">
@@ -6126,7 +6111,7 @@
       <c r="P24" s="4">
         <v>1342</v>
       </c>
-      <c r="Q24" s="27">
+      <c r="Q24" s="5">
         <v>1703</v>
       </c>
       <c r="R24" s="4"/>
@@ -6147,7 +6132,7 @@
       <c r="Z24" s="4">
         <v>2200.28</v>
       </c>
-      <c r="AA24" s="27">
+      <c r="AA24" s="5">
         <v>2221.25</v>
       </c>
       <c r="AB24" s="4"/>
@@ -6179,7 +6164,7 @@
       <c r="Z25" s="7">
         <v>1981.15</v>
       </c>
-      <c r="AA25" s="28">
+      <c r="AA25" s="27">
         <v>1511.75</v>
       </c>
       <c r="AB25" s="7">
@@ -6225,7 +6210,7 @@
       <c r="Z26" s="7">
         <v>2086.03</v>
       </c>
-      <c r="AA26" s="28">
+      <c r="AA26" s="27">
         <v>2613.9</v>
       </c>
       <c r="AB26" s="7">
@@ -6276,7 +6261,7 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" spans="2:2">
-      <c r="B29" s="29"/>
+      <c r="B29" s="28"/>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.75" customHeight="1"/>
@@ -7294,8 +7279,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G24"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC26" sqref="AC25:AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Criação da tabela de comparação entre HVMP e Híbrida 2
</commit_message>
<xml_diff>
--- a/Comparaçoes/Heurísticas.xlsx
+++ b/Comparaçoes/Heurísticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500"/>
+    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K = n|4" sheetId="1" r:id="rId1"/>
@@ -305,10 +305,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -324,16 +324,22 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -346,30 +352,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,9 +367,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,7 +392,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -410,6 +403,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -430,17 +431,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,15 +455,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -520,6 +520,156 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -532,91 +682,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,79 +700,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,8 +859,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,15 +891,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -913,17 +919,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,148 +956,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1526,7 +1526,7 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
@@ -7279,8 +7279,8 @@
   <sheetPr/>
   <dimension ref="B1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC25:AD26"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>